<commit_message>
Updated mappings and added revised LO mainpulation
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW2"/>
+  <dimension ref="A1:AW3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -556,76 +556,76 @@
         <v>2024/25</v>
       </c>
       <c r="B2" t="str">
-        <v>02</v>
+        <v>07</v>
       </c>
       <c r="C2" t="str">
-        <v>School of Sport, Exercise and Rehabilitation Sciences</v>
+        <v>Birmingham Business School</v>
       </c>
       <c r="D2" t="str">
-        <v>036</v>
+        <v>012</v>
       </c>
       <c r="E2" t="str">
-        <v>Physiotherapy</v>
+        <v>Management</v>
       </c>
       <c r="F2" t="str">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="G2" t="str">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H2" t="str">
-        <v>Physiotherapy practice-based education placement III</v>
+        <v>The Purposeful Leader</v>
       </c>
       <c r="I2" t="str">
-        <v>LH Physiot practice edu pla II</v>
+        <v>LM The Purposeful Leader</v>
       </c>
       <c r="J2" t="str">
-        <v>LH Physiotherapy practice-based education placement III</v>
+        <v>LM The Purposeful Leader</v>
       </c>
       <c r="K2" t="str">
-        <v>tbc</v>
+        <v>= £16,500) SFAre there any related programme modifications? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?YesB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryThere were a series of consultations with alumni, existing students and sponsors of prospective students. In each consultation programme aims, programme learning outcomes and programme structure was shared and feedback was collected.   The consultations took place on the following dates:   06/10/2022: Consultations with Alumni in relevant management positions 21/10/2022: On 21st October there were 3 consultations with existing students, one for each of the locations PT MBA Singapore Institute of Management; FT MBA (Edgbaston) and Exec MBA (Edgbaston)  Following the consultations above feedback was taken on board and proposal amended accordingly where appropriate.  The updated proposal was used for final consultations with employers sponsoring their team to join our PGDip and follow into the Executive MBA in the UK. Employer consultations took place on the following dates:  25th November 2022 15th December 2022 6th January 2022 QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)This module is not available for students outside the programmes in which it is a core module.   There is a Dubai equivalent based being proposed as the new MBA will also be offered in Dubai. As this is a new offer in Dubai, there is no programme lead appointed, but it is in line with the plans of Dubai to offer such programme in the Dubai Campus. QIf the module/programme is subject to accreditation, please provide details of consultation with the professional body QIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision Q8ApprovalSchool/InstituteDate: 07/02/2023Approving body: SPARCCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{Birmingham Business School[Management] module delivered in collaboration with another organisation? YesIf ‘yes’ please state the organisation’s name:Singapore Institute of ManagementB Q SFIs this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)Association of MBAs (AMBA) ʓThe Purposeful Leader #</v>
       </c>
       <c r="L2" t="str">
-        <v>LH</v>
+        <v>LM</v>
       </c>
       <c r="M2" t="str">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N2" t="str">
-        <v>UG</v>
+        <v>GT</v>
       </c>
       <c r="O2" t="str">
         <v>Z</v>
       </c>
       <c r="P2" t="str">
-        <v>103</v>
+        <v/>
       </c>
       <c r="Q2" t="str">
-        <v>B160</v>
+        <v>N200</v>
       </c>
       <c r="R2" t="str">
-        <v>100252</v>
+        <v>100089</v>
       </c>
       <c r="S2" t="str">
-        <v>605G – MSci PhysiotherapyMSci Physiotherapy PTMSci Physiotherapy w Int Yr FTAs an optional module (including any information regarding the basket to which it should be assigned):</v>
+        <v>Master of Business Administration SIM Part-Time (Code TBC)As an optional module (including any information about its grouping, if relevant):</v>
       </c>
       <c r="T2" t="str">
         <v/>
       </c>
       <c r="U2" t="str">
-        <v>Students must have completed Year 2 of the MSci Physiotherapy programme.</v>
+        <v>None</v>
       </c>
       <c r="V2" t="str">
         <v>None</v>
       </c>
       <c r="W2" t="str">
-        <v>Choose an item.</v>
+        <v>Other (please state below)</v>
       </c>
       <c r="X2" t="str">
         <v/>
       </c>
       <c r="Y2" t="str">
-        <v>, including approved exceptions relating to the semesterised ÅNone</v>
+        <v>This module requires an exemption from the semesterised teaching year. This research module requires to be an open-ended module, which students complete with the taught element, supplying a final project proposal as part of their assessment portfolio.</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -643,7 +643,7 @@
         <v>0</v>
       </c>
       <c r="AE2">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AF2">
         <v>0</v>
@@ -655,54 +655,203 @@
         <v>0</v>
       </c>
       <c r="AI2">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>0</v>
+        <v>174</v>
       </c>
       <c r="AK2">
         <v>0</v>
       </c>
       <c r="AL2" t="str">
-        <v>This placement module is the third of six placement modules that feature as part of the MSci Physiotherapy programme. The student will have an identified clinical educator within a health care setting (that is typically external to the university) where they will have the opportunity to use and develop clinical knowledge and skills acquired during the previous modules, components and placement Physiotherapy practice-based education placements I and II. The student will have the opportunity to identify learning needs from previous practice-based placement experiences and attempt to address these needs within a different setting. The opportunity will exist to learn new profession-specific skills and to acquire new knowledge. Different students within the cohort will be allocated to a diverse range placement settings and learning outcomes should be interpreted flexibly in order that students are assessed optimally.</v>
+        <v>This is a reflective and developmental module for students to explore their leadership and career aspirations in relation to their purposive values. The module will include four types of learning engagements: &lt;br&gt;An examination of current values-based and purpose-led theories of leadership. Students will be encouraged to critically examine theories they study, and apply them to their own contexts and experiences; &lt;br&gt;Critical reflective practice about how they enact and embody purposeful/values-based leading and aspects of their organizational context which impacts on their ability to lead from this orientation; &lt;br&gt;Professional skills development activities, including coaching to enhance their capacity to lead effectively that will be coordinated and delivered by the BBS Career team; &lt;br&gt;The development of reflective practitioner and associated research skills, culminating in the creation of a plan to underpin career aspirations. &lt;br&gt; &lt;br&gt;Students will be expected to keep a portfolio of reflective practice on their purposeful leadership approach throughout the module, and how what they have learned on different modules is influencing this.</v>
       </c>
       <c r="AM2" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Demonstrate sound subjective and objective assessment skills, developing skills in writing effective problem lists and treatment plans&lt;/li&gt;&lt;li&gt;Demonstrate clinical reasoning skills, using evidence-based practice to underpin the core skills outlined above, enabling effective assessment and treatment of a range of patient presentations&lt;/li&gt;&lt;li&gt;Demonstrate knowledge and use of objective measures&lt;/li&gt;&lt;li&gt;Demonstrate safe and effective treatment skills&lt;/li&gt;&lt;li&gt;Demonstrate a variety of communication skills across a wide range of service users with a variety of challenges to communication.&lt;/li&gt;&lt;li&gt;Demonstrate efficient time management skills appropriate to clinical area&lt;/li&gt;&lt;li&gt;Demonstrate effective communication skills with the multidisciplinary team (MDT) - engaging with the process of MDT communication and working&lt;/li&gt;&lt;li&gt;Reflect on the function of MDT appropriate to clinical area alongside the specific role of physiotherapy within the MDT, demonstrating active participation in MDT working&lt;/li&gt;&lt;li&gt;Engage in inter-professional learning within the MDT&lt;/li&gt;&lt;/ul&gt;</v>
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Critically analyse theories and practice of purposeful leadership &lt;/li&gt;&lt;li&gt;Reflect critically on their own leadership practice and the way in which it reflects their purpose &lt;/li&gt;&lt;li&gt;Design and plan an independent project which identifies a business issue of strategic relevance to their organization or plan for an entrepreneurial development. &lt;/li&gt;&lt;li&gt;Identify their leadership skills gaps, demonstrate and reflect upon actions taken to address the gaps through authentic assessment, coaching, mentoring training, reflective group discussions and evaluate your learning journey.&lt;/li&gt;&lt;/ul&gt;</v>
       </c>
       <c r="AN2" t="str">
-        <v>Feedback from clinical educator and link tutor.</v>
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{Birmingham Business School[Management𓏉The Purposeful Leader`2024/25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThis module is a 20-credit compulsory module proposed in conjunction with the new Executive Master of Business Administration programme proposal.  It is one of the two core integrative modules that will anchor the responsible business vision of the MBA suite of programmes by focusing on what it means in terms of students’ purposeful leadership approach and how to put their values and approach into practice and related personal and professional development activities throughout the programme. It is key for delivering the strategic learning outcomes of the Business School around responsible business and thought leadership.  The module is also required to meet AMBA programme design objectives and to meet Senior Leader Apprenticeship Standards with respect to specific knowledge, skills and behaviours (KSBs), as listed below.   Knowledge K6: Ethics and values-based leadership theories and principles. K10: Organisational; team dynamics and how to build engagement and develop high performance, agile and collaborative cultures. K12: Influencing and negotiating strategies both upwards and outwards. K13: The external and social and political environment and use of diplomacy with diverse groups of internal and external stakeholders. K14 Working with board and company leadership structures. K18: Coaching and mentoring techniques. K19: Approaches to developing a CSR programme. AMBA:  Business research methods and consulting skills Leadership and entrepreneurship An understanding of the impact of ethics and risk management on issues of CSR, sustainable development and societal well being  Skills S2: Set strategic direction and gain support for it from key stakeholders S7: Challenge strategies and operations in terms of ethics, responsibility, sustainability, resource allocation and business continuity; risk management. S13: Use personal presence and storytelling to articulate and translate vision into operational strategies, demonstrate clarity in thinking such as consideration of sustainable approaches. S14: Create an inclusive culture, encouraging diversity and difference and promoting well-being. S15: Give and receive feedback at all levels, building confidence and developing trust, and enable people to take risks and challenge where appropriate. S17: Lead and influence people, building constructive working relationships across teams, using matrix management where required. S20: Lead within their area of control, authority, influencing both upwards and outwards, negotiating and using advocacy skills to build reputation and effective collaboration. AMBA: Leadership Dealing with ambiguity Values  Behaviours B2: Take personal accountability aligned to clear values. B4: Value difference and champion diversity. B5: Seek continuous professional development opportunities for self and wider team.  The Purposeful Leader module together with one of the 40 credits electives for final project modules involves student research and make up 60 credits of independent learning based on student research within the MBA Programme. Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)For this module to be delivered as proposed it requires a new Professional service member of staff Grade 7 to be added to the Careers team to manage all leadership coaches and manage and deliver 26h of practical classes across the portfolio.    There is an additional cost of £300/student for the external coach. This consists of 3 coaching sessions of 1 hour each at a rate of £100/hour. The cost of coaches per cohort for the Executive MBA UK is estimated at £16,500. This number is a function of recruitment. (Cost x target: £300 x 55 students = £16,500) SFAre there any related programme modifications? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?YesB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryThere were a series of consultations with alumni, existing students and sponsors of prospective students. In each consultation programme aims, programme learning outcomes and programme structure was shared and feedback was collected.   The consultations took place on the following dates:   06/10/2022: Consultations with Alumni in relevant management positions 21/10/2022: On 21st October there were 3 consultations with existing students, one for each of the locations PT MBA Singapore Institute of Management; FT MBA (Edgbaston) and Exec MBA (Edgbaston)  Following the consultations above feedback was taken on board and proposal amended accordingly where appropriate.  The updated proposal was used for final consultations with employers sponsoring their team to join our PGDip and follow into the Executive MBA in the UK. Employer consultations took place on the following dates:  25th November 2022 15th December 2022 6th January 2022 QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)This module is not available for students outside the programmes in which it is a core module.   There is a Dubai equivalent based being proposed as the new MBA will also be offered in Dubai. As this is a new offer in Dubai, there is no programme lead appointed, but it is in line with the plans of Dubai to offer such programme in the Dubai Campus. QIf the module/programme is subject to accreditation, please provide details of consultation with the professional body QIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision Q8ApprovalSchool/InstituteDate: 07/02/2023Approving body: SPARCCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{Birmingham Business School[Management] module delivered in collaboration with another organisation? YesIf ‘yes’ please state the organisation’s name:Singapore Institute of ManagementB Q SFIs this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)Association of MBAs (AMBA) ʓThe Purposeful Leader #TBC=Masters - LM@20$, if relevantN/A⸮Full TermﱙAs a compulsory module (i.e. every student in the year should be ǕMaster of Business Administration SIM Part-Time (Code TBC)As an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableNoneÂNoneÃOther (please state below)ÄTeaching will take place both at the Singapore Institute of Management and online.   Ä on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupOur School fully supports the University’s commitment to inclusivity.  All modules are designed to promote equality of access to teaching sessions and assessment opportunities.  The School engages with Student Services to ensure that students with additional support needs receive appropriate support for their learning and that, where needed, reasonable adjustments are made to delivery of teaching and to examination arrangements.  Q ÅThis module requires an exemption from the semesterised teaching year. This research module requires to be an open-ended module, which students complete with the taught element, supplying a final project proposal as part of their assessment portfolio. Æ effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q ÇÈ Éꮛꮜꮝ26ꮞꮟꮠꮡꮢ174ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis is a reflective and developmental module for students to explore their leadership and career aspirations in relation to their purposive values. The module will include four types of learning engagements:  An examination of current values-based and purpose-led theories of leadership.  Students will be encouraged to critically examine theories they study, and apply them to their own contexts and experiences; Critical reflective practice about how they enact and embody purposeful/values-based leading and aspects of their organizational context which impacts on their ability to lead from this orientation; Professional skills development activities, including coaching to enhance their capacity to lead effectively that will be coordinated and delivered by the BBS Career team; The development of reflective practitioner and associated research skills, culminating in the creation of a plan to underpin career aspirations.  Students will be expected to keep a portfolio of reflective practice on their purposeful leadership approach throughout the module, and how what they have learned on different modules is influencing this.  ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:Critically analyse theories and practice of purposeful leadership Reflect critically on their own leadership practice and the way in which it reflects their purpose Design and plan an independent project which identifies a business issue of strategic relevance to their organization or plan for an entrepreneurial development. Identify their leadership skills gaps, demonstrate and reflect upon actions taken to address the gaps through authentic assessment, coaching, mentoring training, reflective group discussions and evaluate your learning journey. ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
       </c>
       <c r="AO2" t="str">
-        <v>Assessment using the Common Placement Assessment Form (CPAF) – 100%&lt;br&gt;&lt;br&gt;As a required component (zero credit), grading will not be credit-bearing but will be offered as part of feedback.&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+        <v>&lt;br&gt;Portfolio of work which will include: &lt;br&gt; &lt;br&gt;Reflective log of their experimenting with purposeful leadership practice; (A summary statement of what has been learned and a plan for further development up to 3000 words, 75% of the grade) &lt;br&gt;Independent project proposal (1000 words or equivalent, 25% of the grade) &lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AP2" t="str">
-        <v>N/A - not examined</v>
+        <v>No</v>
       </c>
       <c r="AQ2" t="str">
         <v>N/A - not examined</v>
       </c>
       <c r="AR2" t="str">
-        <v>This placement module must be passed.</v>
+        <v>None</v>
       </c>
       <c r="AS2" t="str">
-        <v>Repeat placement</v>
+        <v>A portfolio including: &lt;br&gt; &lt;br&gt;Reflective log of their experimenting with purposeful leadership practice; (A summary statement of what has been learned and a plan for further development up to 3000 words, 75% of the grade) &lt;br&gt;Independent project proposal (1000 words or equivalent, 25% of the grade) &lt;br&gt;</v>
       </c>
       <c r="AT2" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Assessment using the Common Placement Assessment Form (CPAF) – 100%&lt;br&gt;&lt;br&gt;As a required component (zero credit), grading will not be credit-bearing but will be offered as part of feedback.&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Repeat placement</v>
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Portfolio of work which will include: &lt;br&gt; &lt;br&gt;Reflective log of their experimenting with purposeful leadership practice; (A summary statement of what has been learned and a plan for further development up to 3000 words, 75% of the grade) &lt;br&gt;Independent project proposal (1000 words or equivalent, 25% of the grade) &lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;A portfolio including: &lt;br&gt; &lt;br&gt;Reflective log of their experimenting with purposeful leadership practice; (A summary statement of what has been learned and a plan for further development up to 3000 words, 75% of the grade) &lt;br&gt;Independent project proposal (1000 words or equivalent, 25% of the grade) &lt;br&gt;</v>
       </c>
       <c r="AU2" t="str">
-        <v>Delivered twice in ac. year (semester 1 and 2)</v>
+        <v>Full Term</v>
       </c>
       <c r="AV2" t="str">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AW2" t="str">
-        <v>TBC</v>
+        <v>Donna Ladkin; Joanne Murphy and Sandy Purewal</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2024-25</v>
+      </c>
+      <c r="B3" t="str">
+        <v>09</v>
+      </c>
+      <c r="C3" t="str">
+        <v>School of History and Cultures</v>
+      </c>
+      <c r="D3" t="str">
+        <v>047</v>
+      </c>
+      <c r="E3" t="str">
+        <v>History</v>
+      </c>
+      <c r="F3" t="str">
+        <v>225</v>
+      </c>
+      <c r="G3" t="str">
+        <v>11</v>
+      </c>
+      <c r="H3" t="str">
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J3" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K3" t="str">
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <v>UG</v>
+      </c>
+      <c r="O3" t="str">
+        <v>Z</v>
+      </c>
+      <c r="P3" t="str">
+        <v>139</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>V100</v>
+      </c>
+      <c r="R3" t="str">
+        <v>100302</v>
+      </c>
+      <c r="S3" t="str">
+        <v>515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):</v>
+      </c>
+      <c r="T3" t="str">
+        <v/>
+      </c>
+      <c r="U3" t="str">
+        <v>None</v>
+      </c>
+      <c r="V3" t="str">
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of History and Cultures[History𓏉LM Heritage Management Practice`2024-25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThe change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)No new resource requirementsSFAre there any related programme modifications? (for proposals and significant module modifications)NoB QIf yes, have they been submitted for approval alongside this proposal?N/AB Q7Consultation (required for modifications, advised for proposals, where applicable)Prospective/existing students where necessaryAs this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 07/08/2023Approving body: SHAC PARCCollege (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC via Chairs ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.1{School of History and CulturesB2Department (if applicable)HistoryB3Is the module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SF4Is this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SF5Accrediting body (if applicable)N/AQ6Module title LM The Business of Heritage  B Q7Module code(s) (if known)38901B8Module levelMasters - LMB Q9Module credits 20B Q10Module attribute, if relevantn/aB11Semester in which the module will runSemester 1B12Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/A14Â</v>
+      </c>
+      <c r="W3" t="str">
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of History and Cultures[History𓏉LM Heritage Management Practice`2024-25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThe change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)No new resource requirementsSFAre there any related programme modifications? (for proposals and significant module modifications)NoB QIf yes, have they been submitted for approval alongside this proposal?N/AB Q7Consultation (required for modifications, advised for proposals, where applicable)Prospective/existing students where necessaryAs this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 07/08/2023Approving body: SHAC PARCCollege (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC via Chairs ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.1{School of History and CulturesB2Department (if applicable)HistoryB3Is the module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SF4Is this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SF5Accrediting body (if applicable)N/AQ6Module title LM The Business of Heritage  B Q7Module code(s) (if known)38901B8Module levelMasters - LMB Q9Module credits 20B Q10Module attribute, if relevantn/aB11Semester in which the module will runSemester 1B12Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/A14ÂN/AB15Where will the teaching take place? UoB Campus Edgbaston</v>
+      </c>
+      <c r="X3" t="str">
+        <v>B</v>
+      </c>
+      <c r="Y3" t="str">
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of History and Cultures[History𓏉LM Heritage Management Practice`2024-25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThe change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)No new resource requirementsSFAre there any related programme modifications? (for proposals and significant module modifications)NoB QIf yes, have they been submitted for approval alongside this proposal?N/AB Q7Consultation (required for modifications, advised for proposals, where applicable)Prospective/existing students where necessaryAs this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 07/08/2023Approving body: SHAC PARCCollege (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC via Chairs ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.1{School of History and CulturesB2Department (if applicable)HistoryB3Is the module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SF4Is this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SF5Accrediting body (if applicable)N/AQ6Module title LM The Business of Heritage  B Q7Module code(s) (if known)38901B8Module levelMasters - LMB Q9Module credits 20B Q10Module attribute, if relevantn/aB11Semester in which the module will runSemester 1B12Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/A14ÂN/AB15Where will the teaching take place? UoB Campus EdgbastonÄB Q SF16Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe school is committed to ensuring modules and programmes are inclusive and work closely with the University’s Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.Q 17Å</v>
+      </c>
+      <c r="Z3">
+        <v>NaN</v>
+      </c>
+      <c r="AA3">
+        <v>NaN</v>
+      </c>
+      <c r="AB3">
+        <v>NaN</v>
+      </c>
+      <c r="AC3">
+        <v>NaN</v>
+      </c>
+      <c r="AD3">
+        <v>NaN</v>
+      </c>
+      <c r="AE3">
+        <v>NaN</v>
+      </c>
+      <c r="AF3">
+        <v>NaN</v>
+      </c>
+      <c r="AG3">
+        <v>NaN</v>
+      </c>
+      <c r="AH3">
+        <v>NaN</v>
+      </c>
+      <c r="AI3">
+        <v>NaN</v>
+      </c>
+      <c r="AJ3">
+        <v>NaN</v>
+      </c>
+      <c r="AK3">
+        <v>19</v>
+      </c>
+      <c r="AL3" t="str">
+        <v>["&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Modification&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;LM Heritage Management Practice&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;2024-25&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;No new resource requirements&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;No&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;As this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 07/08/2023&lt;br&gt;Approving body: SHAC PARC&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC via Chairs Action&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.&lt;br&gt; &lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;4&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;5&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;6&lt;br&gt;Module title &lt;br&gt;LM The Business of Heritage &lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Module code(s) (if known)&lt;br&gt;38901&lt;br&gt;B&lt;br&gt;8&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;9&lt;br&gt;Module credits &lt;br&gt;20&lt;br&gt;B Q&lt;br&gt;10&lt;br&gt;Module attribute, if relevant&lt;br&gt;n/a&lt;br&gt;B&lt;br&gt;11&lt;br&gt;Semester in which the module will run&lt;br&gt;Semester 1&lt;br&gt;&lt;br&gt;B&lt;br&gt;12&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e. every student in the year should be registered on this module code):&lt;br&gt;515H LM International Heritage Management FT&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant):&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;None&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;14&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;15&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Edgbaston&lt;br&gt;&lt;br&gt;If 'other' please state here:&lt;br&gt;B Q SF&lt;br&gt;16&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected group&lt;br&gt;The school is committed to ensuring modules and programmes are inclusive and work closely with the University's Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.&lt;br&gt;Q &lt;br&gt;17&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;18&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)&lt;br&gt;B Q SF&lt;br&gt;18.1&lt;br&gt;Lecture&lt;br&gt;10&lt;br&gt;&lt;br&gt;18.2&lt;br&gt;Seminar &lt;br&gt;10&lt;br&gt;&lt;br&gt;18.3&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;18.4&lt;br&gt;Project supervision&lt;br&gt;&lt;br&gt;18.5&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;18.6&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;18.7&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;18.8&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;18.9&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;18.10&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;18.11&lt;br&gt;Guided independent study&lt;br&gt;180&lt;br&gt;&lt;br&gt;18.12&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;19&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥ</v>
+      </c>
+      <c r="AM3" t="str">
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;20.1&lt;/li&gt;&lt;li&gt;Demonstrate critical awareness of the need to manage heritage sites financially and administratively&lt;/li&gt;&lt;li&gt;20.2&lt;/li&gt;&lt;li&gt; Demonstratean understanding of the nature and importance of marketing in the context of heritage sites&lt;/li&gt;&lt;li&gt;20.3&lt;/li&gt;&lt;li&gt;Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function&lt;/li&gt;&lt;li&gt;20.4&lt;/li&gt;&lt;li&gt;Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard&lt;/li&gt;&lt;li&gt;21&lt;/li&gt;&lt;/ul&gt;</v>
+      </c>
+      <c r="AN3" t="str">
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of History and Cultures[History𓏉LM Heritage Management Practice`2024-25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThe change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)No new resource requirementsSFAre there any related programme modifications? (for proposals and significant module modifications)NoB QIf yes, have they been submitted for approval alongside this proposal?N/AB Q7Consultation (required for modifications, advised for proposals, where applicable)Prospective/existing students where necessaryAs this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 07/08/2023Approving body: SHAC PARCCollege (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC via Chairs ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.1{School of History and CulturesB2Department (if applicable)HistoryB3Is the module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SF4Is this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SF5Accrediting body (if applicable)N/AQ6Module title LM The Business of Heritage  B Q7Module code(s) (if known)38901B8Module levelMasters - LMB Q9Module credits 20B Q10Module attribute, if relevantn/aB11Semester in which the module will runSemester 1B12Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/A14ÂN/AB15Where will the teaching take place? UoB Campus EdgbastonÄB Q SF16Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe school is committed to ensuring modules and programmes are inclusive and work closely with the University’s Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.Q 17ÅN/AQ18Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)B Q SF18.1Lecture1018.2È 1018.3É18.4ꮛ18.5ꮜ18.6ꮝ18.7ꮞ18.8ꮟ18.9ꮠ18.10ꮡ18.11ꮢ18018.12ꮣ19ꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students’ awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.Q20Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:20.1Demonstrate critical awareness of the need to manage heritage sites financially and administratively20.2 Demonstratean understanding of the nature and importance of marketing in the context of heritage sites20.3Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function20.4Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard21ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+      </c>
+      <c r="AO3" t="str">
+        <v>["&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Modification&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;LM Heritage Management Practice&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;2024-25&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).&lt;br&gt;&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;No new resource requirements&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;No&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;As this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 07/08/2023&lt;br&gt;Approving body: SHAC PARC&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC via Chairs Action&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.&lt;br&gt; &lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;4&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;5&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;6&lt;br&gt;Module title &lt;br&gt;LM The Business of Heritage &lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Module code(s) (if known)&lt;br&gt;38901&lt;br&gt;B&lt;br&gt;8&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;9&lt;br&gt;Module credits &lt;br&gt;20&lt;br&gt;B Q&lt;br&gt;10&lt;br&gt;Module attribute, if relevant&lt;br&gt;n/a&lt;br&gt;B&lt;br&gt;11&lt;br&gt;Semester in which the module will run&lt;br&gt;Semester 1&lt;br&gt;&lt;br&gt;B&lt;br&gt;12&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e. every student in the year should be registered on this module code):&lt;br&gt;515H LM International Heritage Management FT&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant):&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;None&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;14&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;15&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Edgbaston&lt;br&gt;&lt;br&gt;If 'other' please state here:&lt;br&gt;B Q SF&lt;br&gt;16&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected group&lt;br&gt;The school is committed to ensuring modules and programmes are inclusive and work closely with the University's Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.&lt;br&gt;Q &lt;br&gt;17&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;18&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)&lt;br&gt;B Q SF&lt;br&gt;18.1&lt;br&gt;Lecture&lt;br&gt;10&lt;br&gt;&lt;br&gt;18.2&lt;br&gt;Seminar &lt;br&gt;10&lt;br&gt;&lt;br&gt;18.3&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;&lt;br&gt;18.4&lt;br&gt;Project supervision&lt;br&gt;&lt;br&gt;&lt;br&gt;18.5&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;&lt;br&gt;18.6&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;&lt;br&gt;18.7&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;&lt;br&gt;18.8&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;&lt;br&gt;18.9&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;&lt;br&gt;18.10&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;&lt;br&gt;18.11&lt;br&gt;Guided independent study&lt;br&gt;180&lt;br&gt;&lt;br&gt;18.12&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;&lt;br&gt;19&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students' awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.&lt;br&gt;Q&lt;br&gt;20&lt;br&gt;Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student's failure of the module. The QAA publish guidance related to 'levelness' in the Frameworks for Higher Education Qualifications and in their Subject Benchmark Statements. Schools/Institutes are also encouraged to refer to the Birmingham Graduate Attributes. &lt;br&gt;&lt;br&gt;ꮧ20.1&lt;br&gt;Demonstrate critical awareness of the need to manage heritage sites financially and administratively&lt;br&gt;20.2&lt;br&gt; Demonstratean understanding of the nature and importance of marketing in the context of heritage sites&lt;br&gt;20.3&lt;br&gt;Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function&lt;br&gt;20.4&lt;br&gt;Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard&lt;br&gt;21ꮨ(i.e. assessment that does not produce a mark that contributes to the overall module mark)&lt;br&gt; 10 minute presentation: Online presentation to Course Convenor on proposed heritage project and outline of key topics of business plan. Feedback will be provided immediately after online presentation verbally to student.&lt;br&gt;Q&lt;br&gt;22&lt;br&gt;Assessment category (multiple assessments should be included in the same category, e.g. a module with two written tasks and an oral presentation would be 'coursework 100%')&lt;br&gt;If the module is wholly or partly assessed by coursework, please state the overall weighting: &lt;br&gt;&lt;br&gt;100% &lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;&lt;br&gt;If the module is wholly or partly assessed by examination, please state the overall weighting: &lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;23&lt;br&gt;Additional information on the method(s) of summative assessment and weighting, ꮫ</v>
+      </c>
+      <c r="AP3" t="str">
+        <v>No</v>
+      </c>
+      <c r="AQ3" t="str">
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of History and Cultures[History𓏉LM Heritage Management Practice`2024-25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThe change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)No new resource requirementsSFAre there any related programme modifications? (for proposals and significant module modifications)NoB QIf yes, have they been submitted for approval alongside this proposal?N/AB Q7Consultation (required for modifications, advised for proposals, where applicable)Prospective/existing students where necessaryAs this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 07/08/2023Approving body: SHAC PARCCollege (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC via Chairs ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.1{School of History and CulturesB2Department (if applicable)HistoryB3Is the module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SF4Is this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SF5Accrediting body (if applicable)N/AQ6Module title LM The Business of Heritage  B Q7Module code(s) (if known)38901B8Module levelMasters - LMB Q9Module credits 20B Q10Module attribute, if relevantn/aB11Semester in which the module will runSemester 1B12Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/A14ÂN/AB15Where will the teaching take place? UoB Campus EdgbastonÄB Q SF16Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe school is committed to ensuring modules and programmes are inclusive and work closely with the University’s Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.Q 17ÅN/AQ18Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)B Q SF18.1Lecture1018.2È 1018.3É18.4ꮛ18.5ꮜ18.6ꮝ18.7ꮞ18.8ꮟ18.9ꮠ18.10ꮡ18.11ꮢ18018.12ꮣ19ꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students’ awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.Q20Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:20.1Demonstrate critical awareness of the need to manage heritage sites financially and administratively20.2 Demonstratean understanding of the nature and importance of marketing in the context of heritage sites20.3Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function20.4Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard21ꮨ(i.e. assessment that does not produce a mark that ꮩ 10 minute presentation: Online presentation to Course Convenor on proposed heritage project and outline of key topics of business plan. Feedback will be provided immediately after online presentation verbally to student.Q22Assessment category (multiple assessments should be included in the same category, e.g. a module with two written tasks and an oral presentation would be ‘coursework 100%’)ɸ 100% B ∏   23Ŋ and weighting, ꮫ1 x 3,000 word heritage project business plan  (100%)B Q23.1If there is an examination, is it centrally ꮭNoꮮ If ‘yes’ is this available for students to take overseas?N/AB23.2If there is an examination, ꮯ</v>
+      </c>
+      <c r="AR3" t="str">
+        <v/>
+      </c>
+      <c r="AS3" t="str">
+        <v>["&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Modification&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;LM Heritage Management Practice&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;2024-25&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).&lt;br&gt;&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;No new resource requirements&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;No&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;As this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 07/08/2023&lt;br&gt;Approving body: SHAC PARC&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC via Chairs Action&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.&lt;br&gt; &lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;4&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;5&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;6&lt;br&gt;Module title &lt;br&gt;LM The Business of Heritage &lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Module code(s) (if known)&lt;br&gt;38901&lt;br&gt;B&lt;br&gt;8&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;9&lt;br&gt;Module credits &lt;br&gt;20&lt;br&gt;B Q&lt;br&gt;10&lt;br&gt;Module attribute, if relevant&lt;br&gt;n/a&lt;br&gt;B&lt;br&gt;11&lt;br&gt;Semester in which the module will run&lt;br&gt;Semester 1&lt;br&gt;&lt;br&gt;B&lt;br&gt;12&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e. every student in the year should be registered on this module code):&lt;br&gt;515H LM International Heritage Management FT&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant):&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;None&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;14&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;15&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Edgbaston&lt;br&gt;&lt;br&gt;If 'other' please state here:&lt;br&gt;B Q SF&lt;br&gt;16&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected group&lt;br&gt;The school is committed to ensuring modules and programmes are inclusive and work closely with the University's Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.&lt;br&gt;Q &lt;br&gt;17&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;18&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)&lt;br&gt;B Q SF&lt;br&gt;18.1&lt;br&gt;Lecture&lt;br&gt;10&lt;br&gt;&lt;br&gt;18.2&lt;br&gt;Seminar &lt;br&gt;10&lt;br&gt;&lt;br&gt;18.3&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;&lt;br&gt;18.4&lt;br&gt;Project supervision&lt;br&gt;&lt;br&gt;&lt;br&gt;18.5&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;&lt;br&gt;18.6&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;&lt;br&gt;18.7&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;&lt;br&gt;18.8&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;&lt;br&gt;18.9&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;&lt;br&gt;18.10&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;&lt;br&gt;18.11&lt;br&gt;Guided independent study&lt;br&gt;180&lt;br&gt;&lt;br&gt;18.12&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;&lt;br&gt;19&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students' awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.&lt;br&gt;Q&lt;br&gt;20&lt;br&gt;Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student's failure of the module. The QAA publish guidance related to 'levelness' in the Frameworks for Higher Education Qualifications and in their Subject Benchmark Statements. Schools/Institutes are also encouraged to refer to the Birmingham Graduate Attributes. &lt;br&gt;&lt;br&gt;ꮧ20.1&lt;br&gt;Demonstrate critical awareness of the need to manage heritage sites financially and administratively&lt;br&gt;20.2&lt;br&gt; Demonstratean understanding of the nature and importance of marketing in the context of heritage sites&lt;br&gt;20.3&lt;br&gt;Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function&lt;br&gt;20.4&lt;br&gt;Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard&lt;br&gt;21ꮨ(i.e. assessment that does not produce a mark that contributes to the overall module mark)&lt;br&gt; 10 minute presentation: Online presentation to Course Convenor on proposed heritage project and outline of key topics of business plan. Feedback will be provided immediately after online presentation verbally to student.&lt;br&gt;Q&lt;br&gt;22&lt;br&gt;Assessment category (multiple assessments should be included in the same category, e.g. a module with two written tasks and an oral presentation would be 'coursework 100%')&lt;br&gt;If the module is wholly or partly assessed by coursework, please state the overall weighting: &lt;br&gt;&lt;br&gt;100% &lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;&lt;br&gt;If the module is wholly or partly assessed by examination, please state the overall weighting: &lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;23&lt;br&gt;Additional information on the method(s) of summative assessment and weighting, ꮫ&lt;br&gt;1 x 3,000 word heritage project business plan (100%)&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;23.1&lt;br&gt;If there is an examination, is it centrally timetabled?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please specify the length of the examination: &lt;br&gt;&lt;br&gt;If 'yes' is this available for students to take overseas?&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;23.2&lt;br&gt;If there is an examination, select examination period&lt;br&gt;N/A - not examined&lt;br&gt;&lt;br&gt;B&lt;br&gt;&lt;br&gt;24&lt;br&gt;Please describe any internal hurdles&lt;br&gt;None&lt;br&gt;B Q&lt;br&gt;25&lt;br&gt;Method(s) of reassessment students would be expected to undertake should they fail to pass the module at the first attempt. The reassessment method(s) must enable students to ꮲ</v>
+      </c>
+      <c r="AT3" t="str">
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;["&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Modification&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;LM Heritage Management Practice&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;2024-25&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;No new resource requirements&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;No&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;As this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 07/08/2023&lt;br&gt;Approving body: SHAC PARC&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC via Chairs Action&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.&lt;br&gt; &lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;4&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;5&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;6&lt;br&gt;Module title &lt;br&gt;LM The Business of Heritage &lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Module code(s) (if known)&lt;br&gt;38901&lt;br&gt;B&lt;br&gt;8&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;9&lt;br&gt;Module credits &lt;br&gt;20&lt;br&gt;B Q&lt;br&gt;10&lt;br&gt;Module attribute, if relevant&lt;br&gt;n/a&lt;br&gt;B&lt;br&gt;11&lt;br&gt;Semester in which the module will run&lt;br&gt;Semester 1&lt;br&gt;&lt;br&gt;B&lt;br&gt;12&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e. every student in the year should be registered on this module code):&lt;br&gt;515H LM International Heritage Management FT&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant):&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;None&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;14&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;15&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Edgbaston&lt;br&gt;&lt;br&gt;If 'other' please state here:&lt;br&gt;B Q SF&lt;br&gt;16&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected group&lt;br&gt;The school is committed to ensuring modules and programmes are inclusive and work closely with the University's Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.&lt;br&gt;Q &lt;br&gt;17&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;18&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)&lt;br&gt;B Q SF&lt;br&gt;18.1&lt;br&gt;Lecture&lt;br&gt;10&lt;br&gt;&lt;br&gt;18.2&lt;br&gt;Seminar &lt;br&gt;10&lt;br&gt;&lt;br&gt;18.3&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;18.4&lt;br&gt;Project supervision&lt;br&gt;&lt;br&gt;18.5&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;18.6&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;18.7&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;18.8&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;18.9&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;18.10&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;18.11&lt;br&gt;Guided independent study&lt;br&gt;180&lt;br&gt;&lt;br&gt;18.12&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;19&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students' awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.&lt;br&gt;Q&lt;br&gt;20&lt;br&gt;Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student's failure of the module. The QAA publish guidance related to 'levelness' in the Frameworks for Higher Education Qualifications and in their Subject Benchmark Statements. Schools/Institutes are also encouraged to refer to the Birmingham Graduate Attributes. &lt;br&gt;&lt;br&gt;ꮧ20.1&lt;br&gt;Demonstrate critical awareness of the need to manage heritage sites financially and administratively&lt;br&gt;20.2&lt;br&gt; Demonstratean understanding of the nature and importance of marketing in the context of heritage sites&lt;br&gt;20.3&lt;br&gt;Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function&lt;br&gt;20.4&lt;br&gt;Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard&lt;br&gt;21ꮨ(i.e. assessment that does not produce a mark that contributes to the overall module mark)&lt;br&gt; 10 minute presentation: Online presentation to Course Convenor on proposed heritage project and outline of key topics of business plan. Feedback will be provided immediately after online presentation verbally to student.&lt;br&gt;Q&lt;br&gt;22&lt;br&gt;Assessment category (multiple assessments should be included in the same category, e.g. a module with two written tasks and an oral presentation would be 'coursework 100%')&lt;br&gt;If the module is wholly or partly assessed by coursework, please state the overall weighting: &lt;br&gt;&lt;br&gt;100% &lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If the module is wholly or partly assessed by examination, please state the overall weighting: &lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;23&lt;br&gt;Additional information on the method(s) of summative assessment and weighting, ꮫ&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;["&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Modification&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;LM Heritage Management Practice&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;2024-25&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;No new resource requirements&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;No&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;As this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 07/08/2023&lt;br&gt;Approving body: SHAC PARC&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC via Chairs Action&lt;br&gt;&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.&lt;br&gt; &lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;4&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;5&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;6&lt;br&gt;Module title &lt;br&gt;LM The Business of Heritage &lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Module code(s) (if known)&lt;br&gt;38901&lt;br&gt;B&lt;br&gt;8&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;9&lt;br&gt;Module credits &lt;br&gt;20&lt;br&gt;B Q&lt;br&gt;10&lt;br&gt;Module attribute, if relevant&lt;br&gt;n/a&lt;br&gt;B&lt;br&gt;11&lt;br&gt;Semester in which the module will run&lt;br&gt;Semester 1&lt;br&gt;&lt;br&gt;B&lt;br&gt;12&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e. every student in the year should be registered on this module code):&lt;br&gt;515H LM International Heritage Management FT&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant):&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;None&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;14&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;15&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Edgbaston&lt;br&gt;&lt;br&gt;If 'other' please state here:&lt;br&gt;B Q SF&lt;br&gt;16&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected group&lt;br&gt;The school is committed to ensuring modules and programmes are inclusive and work closely with the University's Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.&lt;br&gt;Q &lt;br&gt;17&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;18&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)&lt;br&gt;B Q SF&lt;br&gt;18.1&lt;br&gt;Lecture&lt;br&gt;10&lt;br&gt;&lt;br&gt;18.2&lt;br&gt;Seminar &lt;br&gt;10&lt;br&gt;&lt;br&gt;18.3&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;18.4&lt;br&gt;Project supervision&lt;br&gt;&lt;br&gt;18.5&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;18.6&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;18.7&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;18.8&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;18.9&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;18.10&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;18.11&lt;br&gt;Guided independent study&lt;br&gt;180&lt;br&gt;&lt;br&gt;18.12&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;19&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students' awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.&lt;br&gt;Q&lt;br&gt;20&lt;br&gt;Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student's failure of the module. The QAA publish guidance related to 'levelness' in the Frameworks for Higher Education Qualifications and in their Subject Benchmark Statements. Schools/Institutes are also encouraged to refer to the Birmingham Graduate Attributes. &lt;br&gt;&lt;br&gt;ꮧ20.1&lt;br&gt;Demonstrate critical awareness of the need to manage heritage sites financially and administratively&lt;br&gt;20.2&lt;br&gt; Demonstratean understanding of the nature and importance of marketing in the context of heritage sites&lt;br&gt;20.3&lt;br&gt;Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function&lt;br&gt;20.4&lt;br&gt;Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard&lt;br&gt;21ꮨ(i.e. assessment that does not produce a mark that contributes to the overall module mark)&lt;br&gt; 10 minute presentation: Online presentation to Course Convenor on proposed heritage project and outline of key topics of business plan. Feedback will be provided immediately after online presentation verbally to student.&lt;br&gt;Q&lt;br&gt;22&lt;br&gt;Assessment category (multiple assessments should be included in the same category, e.g. a module with two written tasks and an oral presentation would be 'coursework 100%')&lt;br&gt;If the module is wholly or partly assessed by coursework, please state the overall weighting: &lt;br&gt;&lt;br&gt;100% &lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If the module is wholly or partly assessed by examination, please state the overall weighting: &lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;23&lt;br&gt;Additional information on the method(s) of summative assessment and weighting, ꮫ&lt;br&gt;1 x 3,000 word heritage project business plan (100%)&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;23.1&lt;br&gt;If there is an examination, is it centrally timetabled?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please specify the length of the examination: &lt;br&gt;&lt;br&gt;If 'yes' is this available for students to take overseas?&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;23.2&lt;br&gt;If there is an examination, select examination period&lt;br&gt;N/A - not examined&lt;br&gt;&lt;br&gt;B&lt;br&gt;&lt;br&gt;24&lt;br&gt;Please describe any internal hurdles&lt;br&gt;None&lt;br&gt;B Q&lt;br&gt;25&lt;br&gt;Method(s) of reassessment students would be expected to undertake should they fail to pass the module at the first attempt. The reassessment method(s) must enable students to ꮲ</v>
+      </c>
+      <c r="AU3" t="str">
+        <v/>
+      </c>
+      <c r="AV3" t="str">
+        <v/>
+      </c>
+      <c r="AW3" t="str">
+        <v>Dr Ioanna Katapidi</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AW2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AW3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated mappings due to new structure
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW3"/>
+  <dimension ref="A1:AW8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -553,37 +553,37 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2024/25</v>
+        <v>002025</v>
       </c>
       <c r="B2" t="str">
-        <v>07</v>
+        <v>08</v>
       </c>
       <c r="C2" t="str">
-        <v>Birmingham Business School</v>
+        <v>School of Social Policy</v>
       </c>
       <c r="D2" t="str">
-        <v>012</v>
+        <v>035</v>
       </c>
       <c r="E2" t="str">
-        <v>Management</v>
+        <v>Health Services Management Centre</v>
       </c>
       <c r="F2" t="str">
-        <v>261</v>
+        <v>122</v>
       </c>
       <c r="G2" t="str">
         <v>12</v>
       </c>
       <c r="H2" t="str">
-        <v>The Purposeful Leader</v>
+        <v>Emergency Preparedness, Response &amp; Resilience</v>
       </c>
       <c r="I2" t="str">
-        <v>LM The Purposeful Leader</v>
+        <v>LM Eme Prepare Res &amp; Resil Dub</v>
       </c>
       <c r="J2" t="str">
-        <v>LM The Purposeful Leader</v>
+        <v>LM Emergency Preparedness, Response &amp; Resilience</v>
       </c>
       <c r="K2" t="str">
-        <v>= £16,500) SFAre there any related programme modifications? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?YesB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryThere were a series of consultations with alumni, existing students and sponsors of prospective students. In each consultation programme aims, programme learning outcomes and programme structure was shared and feedback was collected.   The consultations took place on the following dates:   06/10/2022: Consultations with Alumni in relevant management positions 21/10/2022: On 21st October there were 3 consultations with existing students, one for each of the locations PT MBA Singapore Institute of Management; FT MBA (Edgbaston) and Exec MBA (Edgbaston)  Following the consultations above feedback was taken on board and proposal amended accordingly where appropriate.  The updated proposal was used for final consultations with employers sponsoring their team to join our PGDip and follow into the Executive MBA in the UK. Employer consultations took place on the following dates:  25th November 2022 15th December 2022 6th January 2022 QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)This module is not available for students outside the programmes in which it is a core module.   There is a Dubai equivalent based being proposed as the new MBA will also be offered in Dubai. As this is a new offer in Dubai, there is no programme lead appointed, but it is in line with the plans of Dubai to offer such programme in the Dubai Campus. QIf the module/programme is subject to accreditation, please provide details of consultation with the professional body QIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision Q8ApprovalSchool/InstituteDate: 07/02/2023Approving body: SPARCCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{Birmingham Business School[Management] module delivered in collaboration with another organisation? YesIf ‘yes’ please state the organisation’s name:Singapore Institute of ManagementB Q SFIs this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)Association of MBAs (AMBA) ʓThe Purposeful Leader #</v>
+        <v>TBC</v>
       </c>
       <c r="L2" t="str">
         <v>LM</v>
@@ -598,43 +598,43 @@
         <v>Z</v>
       </c>
       <c r="P2" t="str">
-        <v/>
+        <v>131</v>
       </c>
       <c r="Q2" t="str">
-        <v>N200</v>
+        <v>B900</v>
       </c>
       <c r="R2" t="str">
-        <v>100089</v>
+        <v>100260</v>
       </c>
       <c r="S2" t="str">
-        <v>Master of Business Administration SIM Part-Time (Code TBC)As an optional module (including any information about its grouping, if relevant):</v>
+        <v>MSc Global Health System Leadership (Dubai campus)PG Dip Global Health System Leadership (Dubai campus) (alternative qual)As an optional module (including any information about its grouping, if relevant):PG Cert Global Health System Leadership (Dubai campus) (alternative qual)</v>
       </c>
       <c r="T2" t="str">
         <v/>
       </c>
       <c r="U2" t="str">
-        <v>None</v>
+        <v>N/A</v>
       </c>
       <c r="V2" t="str">
-        <v>None</v>
+        <v>N/A</v>
       </c>
       <c r="W2" t="str">
-        <v>Other (please state below)</v>
+        <v>UoB Campus Dubai</v>
       </c>
       <c r="X2" t="str">
-        <v/>
+        <v>U</v>
       </c>
       <c r="Y2" t="str">
-        <v>This module requires an exemption from the semesterised teaching year. This research module requires to be an open-ended module, which students complete with the taught element, supplying a final project proposal as part of their assessment portfolio.</v>
+        <v>N/A</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -643,7 +643,7 @@
         <v>0</v>
       </c>
       <c r="AE2">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="AF2">
         <v>0</v>
@@ -658,200 +658,945 @@
         <v>0</v>
       </c>
       <c r="AJ2">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="AK2">
         <v>0</v>
       </c>
       <c r="AL2" t="str">
-        <v>This is a reflective and developmental module for students to explore their leadership and career aspirations in relation to their purposive values. The module will include four types of learning engagements: &lt;br&gt;An examination of current values-based and purpose-led theories of leadership. Students will be encouraged to critically examine theories they study, and apply them to their own contexts and experiences; &lt;br&gt;Critical reflective practice about how they enact and embody purposeful/values-based leading and aspects of their organizational context which impacts on their ability to lead from this orientation; &lt;br&gt;Professional skills development activities, including coaching to enhance their capacity to lead effectively that will be coordinated and delivered by the BBS Career team; &lt;br&gt;The development of reflective practitioner and associated research skills, culminating in the creation of a plan to underpin career aspirations. &lt;br&gt; &lt;br&gt;Students will be expected to keep a portfolio of reflective practice on their purposeful leadership approach throughout the module, and how what they have learned on different modules is influencing this.</v>
+        <v>Globally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region face many diverse conflict and instability and double burden of disease. &lt;br&gt;&lt;br&gt;This module will allow students to develop an integrated, theoretical and practical knowledge of Health Emergency Preparedness Response and Resilience (EPRR) and to develop the capacity to apply this knowledge in the field of global health system while considering the intersection of health security, primary health care and health promotion, and interface with multiple non-health sectors and stakeholders at national, regional and global levels.&lt;br&gt;&lt;br&gt;The module enables students to develop a Health Emergency Preparedness, Response and Resilience plan including, collaborative surveillance; community protection; safe and scalable care fundamentals in response to a health emergency to advance the global architecture for EPRR and health security.</v>
       </c>
       <c r="AM2" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Critically analyse theories and practice of purposeful leadership &lt;/li&gt;&lt;li&gt;Reflect critically on their own leadership practice and the way in which it reflects their purpose &lt;/li&gt;&lt;li&gt;Design and plan an independent project which identifies a business issue of strategic relevance to their organization or plan for an entrepreneurial development. &lt;/li&gt;&lt;li&gt;Identify their leadership skills gaps, demonstrate and reflect upon actions taken to address the gaps through authentic assessment, coaching, mentoring training, reflective group discussions and evaluate your learning journey.&lt;/li&gt;&lt;/ul&gt;</v>
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Demonstrate an integrated, theoretical and practical knowledge of Health Emergency Preparedness Response and Resilience (EPRR).&lt;/li&gt;&lt;li&gt;Demonstrate the ability to synthesise and critically analyse theory and evidence from a variety of sources on a range of aspects in the field of health emergency preparedness response and resilience while considering the intersection of health security, primary health care and health promotion, and interface with multiple non-health sectors and stakeholders at national, regional and global levels.&lt;/li&gt;&lt;li&gt;Analyse and evaluate health emergency preparedness response and resilience plans across different complex, stable and fragile conflict-affected vulnerable settings (FCV), cultures and countries using theoretical and comparative approaches and tools to present a coherent critique. &lt;/li&gt;&lt;li&gt;To develop capabilities in health emergency preparedness response and resilience planning including, collaborative surveillance; community protection; safe and scalable care fundamentals in response to a health emergency to advance the global architecture for EPRR and health security.&lt;/li&gt;&lt;/ul&gt;</v>
       </c>
       <c r="AN2" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{Birmingham Business School[Management𓏉The Purposeful Leader`2024/25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThis module is a 20-credit compulsory module proposed in conjunction with the new Executive Master of Business Administration programme proposal.  It is one of the two core integrative modules that will anchor the responsible business vision of the MBA suite of programmes by focusing on what it means in terms of students’ purposeful leadership approach and how to put their values and approach into practice and related personal and professional development activities throughout the programme. It is key for delivering the strategic learning outcomes of the Business School around responsible business and thought leadership.  The module is also required to meet AMBA programme design objectives and to meet Senior Leader Apprenticeship Standards with respect to specific knowledge, skills and behaviours (KSBs), as listed below.   Knowledge K6: Ethics and values-based leadership theories and principles. K10: Organisational; team dynamics and how to build engagement and develop high performance, agile and collaborative cultures. K12: Influencing and negotiating strategies both upwards and outwards. K13: The external and social and political environment and use of diplomacy with diverse groups of internal and external stakeholders. K14 Working with board and company leadership structures. K18: Coaching and mentoring techniques. K19: Approaches to developing a CSR programme. AMBA:  Business research methods and consulting skills Leadership and entrepreneurship An understanding of the impact of ethics and risk management on issues of CSR, sustainable development and societal well being  Skills S2: Set strategic direction and gain support for it from key stakeholders S7: Challenge strategies and operations in terms of ethics, responsibility, sustainability, resource allocation and business continuity; risk management. S13: Use personal presence and storytelling to articulate and translate vision into operational strategies, demonstrate clarity in thinking such as consideration of sustainable approaches. S14: Create an inclusive culture, encouraging diversity and difference and promoting well-being. S15: Give and receive feedback at all levels, building confidence and developing trust, and enable people to take risks and challenge where appropriate. S17: Lead and influence people, building constructive working relationships across teams, using matrix management where required. S20: Lead within their area of control, authority, influencing both upwards and outwards, negotiating and using advocacy skills to build reputation and effective collaboration. AMBA: Leadership Dealing with ambiguity Values  Behaviours B2: Take personal accountability aligned to clear values. B4: Value difference and champion diversity. B5: Seek continuous professional development opportunities for self and wider team.  The Purposeful Leader module together with one of the 40 credits electives for final project modules involves student research and make up 60 credits of independent learning based on student research within the MBA Programme. Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)For this module to be delivered as proposed it requires a new Professional service member of staff Grade 7 to be added to the Careers team to manage all leadership coaches and manage and deliver 26h of practical classes across the portfolio.    There is an additional cost of £300/student for the external coach. This consists of 3 coaching sessions of 1 hour each at a rate of £100/hour. The cost of coaches per cohort for the Executive MBA UK is estimated at £16,500. This number is a function of recruitment. (Cost x target: £300 x 55 students = £16,500) SFAre there any related programme modifications? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?YesB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryThere were a series of consultations with alumni, existing students and sponsors of prospective students. In each consultation programme aims, programme learning outcomes and programme structure was shared and feedback was collected.   The consultations took place on the following dates:   06/10/2022: Consultations with Alumni in relevant management positions 21/10/2022: On 21st October there were 3 consultations with existing students, one for each of the locations PT MBA Singapore Institute of Management; FT MBA (Edgbaston) and Exec MBA (Edgbaston)  Following the consultations above feedback was taken on board and proposal amended accordingly where appropriate.  The updated proposal was used for final consultations with employers sponsoring their team to join our PGDip and follow into the Executive MBA in the UK. Employer consultations took place on the following dates:  25th November 2022 15th December 2022 6th January 2022 QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)This module is not available for students outside the programmes in which it is a core module.   There is a Dubai equivalent based being proposed as the new MBA will also be offered in Dubai. As this is a new offer in Dubai, there is no programme lead appointed, but it is in line with the plans of Dubai to offer such programme in the Dubai Campus. QIf the module/programme is subject to accreditation, please provide details of consultation with the professional body QIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision Q8ApprovalSchool/InstituteDate: 07/02/2023Approving body: SPARCCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{Birmingham Business School[Management] module delivered in collaboration with another organisation? YesIf ‘yes’ please state the organisation’s name:Singapore Institute of ManagementB Q SFIs this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)Association of MBAs (AMBA) ʓThe Purposeful Leader #TBC=Masters - LM@20$, if relevantN/A⸮Full TermﱙAs a compulsory module (i.e. every student in the year should be ǕMaster of Business Administration SIM Part-Time (Code TBC)As an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableNoneÂNoneÃOther (please state below)ÄTeaching will take place both at the Singapore Institute of Management and online.   Ä on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupOur School fully supports the University’s commitment to inclusivity.  All modules are designed to promote equality of access to teaching sessions and assessment opportunities.  The School engages with Student Services to ensure that students with additional support needs receive appropriate support for their learning and that, where needed, reasonable adjustments are made to delivery of teaching and to examination arrangements.  Q ÅThis module requires an exemption from the semesterised teaching year. This research module requires to be an open-ended module, which students complete with the taught element, supplying a final project proposal as part of their assessment portfolio. Æ effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q ÇÈ Éꮛꮜꮝ26ꮞꮟꮠꮡꮢ174ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis is a reflective and developmental module for students to explore their leadership and career aspirations in relation to their purposive values. The module will include four types of learning engagements:  An examination of current values-based and purpose-led theories of leadership.  Students will be encouraged to critically examine theories they study, and apply them to their own contexts and experiences; Critical reflective practice about how they enact and embody purposeful/values-based leading and aspects of their organizational context which impacts on their ability to lead from this orientation; Professional skills development activities, including coaching to enhance their capacity to lead effectively that will be coordinated and delivered by the BBS Career team; The development of reflective practitioner and associated research skills, culminating in the creation of a plan to underpin career aspirations.  Students will be expected to keep a portfolio of reflective practice on their purposeful leadership approach throughout the module, and how what they have learned on different modules is influencing this.  ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:Critically analyse theories and practice of purposeful leadership Reflect critically on their own leadership practice and the way in which it reflects their purpose Design and plan an independent project which identifies a business issue of strategic relevance to their organization or plan for an entrepreneurial development. Identify their leadership skills gaps, demonstrate and reflect upon actions taken to address the gaps through authentic assessment, coaching, mentoring training, reflective group discussions and evaluate your learning journey. ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Social Policy[Health Services Management Centre𓏉Emergency, Preparedness, Response &amp; Resilience `January 2025¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThis module provides an integrated, theoretical and practical knowledge of Health Emergency, Preparedness, Response and Resilience (EPRR) and to develop the capacity to apply this knowledge in the field of global health system while considering the intersection of health security, primary health care and health promotion, and interface with multiple non-health sectors and stakeholders at national, regional and global levels.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Resource implications have been arranged across Edgbaston and Dubai campuses.SFAre there any related programme modifications? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?YesB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryN/AQIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 10/08/2023Approving body: SEQC (Chair’s action)College (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC (Chair’s action)Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Social Policy[Health Services Management Centre] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)N/AʓEmergency Preparedness, Response &amp; Resilience#TBC=Masters - LM@20$, if relevantN/A⸮Semester 2ﱙAs a compulsory module (i.e. every student in the year should be ǕMSc Global Health System Leadership (Dubai campus)PG Dip Global Health System Leadership (Dubai campus) (alternative qual)As an optional module (including any information about its grouping, if relevant):PG Cert Global Health System Leadership (Dubai campus) (alternative qual)À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁN/A☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/AÂN/AÃUoB Campus DubaiÄÄ on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThis programme has been designed to be fully inclusive.  As a University/Department we are committed to ensuring that all our modules/programmes are inclusive and that we comply fully with the Equality Act of 2010. There are no barriers to applications, access, or progression.  The department always considers whether any parts of module delivery might prove disadvantageous to any group.  Module materials are designed to be fully accessible and are made available in advance to students electronically and, where requested, hard copy form. Further adjustments are made where appropriate to support students with SSAs/RAPs.Q ÅN/AÆ effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç10È 10É10ꮛꮜꮝ10ꮞꮟꮠꮡꮢ160ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥGlobally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region face many diverse conflict and instability and double burden of disease. This module will allow students to develop an integrated, theoretical and practical knowledge of Health Emergency Preparedness Response and Resilience (EPRR) and to develop the capacity to apply this knowledge in the field of global health system while considering the intersection of health security, primary health care and health promotion, and interface with multiple non-health sectors and stakeholders at national, regional and global levels.The module enables students to develop a Health Emergency Preparedness, Response and Resilience plan including, collaborative surveillance; community protection; safe and scalable care fundamentals in response to a health emergency to advance the global architecture for EPRR and health security.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:Demonstrate an integrated, theoretical and practical knowledge of Health Emergency Preparedness Response and Resilience (EPRR).Demonstrate the ability to synthesise and critically analyse theory and evidence from a variety of sources on a range of aspects in the field of health emergency preparedness response and resilience while considering the intersection of health security, primary health care and health promotion, and interface with multiple non-health sectors and stakeholders at national, regional and global levels.Analyse and evaluate health emergency preparedness response and resilience plans across different complex, stable and fragile conflict-affected vulnerable settings (FCV), cultures and countries using theoretical and comparative approaches and tools to present a coherent critique. To develop capabilities in health emergency preparedness response and resilience planning including, collaborative surveillance; community protection; safe and scalable care fundamentals in response to a health emergency to advance the global architecture for EPRR and health security.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
       </c>
       <c r="AO2" t="str">
-        <v>&lt;br&gt;Portfolio of work which will include: &lt;br&gt; &lt;br&gt;Reflective log of their experimenting with purposeful leadership practice; (A summary statement of what has been learned and a plan for further development up to 3000 words, 75% of the grade) &lt;br&gt;Independent project proposal (1000 words or equivalent, 25% of the grade) &lt;br&gt;&lt;br&gt;</v>
+        <v>&lt;br&gt;One 2,500-word assignment (60%), and one in module 10 minute group-based presentation (40%).&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AP2" t="str">
-        <v>No</v>
+        <v>N/A - not examined</v>
       </c>
       <c r="AQ2" t="str">
         <v>N/A - not examined</v>
       </c>
       <c r="AR2" t="str">
-        <v>None</v>
+        <v>N/A</v>
       </c>
       <c r="AS2" t="str">
-        <v>A portfolio including: &lt;br&gt; &lt;br&gt;Reflective log of their experimenting with purposeful leadership practice; (A summary statement of what has been learned and a plan for further development up to 3000 words, 75% of the grade) &lt;br&gt;Independent project proposal (1000 words or equivalent, 25% of the grade) &lt;br&gt;</v>
+        <v>Resubmission of failed component: 2500-word assignment (60%); Individual assignment 1000 words reflective piece. (40%).</v>
       </c>
       <c r="AT2" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Portfolio of work which will include: &lt;br&gt; &lt;br&gt;Reflective log of their experimenting with purposeful leadership practice; (A summary statement of what has been learned and a plan for further development up to 3000 words, 75% of the grade) &lt;br&gt;Independent project proposal (1000 words or equivalent, 25% of the grade) &lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;A portfolio including: &lt;br&gt; &lt;br&gt;Reflective log of their experimenting with purposeful leadership practice; (A summary statement of what has been learned and a plan for further development up to 3000 words, 75% of the grade) &lt;br&gt;Independent project proposal (1000 words or equivalent, 25% of the grade) &lt;br&gt;</v>
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;One 2,500-word assignment (60%), and one in module 10 minute group-based presentation (40%).&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of failed component: 2500-word assignment (60%); Individual assignment 1000 words reflective piece. (40%).</v>
       </c>
       <c r="AU2" t="str">
-        <v>Full Term</v>
+        <v>Semester 2</v>
       </c>
       <c r="AV2" t="str">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AW2" t="str">
-        <v>Donna Ladkin; Joanne Murphy and Sandy Purewal</v>
+        <v>Dr. Ayat Abu-Agla a.s.y.abu-agla@bham.ac.uk</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2024-25</v>
+        <v>002025</v>
       </c>
       <c r="B3" t="str">
-        <v>09</v>
+        <v/>
       </c>
       <c r="C3" t="str">
-        <v>School of History and Cultures</v>
+        <v>Institute of Applied Health ResearchSchool of Social Policy</v>
       </c>
       <c r="D3" t="str">
-        <v>047</v>
+        <v/>
       </c>
       <c r="E3" t="str">
-        <v>History</v>
+        <v>Health Economics UnitHealth Service Management Centre</v>
       </c>
       <c r="F3" t="str">
-        <v>225</v>
+        <v/>
       </c>
       <c r="G3" t="str">
-        <v>11</v>
+        <v/>
       </c>
       <c r="H3" t="str">
-        <v/>
+        <v>Global Health Economics</v>
       </c>
       <c r="I3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>LM Global Health Economics Dub</v>
       </c>
       <c r="J3" t="str">
-        <v xml:space="preserve"> </v>
+        <v>LM Global Health Economics</v>
       </c>
       <c r="K3" t="str">
-        <v/>
+        <v>TBC</v>
       </c>
       <c r="L3" t="str">
-        <v/>
+        <v>LM</v>
       </c>
       <c r="M3" t="str">
-        <v/>
+        <v>20</v>
       </c>
       <c r="N3" t="str">
-        <v>UG</v>
+        <v>GT</v>
       </c>
       <c r="O3" t="str">
         <v>Z</v>
       </c>
       <c r="P3" t="str">
-        <v>139</v>
+        <v/>
       </c>
       <c r="Q3" t="str">
-        <v>V100</v>
+        <v/>
       </c>
       <c r="R3" t="str">
-        <v>100302</v>
+        <v/>
       </c>
       <c r="S3" t="str">
-        <v>515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):</v>
+        <v>MSc Global Health System Leadership (Dubai campus)As an optional module (including any information about its grouping, if relevant):MPH (Dubai) 667G / 668G</v>
       </c>
       <c r="T3" t="str">
         <v/>
       </c>
       <c r="U3" t="str">
-        <v>None</v>
+        <v>N/A</v>
       </c>
       <c r="V3" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of History and Cultures[History𓏉LM Heritage Management Practice`2024-25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThe change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)No new resource requirementsSFAre there any related programme modifications? (for proposals and significant module modifications)NoB QIf yes, have they been submitted for approval alongside this proposal?N/AB Q7Consultation (required for modifications, advised for proposals, where applicable)Prospective/existing students where necessaryAs this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 07/08/2023Approving body: SHAC PARCCollege (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC via Chairs ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.1{School of History and CulturesB2Department (if applicable)HistoryB3Is the module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SF4Is this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SF5Accrediting body (if applicable)N/AQ6Module title LM The Business of Heritage  B Q7Module code(s) (if known)38901B8Module levelMasters - LMB Q9Module credits 20B Q10Module attribute, if relevantn/aB11Semester in which the module will runSemester 1B12Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/A14Â</v>
+        <v>N/A</v>
       </c>
       <c r="W3" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of History and Cultures[History𓏉LM Heritage Management Practice`2024-25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThe change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)No new resource requirementsSFAre there any related programme modifications? (for proposals and significant module modifications)NoB QIf yes, have they been submitted for approval alongside this proposal?N/AB Q7Consultation (required for modifications, advised for proposals, where applicable)Prospective/existing students where necessaryAs this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 07/08/2023Approving body: SHAC PARCCollege (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC via Chairs ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.1{School of History and CulturesB2Department (if applicable)HistoryB3Is the module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SF4Is this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SF5Accrediting body (if applicable)N/AQ6Module title LM The Business of Heritage  B Q7Module code(s) (if known)38901B8Module levelMasters - LMB Q9Module credits 20B Q10Module attribute, if relevantn/aB11Semester in which the module will runSemester 1B12Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/A14ÂN/AB15Where will the teaching take place? UoB Campus Edgbaston</v>
+        <v>UoB Campus Dubai</v>
       </c>
       <c r="X3" t="str">
-        <v>B</v>
+        <v>U</v>
       </c>
       <c r="Y3" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of History and Cultures[History𓏉LM Heritage Management Practice`2024-25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThe change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)No new resource requirementsSFAre there any related programme modifications? (for proposals and significant module modifications)NoB QIf yes, have they been submitted for approval alongside this proposal?N/AB Q7Consultation (required for modifications, advised for proposals, where applicable)Prospective/existing students where necessaryAs this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 07/08/2023Approving body: SHAC PARCCollege (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC via Chairs ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.1{School of History and CulturesB2Department (if applicable)HistoryB3Is the module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SF4Is this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SF5Accrediting body (if applicable)N/AQ6Module title LM The Business of Heritage  B Q7Module code(s) (if known)38901B8Module levelMasters - LMB Q9Module credits 20B Q10Module attribute, if relevantn/aB11Semester in which the module will runSemester 1B12Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/A14ÂN/AB15Where will the teaching take place? UoB Campus EdgbastonÄB Q SF16Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe school is committed to ensuring modules and programmes are inclusive and work closely with the University’s Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.Q 17Å</v>
+        <v>N/A</v>
       </c>
       <c r="Z3">
-        <v>NaN</v>
+        <v>10</v>
       </c>
       <c r="AA3">
-        <v>NaN</v>
+        <v>10</v>
       </c>
       <c r="AB3">
-        <v>NaN</v>
+        <v>10</v>
       </c>
       <c r="AC3">
-        <v>NaN</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <v>NaN</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <v>NaN</v>
+        <v>10</v>
       </c>
       <c r="AF3">
-        <v>NaN</v>
+        <v>0</v>
       </c>
       <c r="AG3">
-        <v>NaN</v>
+        <v>0</v>
       </c>
       <c r="AH3">
-        <v>NaN</v>
+        <v>0</v>
       </c>
       <c r="AI3">
-        <v>NaN</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
-        <v>NaN</v>
+        <v>160</v>
       </c>
       <c r="AK3">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="AL3" t="str">
-        <v>["&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Modification&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;LM Heritage Management Practice&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;2024-25&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;No new resource requirements&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;No&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;As this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 07/08/2023&lt;br&gt;Approving body: SHAC PARC&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC via Chairs Action&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.&lt;br&gt; &lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;4&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;5&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;6&lt;br&gt;Module title &lt;br&gt;LM The Business of Heritage &lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Module code(s) (if known)&lt;br&gt;38901&lt;br&gt;B&lt;br&gt;8&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;9&lt;br&gt;Module credits &lt;br&gt;20&lt;br&gt;B Q&lt;br&gt;10&lt;br&gt;Module attribute, if relevant&lt;br&gt;n/a&lt;br&gt;B&lt;br&gt;11&lt;br&gt;Semester in which the module will run&lt;br&gt;Semester 1&lt;br&gt;&lt;br&gt;B&lt;br&gt;12&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e. every student in the year should be registered on this module code):&lt;br&gt;515H LM International Heritage Management FT&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant):&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;None&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;14&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;15&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Edgbaston&lt;br&gt;&lt;br&gt;If 'other' please state here:&lt;br&gt;B Q SF&lt;br&gt;16&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected group&lt;br&gt;The school is committed to ensuring modules and programmes are inclusive and work closely with the University's Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.&lt;br&gt;Q &lt;br&gt;17&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;18&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)&lt;br&gt;B Q SF&lt;br&gt;18.1&lt;br&gt;Lecture&lt;br&gt;10&lt;br&gt;&lt;br&gt;18.2&lt;br&gt;Seminar &lt;br&gt;10&lt;br&gt;&lt;br&gt;18.3&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;18.4&lt;br&gt;Project supervision&lt;br&gt;&lt;br&gt;18.5&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;18.6&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;18.7&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;18.8&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;18.9&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;18.10&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;18.11&lt;br&gt;Guided independent study&lt;br&gt;180&lt;br&gt;&lt;br&gt;18.12&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;19&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥ</v>
+        <v>Globally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region faces many diverse conflict and instability and double burden of disease. &lt;br&gt;&lt;br&gt;This module examines issues relating to health economics within health systems in high, middle, and low-income countries. It introduces key concepts relating to this area of study, applying a comparative approach to the study of different health economic theories, tools, foundational concepts, and approaches to critically evaluate the impact on global health system and examine long-term sustainability and resilience approaches to combat future shocks and establish the foundation for change, along the \"financing-governance-service delivery\" nexus. &lt;br&gt;&lt;br&gt;The module enables students to develop a health strategy resource mobilization and costing plan applying appropriate methods and tools of economic evaluation and health financing for health development to advance the UHC and SDG agenda. &lt;br&gt;&lt;br&gt;Topics include: Introduction to Health economics theories and tools; Economic evaluation and Health Financing; and Resource mobilisation and Costing.</v>
       </c>
       <c r="AM3" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;20.1&lt;/li&gt;&lt;li&gt;Demonstrate critical awareness of the need to manage heritage sites financially and administratively&lt;/li&gt;&lt;li&gt;20.2&lt;/li&gt;&lt;li&gt; Demonstratean understanding of the nature and importance of marketing in the context of heritage sites&lt;/li&gt;&lt;li&gt;20.3&lt;/li&gt;&lt;li&gt;Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function&lt;/li&gt;&lt;li&gt;20.4&lt;/li&gt;&lt;li&gt;Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard&lt;/li&gt;&lt;li&gt;21&lt;/li&gt;&lt;/ul&gt;</v>
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Demonstrate an understanding of key concepts of different health economic theories, tools and foundational concepts and apply these to different health systems.&lt;/li&gt;&lt;li&gt;Demonstrate the ability to synthesise and critically analyse theory and evidence from a variety of sources on economic evaluation and apply these to critically evaluate the impact on global health system.&lt;/li&gt;&lt;li&gt;Show understanding of core economic concepts/theory relating to markets and market failure&lt;/li&gt;&lt;li&gt;Critically analyse theory and concepts related to the study of health financing of global health systems in relation to concepts of equity and efficiency&lt;/li&gt;&lt;li&gt;Demonstrate the ability to synthesise and critically analyse theory and evidence from a variety of sources on costing health strategy and apply these to develop a costing plan.&lt;/li&gt;&lt;li&gt;understand/explore health economics approaches for the assessment of the progress towards the attainment of UHC and SDGs&lt;/li&gt;&lt;/ul&gt;</v>
       </c>
       <c r="AN3" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of History and Cultures[History𓏉LM Heritage Management Practice`2024-25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThe change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)No new resource requirementsSFAre there any related programme modifications? (for proposals and significant module modifications)NoB QIf yes, have they been submitted for approval alongside this proposal?N/AB Q7Consultation (required for modifications, advised for proposals, where applicable)Prospective/existing students where necessaryAs this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 07/08/2023Approving body: SHAC PARCCollege (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC via Chairs ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.1{School of History and CulturesB2Department (if applicable)HistoryB3Is the module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SF4Is this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SF5Accrediting body (if applicable)N/AQ6Module title LM The Business of Heritage  B Q7Module code(s) (if known)38901B8Module levelMasters - LMB Q9Module credits 20B Q10Module attribute, if relevantn/aB11Semester in which the module will runSemester 1B12Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/A14ÂN/AB15Where will the teaching take place? UoB Campus EdgbastonÄB Q SF16Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe school is committed to ensuring modules and programmes are inclusive and work closely with the University’s Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.Q 17ÅN/AQ18Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)B Q SF18.1Lecture1018.2È 1018.3É18.4ꮛ18.5ꮜ18.6ꮝ18.7ꮞ18.8ꮟ18.9ꮠ18.10ꮡ18.11ꮢ18018.12ꮣ19ꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students’ awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.Q20Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:20.1Demonstrate critical awareness of the need to manage heritage sites financially and administratively20.2 Demonstratean understanding of the nature and importance of marketing in the context of heritage sites20.3Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function20.4Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard21ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{Institute of Applied Health ResearchSchool of Social Policy[Health Economics UnitHealth Service Management Centre𓏉Global Health Economics`January 2025¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFTo successfully lead global health systems requires a critical understanding of economic theories, tools and foundational concepts to support sustainable development and growth.This module is designed to equip students with the knowledge required to understand the relevance of economics in informing decision-making in health care systems and broader policy sectors and the core skills needed to interpret and appraise economic evaluations.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Resource implications have been arranged across Edgbaston and Dubai campuses.SFAre there any related programme modifications? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?YesB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryN/AQIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 10/08/2023/  30/08/2023Approving body: Social Policy SEQC (Chair’s Action) / IAHR HoE, Louise JacksonCollege (mandatory for proposals only)Date: 31/08/2023Approving body: MDS CQAAC via Chair’s ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{Institute of Applied Health ResearchSocial Policy[Health Economics Unit Health Services Management Centre] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School/Institute at UoB?YesIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Health Service Management Centre- School of Social Policy 40%Health Economic Unit- Institute of Applied Health Research 60%B SFAccrediting body (if applicable)N/AʓGlobal Health Economics#TBC=Masters - LM@20$, if relevantN/A⸮Semester 2ﱙAs a compulsory module (i.e. every student in the year should be ǕMSc Global Health System Leadership (Dubai campus)As an optional module (including any information about its grouping, if relevant):MPH (Dubai) 667G / 668GÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁN/A☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/AÂN/AÃUoB Campus DubaiÄÄ on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThis programme has been designed to be fully inclusive.  As a University/Department we are committed to ensuring that all our modules/programmes are inclusive and that we comply fully with the Equality Act of 2010. There are no barriers to applications, access, or progression.  The department always considers whether any parts of module delivery might prove disadvantageous to any group.  Module materials are designed to be fully accessible and are made available in advance to students electronically and, where requested, hard copy form. Further adjustments are made where appropriate to support students with SSAs/RAPs.Q ÅN/AÆ effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç10È 10É10ꮛꮜꮝ10ꮞꮟꮠꮡꮢ160ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥGlobally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region faces many diverse conflict and instability and double burden of disease. This module examines issues relating to health economics within health systems in high, middle, and low-income countries. It introduces key concepts relating to this area of study, applying a comparative approach to the study of different health economic theories, tools, foundational concepts, and approaches to critically evaluate the impact on global health system and examine long-term sustainability and resilience approaches to combat future shocks and establish the foundation for change, along the “financing-governance-service delivery” nexus.  The module enables students to develop a health strategy resource mobilization and costing plan applying appropriate methods and tools of economic evaluation and health financing for health development to advance the UHC and SDG agenda. Topics include: Introduction to Health economics theories and tools; Economic evaluation and Health Financing; and Resource mobilisation and Costing.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:Demonstrate an understanding of key concepts of different health economic theories, tools and foundational concepts and apply these to different health systems.Demonstrate the ability to synthesise and critically analyse theory and evidence from a variety of sources on economic evaluation and apply these to critically evaluate the impact on global health system.Show understanding of core economic concepts/theory relating to markets and market failureCritically analyse theory and concepts related to the study of health financing of global health systems in relation to concepts of equity and efficiencyDemonstrate the ability to synthesise and critically analyse theory and evidence from a variety of sources on costing health strategy and apply these to develop a costing plan.understand/explore health economics approaches for the assessment of the progress towards the attainment of UHC and SDGsꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
       </c>
       <c r="AO3" t="str">
-        <v>["&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Modification&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;LM Heritage Management Practice&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;2024-25&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).&lt;br&gt;&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;No new resource requirements&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;No&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;As this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 07/08/2023&lt;br&gt;Approving body: SHAC PARC&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC via Chairs Action&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.&lt;br&gt; &lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;4&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;5&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;6&lt;br&gt;Module title &lt;br&gt;LM The Business of Heritage &lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Module code(s) (if known)&lt;br&gt;38901&lt;br&gt;B&lt;br&gt;8&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;9&lt;br&gt;Module credits &lt;br&gt;20&lt;br&gt;B Q&lt;br&gt;10&lt;br&gt;Module attribute, if relevant&lt;br&gt;n/a&lt;br&gt;B&lt;br&gt;11&lt;br&gt;Semester in which the module will run&lt;br&gt;Semester 1&lt;br&gt;&lt;br&gt;B&lt;br&gt;12&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e. every student in the year should be registered on this module code):&lt;br&gt;515H LM International Heritage Management FT&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant):&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;None&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;14&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;15&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Edgbaston&lt;br&gt;&lt;br&gt;If 'other' please state here:&lt;br&gt;B Q SF&lt;br&gt;16&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected group&lt;br&gt;The school is committed to ensuring modules and programmes are inclusive and work closely with the University's Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.&lt;br&gt;Q &lt;br&gt;17&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;18&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)&lt;br&gt;B Q SF&lt;br&gt;18.1&lt;br&gt;Lecture&lt;br&gt;10&lt;br&gt;&lt;br&gt;18.2&lt;br&gt;Seminar &lt;br&gt;10&lt;br&gt;&lt;br&gt;18.3&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;&lt;br&gt;18.4&lt;br&gt;Project supervision&lt;br&gt;&lt;br&gt;&lt;br&gt;18.5&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;&lt;br&gt;18.6&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;&lt;br&gt;18.7&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;&lt;br&gt;18.8&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;&lt;br&gt;18.9&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;&lt;br&gt;18.10&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;&lt;br&gt;18.11&lt;br&gt;Guided independent study&lt;br&gt;180&lt;br&gt;&lt;br&gt;18.12&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;&lt;br&gt;19&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students' awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.&lt;br&gt;Q&lt;br&gt;20&lt;br&gt;Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student's failure of the module. The QAA publish guidance related to 'levelness' in the Frameworks for Higher Education Qualifications and in their Subject Benchmark Statements. Schools/Institutes are also encouraged to refer to the Birmingham Graduate Attributes. &lt;br&gt;&lt;br&gt;ꮧ20.1&lt;br&gt;Demonstrate critical awareness of the need to manage heritage sites financially and administratively&lt;br&gt;20.2&lt;br&gt; Demonstratean understanding of the nature and importance of marketing in the context of heritage sites&lt;br&gt;20.3&lt;br&gt;Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function&lt;br&gt;20.4&lt;br&gt;Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard&lt;br&gt;21ꮨ(i.e. assessment that does not produce a mark that contributes to the overall module mark)&lt;br&gt; 10 minute presentation: Online presentation to Course Convenor on proposed heritage project and outline of key topics of business plan. Feedback will be provided immediately after online presentation verbally to student.&lt;br&gt;Q&lt;br&gt;22&lt;br&gt;Assessment category (multiple assessments should be included in the same category, e.g. a module with two written tasks and an oral presentation would be 'coursework 100%')&lt;br&gt;If the module is wholly or partly assessed by coursework, please state the overall weighting: &lt;br&gt;&lt;br&gt;100% &lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;&lt;br&gt;If the module is wholly or partly assessed by examination, please state the overall weighting: &lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;23&lt;br&gt;Additional information on the method(s) of summative assessment and weighting, ꮫ</v>
+        <v>&lt;br&gt;&lt;br&gt;2,000-word assignment&lt;br&gt;&lt;br&gt;50% weighting &lt;br&gt;50% Pass Mark &lt;br&gt;&lt;br&gt;1-hour face to face exam&lt;br&gt;50% weighting &lt;br&gt;50% Pass Mark&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AP3" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AQ3" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of History and Cultures[History𓏉LM Heritage Management Practice`2024-25¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThe change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)No new resource requirementsSFAre there any related programme modifications? (for proposals and significant module modifications)NoB QIf yes, have they been submitted for approval alongside this proposal?N/AB Q7Consultation (required for modifications, advised for proposals, where applicable)Prospective/existing students where necessaryAs this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.QIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 07/08/2023Approving body: SHAC PARCCollege (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC via Chairs ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.1{School of History and CulturesB2Department (if applicable)HistoryB3Is the module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SF4Is this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SF5Accrediting body (if applicable)N/AQ6Module title LM The Business of Heritage  B Q7Module code(s) (if known)38901B8Module levelMasters - LMB Q9Module credits 20B Q10Module attribute, if relevantn/aB11Semester in which the module will runSemester 1B12Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ515H LM International Heritage Management FTAs an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁNone☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/A14ÂN/AB15Where will the teaching take place? UoB Campus EdgbastonÄB Q SF16Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe school is committed to ensuring modules and programmes are inclusive and work closely with the University’s Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.Q 17ÅN/AQ18Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)B Q SF18.1Lecture1018.2È 1018.3É18.4ꮛ18.5ꮜ18.6ꮝ18.7ꮞ18.8ꮟ18.9ꮠ18.10ꮡ18.11ꮢ18018.12ꮣ19ꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students’ awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.Q20Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:20.1Demonstrate critical awareness of the need to manage heritage sites financially and administratively20.2 Demonstratean understanding of the nature and importance of marketing in the context of heritage sites20.3Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function20.4Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard21ꮨ(i.e. assessment that does not produce a mark that ꮩ 10 minute presentation: Online presentation to Course Convenor on proposed heritage project and outline of key topics of business plan. Feedback will be provided immediately after online presentation verbally to student.Q22Assessment category (multiple assessments should be included in the same category, e.g. a module with two written tasks and an oral presentation would be ‘coursework 100%’)ɸ 100% B ∏   23Ŋ and weighting, ꮫ1 x 3,000 word heritage project business plan  (100%)B Q23.1If there is an examination, is it centrally ꮭNoꮮ If ‘yes’ is this available for students to take overseas?N/AB23.2If there is an examination, ꮯ</v>
+        <v>Summer Exam Period</v>
       </c>
       <c r="AR3" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="AS3" t="str">
+        <v>Resubmission of above assignments&lt;br&gt;</v>
+      </c>
+      <c r="AT3" t="str">
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;2,000-word assignment&lt;br&gt;&lt;br&gt;50% weighting &lt;br&gt;50% Pass Mark &lt;br&gt;&lt;br&gt;1-hour face to face exam&lt;br&gt;50% weighting &lt;br&gt;50% Pass Mark&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of above assignments&lt;br&gt;</v>
+      </c>
+      <c r="AU3" t="str">
+        <v>Semester 2</v>
+      </c>
+      <c r="AV3" t="str">
+        <v>6</v>
+      </c>
+      <c r="AW3" t="str">
+        <v>Dr Ayat Abu-Agla</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>002025</v>
+      </c>
+      <c r="B4" t="str">
+        <v>08</v>
+      </c>
+      <c r="C4" t="str">
+        <v>School of Social Policy</v>
+      </c>
+      <c r="D4" t="str">
+        <v>035</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Health Services Management Centre</v>
+      </c>
+      <c r="F4" t="str">
+        <v>122</v>
+      </c>
+      <c r="G4" t="str">
+        <v>12</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Global Health System and Policy</v>
+      </c>
+      <c r="I4" t="str">
+        <v>LM Glob Heal Syste &amp; Polic Dub</v>
+      </c>
+      <c r="J4" t="str">
+        <v>LM Global Health System and Policy</v>
+      </c>
+      <c r="K4" t="str">
+        <v>TBC</v>
+      </c>
+      <c r="L4" t="str">
+        <v>LM</v>
+      </c>
+      <c r="M4" t="str">
+        <v>20</v>
+      </c>
+      <c r="N4" t="str">
+        <v>GT</v>
+      </c>
+      <c r="O4" t="str">
+        <v>Z</v>
+      </c>
+      <c r="P4" t="str">
+        <v>131</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>B900</v>
+      </c>
+      <c r="R4" t="str">
+        <v>100260</v>
+      </c>
+      <c r="S4" t="str">
+        <v>MSc Global Health System Leadership (Dubai campus)As an optional module (including any information about its grouping, if relevant):</v>
+      </c>
+      <c r="T4" t="str">
         <v/>
       </c>
-      <c r="AS3" t="str">
-        <v>["&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Modification&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;LM Heritage Management Practice&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;2024-25&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).&lt;br&gt;&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;No new resource requirements&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;No&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;As this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 07/08/2023&lt;br&gt;Approving body: SHAC PARC&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC via Chairs Action&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.&lt;br&gt; &lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;4&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;5&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;6&lt;br&gt;Module title &lt;br&gt;LM The Business of Heritage &lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Module code(s) (if known)&lt;br&gt;38901&lt;br&gt;B&lt;br&gt;8&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;9&lt;br&gt;Module credits &lt;br&gt;20&lt;br&gt;B Q&lt;br&gt;10&lt;br&gt;Module attribute, if relevant&lt;br&gt;n/a&lt;br&gt;B&lt;br&gt;11&lt;br&gt;Semester in which the module will run&lt;br&gt;Semester 1&lt;br&gt;&lt;br&gt;B&lt;br&gt;12&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e. every student in the year should be registered on this module code):&lt;br&gt;515H LM International Heritage Management FT&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant):&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;None&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;14&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;15&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Edgbaston&lt;br&gt;&lt;br&gt;If 'other' please state here:&lt;br&gt;B Q SF&lt;br&gt;16&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected group&lt;br&gt;The school is committed to ensuring modules and programmes are inclusive and work closely with the University's Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.&lt;br&gt;Q &lt;br&gt;17&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;18&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)&lt;br&gt;B Q SF&lt;br&gt;18.1&lt;br&gt;Lecture&lt;br&gt;10&lt;br&gt;&lt;br&gt;18.2&lt;br&gt;Seminar &lt;br&gt;10&lt;br&gt;&lt;br&gt;18.3&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;&lt;br&gt;18.4&lt;br&gt;Project supervision&lt;br&gt;&lt;br&gt;&lt;br&gt;18.5&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;&lt;br&gt;18.6&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;&lt;br&gt;18.7&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;&lt;br&gt;18.8&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;&lt;br&gt;18.9&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;&lt;br&gt;18.10&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;&lt;br&gt;18.11&lt;br&gt;Guided independent study&lt;br&gt;180&lt;br&gt;&lt;br&gt;18.12&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;&lt;br&gt;19&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students' awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.&lt;br&gt;Q&lt;br&gt;20&lt;br&gt;Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student's failure of the module. The QAA publish guidance related to 'levelness' in the Frameworks for Higher Education Qualifications and in their Subject Benchmark Statements. Schools/Institutes are also encouraged to refer to the Birmingham Graduate Attributes. &lt;br&gt;&lt;br&gt;ꮧ20.1&lt;br&gt;Demonstrate critical awareness of the need to manage heritage sites financially and administratively&lt;br&gt;20.2&lt;br&gt; Demonstratean understanding of the nature and importance of marketing in the context of heritage sites&lt;br&gt;20.3&lt;br&gt;Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function&lt;br&gt;20.4&lt;br&gt;Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard&lt;br&gt;21ꮨ(i.e. assessment that does not produce a mark that contributes to the overall module mark)&lt;br&gt; 10 minute presentation: Online presentation to Course Convenor on proposed heritage project and outline of key topics of business plan. Feedback will be provided immediately after online presentation verbally to student.&lt;br&gt;Q&lt;br&gt;22&lt;br&gt;Assessment category (multiple assessments should be included in the same category, e.g. a module with two written tasks and an oral presentation would be 'coursework 100%')&lt;br&gt;If the module is wholly or partly assessed by coursework, please state the overall weighting: &lt;br&gt;&lt;br&gt;100% &lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;&lt;br&gt;If the module is wholly or partly assessed by examination, please state the overall weighting: &lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;23&lt;br&gt;Additional information on the method(s) of summative assessment and weighting, ꮫ&lt;br&gt;1 x 3,000 word heritage project business plan (100%)&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;23.1&lt;br&gt;If there is an examination, is it centrally timetabled?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please specify the length of the examination: &lt;br&gt;&lt;br&gt;If 'yes' is this available for students to take overseas?&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;23.2&lt;br&gt;If there is an examination, select examination period&lt;br&gt;N/A - not examined&lt;br&gt;&lt;br&gt;B&lt;br&gt;&lt;br&gt;24&lt;br&gt;Please describe any internal hurdles&lt;br&gt;None&lt;br&gt;B Q&lt;br&gt;25&lt;br&gt;Method(s) of reassessment students would be expected to undertake should they fail to pass the module at the first attempt. The reassessment method(s) must enable students to ꮲ</v>
-      </c>
-      <c r="AT3" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;["&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Modification&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;LM Heritage Management Practice&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;2024-25&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;No new resource requirements&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;No&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;As this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 07/08/2023&lt;br&gt;Approving body: SHAC PARC&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC via Chairs Action&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.&lt;br&gt; &lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;4&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;5&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;6&lt;br&gt;Module title &lt;br&gt;LM The Business of Heritage &lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Module code(s) (if known)&lt;br&gt;38901&lt;br&gt;B&lt;br&gt;8&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;9&lt;br&gt;Module credits &lt;br&gt;20&lt;br&gt;B Q&lt;br&gt;10&lt;br&gt;Module attribute, if relevant&lt;br&gt;n/a&lt;br&gt;B&lt;br&gt;11&lt;br&gt;Semester in which the module will run&lt;br&gt;Semester 1&lt;br&gt;&lt;br&gt;B&lt;br&gt;12&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e. every student in the year should be registered on this module code):&lt;br&gt;515H LM International Heritage Management FT&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant):&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;None&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;14&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;15&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Edgbaston&lt;br&gt;&lt;br&gt;If 'other' please state here:&lt;br&gt;B Q SF&lt;br&gt;16&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected group&lt;br&gt;The school is committed to ensuring modules and programmes are inclusive and work closely with the University's Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.&lt;br&gt;Q &lt;br&gt;17&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;18&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)&lt;br&gt;B Q SF&lt;br&gt;18.1&lt;br&gt;Lecture&lt;br&gt;10&lt;br&gt;&lt;br&gt;18.2&lt;br&gt;Seminar &lt;br&gt;10&lt;br&gt;&lt;br&gt;18.3&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;18.4&lt;br&gt;Project supervision&lt;br&gt;&lt;br&gt;18.5&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;18.6&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;18.7&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;18.8&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;18.9&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;18.10&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;18.11&lt;br&gt;Guided independent study&lt;br&gt;180&lt;br&gt;&lt;br&gt;18.12&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;19&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students' awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.&lt;br&gt;Q&lt;br&gt;20&lt;br&gt;Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student's failure of the module. The QAA publish guidance related to 'levelness' in the Frameworks for Higher Education Qualifications and in their Subject Benchmark Statements. Schools/Institutes are also encouraged to refer to the Birmingham Graduate Attributes. &lt;br&gt;&lt;br&gt;ꮧ20.1&lt;br&gt;Demonstrate critical awareness of the need to manage heritage sites financially and administratively&lt;br&gt;20.2&lt;br&gt; Demonstratean understanding of the nature and importance of marketing in the context of heritage sites&lt;br&gt;20.3&lt;br&gt;Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function&lt;br&gt;20.4&lt;br&gt;Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard&lt;br&gt;21ꮨ(i.e. assessment that does not produce a mark that contributes to the overall module mark)&lt;br&gt; 10 minute presentation: Online presentation to Course Convenor on proposed heritage project and outline of key topics of business plan. Feedback will be provided immediately after online presentation verbally to student.&lt;br&gt;Q&lt;br&gt;22&lt;br&gt;Assessment category (multiple assessments should be included in the same category, e.g. a module with two written tasks and an oral presentation would be 'coursework 100%')&lt;br&gt;If the module is wholly or partly assessed by coursework, please state the overall weighting: &lt;br&gt;&lt;br&gt;100% &lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If the module is wholly or partly assessed by examination, please state the overall weighting: &lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;23&lt;br&gt;Additional information on the method(s) of summative assessment and weighting, ꮫ&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;["&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Modification&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;LM Heritage Management Practice&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;2024-25&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The change is to update the title to The Business of Heritage to more clearly reflect content of course and focus on course of teaching relatinged to heritage as business (including financial, HR, legal requirements, sustainability) , in line with student feedback. Also, to demonstrate significant difference from module titled Heritage Conservation Management (these two modules with similar titles have in past caused confusion).&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;No new resource requirements&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;No&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;As this is within CMA timeline guidelines, no consultation is necessary as this will not affect existing students and prospective students will have this information.&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint degree, major/minor degree, or discovery/interdisciplinary degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 07/08/2023&lt;br&gt;Approving body: SHAC PARC&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC via Chairs Action&lt;br&gt;&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.&lt;br&gt; &lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of History and Cultures&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;History&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;4&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;5&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;6&lt;br&gt;Module title &lt;br&gt;LM The Business of Heritage &lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Module code(s) (if known)&lt;br&gt;38901&lt;br&gt;B&lt;br&gt;8&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;9&lt;br&gt;Module credits &lt;br&gt;20&lt;br&gt;B Q&lt;br&gt;10&lt;br&gt;Module attribute, if relevant&lt;br&gt;n/a&lt;br&gt;B&lt;br&gt;11&lt;br&gt;Semester in which the module will run&lt;br&gt;Semester 1&lt;br&gt;&lt;br&gt;B&lt;br&gt;12&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e. every student in the year should be registered on this module code):&lt;br&gt;515H LM International Heritage Management FT&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant):&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;None&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;14&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;15&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Edgbaston&lt;br&gt;&lt;br&gt;If 'other' please state here:&lt;br&gt;B Q SF&lt;br&gt;16&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected group&lt;br&gt;The school is committed to ensuring modules and programmes are inclusive and work closely with the University's Equality and Diversity advisor in developing our practice in this area. In terms of content, mode of delivery and assessment this module poses no general or systematic barriers to access or progression for any student or protected group. In individual cases, in so far as it may become necessary, reasonable adjustments will be made for students with disabilities in accordance with their Reasonable Adjustments Plan.&lt;br&gt;Q &lt;br&gt;17&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;18&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;200 hours in total. 20 hours of taught content. Students are expected to put in an additional 18 hours per week of study/appropriate activity (site visits etc.)&lt;br&gt;B Q SF&lt;br&gt;18.1&lt;br&gt;Lecture&lt;br&gt;10&lt;br&gt;&lt;br&gt;18.2&lt;br&gt;Seminar &lt;br&gt;10&lt;br&gt;&lt;br&gt;18.3&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;18.4&lt;br&gt;Project supervision&lt;br&gt;&lt;br&gt;18.5&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;18.6&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;18.7&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;18.8&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;18.9&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;18.10&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;18.11&lt;br&gt;Guided independent study&lt;br&gt;180&lt;br&gt;&lt;br&gt;18.12&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;19&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥThis module seeks to explore the management skills necessary to deliver successful heritage management to the sector. It includes issues relating to marketing, budgeting and costings, project management, human resource activities and visitor management services. The module also seeks to develop students' awareness of the skills base necessary to curate museum collections, including the ability to draw together the required materials for an exhibition. The module is delivered by practitioners where possible to enable the relevant skills set from the profession to be passed onto the student cohort.&lt;br&gt;Q&lt;br&gt;20&lt;br&gt;Module outcomes: each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student's failure of the module. The QAA publish guidance related to 'levelness' in the Frameworks for Higher Education Qualifications and in their Subject Benchmark Statements. Schools/Institutes are also encouraged to refer to the Birmingham Graduate Attributes. &lt;br&gt;&lt;br&gt;ꮧ20.1&lt;br&gt;Demonstrate critical awareness of the need to manage heritage sites financially and administratively&lt;br&gt;20.2&lt;br&gt; Demonstratean understanding of the nature and importance of marketing in the context of heritage sites&lt;br&gt;20.3&lt;br&gt;Display critical awareness of the control of human resources in an effective manner to control heritage sites and allow them to function&lt;br&gt;20.4&lt;br&gt;Demonstrate awareness of the skills required to display and maintain collections to an appropriate curatorial standard&lt;br&gt;21ꮨ(i.e. assessment that does not produce a mark that contributes to the overall module mark)&lt;br&gt; 10 minute presentation: Online presentation to Course Convenor on proposed heritage project and outline of key topics of business plan. Feedback will be provided immediately after online presentation verbally to student.&lt;br&gt;Q&lt;br&gt;22&lt;br&gt;Assessment category (multiple assessments should be included in the same category, e.g. a module with two written tasks and an oral presentation would be 'coursework 100%')&lt;br&gt;If the module is wholly or partly assessed by coursework, please state the overall weighting: &lt;br&gt;&lt;br&gt;100% &lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If the module is wholly or partly assessed by examination, please state the overall weighting: &lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;23&lt;br&gt;Additional information on the method(s) of summative assessment and weighting, ꮫ&lt;br&gt;1 x 3,000 word heritage project business plan (100%)&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;23.1&lt;br&gt;If there is an examination, is it centrally timetabled?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' please specify the length of the examination: &lt;br&gt;&lt;br&gt;If 'yes' is this available for students to take overseas?&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;23.2&lt;br&gt;If there is an examination, select examination period&lt;br&gt;N/A - not examined&lt;br&gt;&lt;br&gt;B&lt;br&gt;&lt;br&gt;24&lt;br&gt;Please describe any internal hurdles&lt;br&gt;None&lt;br&gt;B Q&lt;br&gt;25&lt;br&gt;Method(s) of reassessment students would be expected to undertake should they fail to pass the module at the first attempt. The reassessment method(s) must enable students to ꮲ</v>
-      </c>
-      <c r="AU3" t="str">
+      <c r="U4" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="V4" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="W4" t="str">
+        <v>UoB Campus Dubai</v>
+      </c>
+      <c r="X4" t="str">
+        <v>U</v>
+      </c>
+      <c r="Y4" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="Z4">
+        <v>10</v>
+      </c>
+      <c r="AA4">
+        <v>10</v>
+      </c>
+      <c r="AB4">
+        <v>10</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>10</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>160</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4" t="str">
+        <v>Globally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region face many diverse conflict and instability and double burden of disease. &lt;br&gt;&lt;br&gt;This module provides a systematic understanding of the basic principles and theories of health systems and policy and enables students to critically analyse and evaluate health systems and policies using theoretical and comparative approaches across different complex, stable and fragile conflict-affected vulnerable settings (FCV), cultures and countries.&lt;br&gt;&lt;br&gt;The module enables students to develop and critique a health policy draft informed by evidence and tools towards the realisation of universal health coverage, the Sustainable Development Goals and Health for All.</v>
+      </c>
+      <c r="AM4" t="str">
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Demonstrate a systematic and critical understanding of frameworks for describing, analysing and understanding health systems and policies development and complexities in high, low and middle-income countries.&lt;/li&gt;&lt;li&gt;Demonstrate the ability to synthesise and critically analyse theory and evidence from a variety of sources on a range of aspects exploring power, agency, political economy, and mindsets of health system.&lt;/li&gt;&lt;li&gt;Analyse and evaluate health systems and policies across different complex, stable and fragile conflict-affected vulnerable settings (FCV), cultures and countries using theoretical and comparative approaches and tools to present a coherent critique.&lt;/li&gt;&lt;li&gt;Understand the challenges of managing health systems change and interventions and developing health policies.&lt;/li&gt;&lt;li&gt;Critically evaluate the impact of change in global health systems and policies towards the realisation of universal health coverage, the Sustainable Development Goals and Health for All.&lt;/li&gt;&lt;/ul&gt;</v>
+      </c>
+      <c r="AN4" t="str">
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Social Policy[Health Services Management Centre𓏉Global Health System and Policy`January 2025¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SF This module provides a systematic understanding of the basic principles and theories of health systems and policy and enable students to critically analyse and evaluate health systems and policies using theoretical and comparative approaches across different complex, stable and fragile conflict-affected vulnerable settings (FCV), cultures and countries.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Resource implications have been arranged across Edgbaston and Dubai campuses.SFAre there any related programme modifications? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?YesB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryN/AQIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 10/08/2023Approving body: SEQC (Chair’s action)College (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC (Chair’s action)Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Social Policy[Health Services Management Centre] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)N/AʓGlobal Health System and Policy#TBC=Masters - LM@20$, if relevantN/A⸮Semester 1ﱙAs a compulsory module (i.e. every student in the year should be ǕMSc Global Health System Leadership (Dubai campus)As an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁN/A☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/AÂN/AÃUoB Campus DubaiÄÄ on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThis programme has been designed to be fully inclusive.  As a University/Department we are committed to ensuring that all our modules/programmes are inclusive and that we comply fully with the Equality Act of 2010. There are no barriers to applications, access, or progression.  The department always considers whether any parts of module delivery might prove disadvantageous to any group.  Module materials are designed to be fully accessible and are made available in advance to students electronically and, where requested, hard copy form. Further adjustments are made where appropriate to support students with SSAs/RAPs.Q ÅN/AÆ effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç10È 10É10ꮛꮜꮝ10ꮞꮟꮠꮡꮢ160ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥGlobally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region face many diverse conflict and instability and double burden of disease. This module provides a systematic understanding of the basic principles and theories of health systems and policy and enables students to critically analyse and evaluate health systems and policies using theoretical and comparative approaches across different complex, stable and fragile conflict-affected vulnerable settings (FCV), cultures and countries.The module enables students to develop and critique a health policy draft informed by evidence and tools towards the realisation of universal health coverage, the Sustainable Development Goals and Health for All.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:Demonstrate a systematic and critical understanding of frameworks for describing, analysing and understanding health systems and policies development and complexities in high, low and middle-income countries.Demonstrate the ability to synthesise and critically analyse theory and evidence from a variety of sources on a range of aspects exploring power, agency, political economy, and mindsets of health system.Analyse and evaluate health systems and policies across different complex, stable and fragile conflict-affected vulnerable settings (FCV), cultures and countries using theoretical and comparative approaches and tools to present a coherent critique.Understand the challenges of managing health systems change and interventions and developing health policies.Critically evaluate the impact of change in global health systems and policies towards the realisation of universal health coverage, the Sustainable Development Goals and Health for All.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+      </c>
+      <c r="AO4" t="str">
+        <v>&lt;br&gt;One 2,500-word assignment (60%), and one in module 10 minute group-based presentation (40%). &lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="AP4" t="str">
+        <v>N/A - not examined</v>
+      </c>
+      <c r="AQ4" t="str">
+        <v>N/A - not examined</v>
+      </c>
+      <c r="AR4" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="AS4" t="str">
+        <v>Resubmission of failed component: 2500-word assignment (60%); Individual assignment 1000 words reflective piece. (40%).</v>
+      </c>
+      <c r="AT4" t="str">
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;One 2,500-word assignment (60%), and one in module 10 minute group-based presentation (40%). &lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of failed component: 2500-word assignment (60%); Individual assignment 1000 words reflective piece. (40%).</v>
+      </c>
+      <c r="AU4" t="str">
+        <v>Semester 1</v>
+      </c>
+      <c r="AV4" t="str">
+        <v>5</v>
+      </c>
+      <c r="AW4" t="str">
+        <v>Dr. Ayat Abu-Agla a.s.y.abu-agla@bham.ac.uk</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>002025</v>
+      </c>
+      <c r="B5" t="str">
+        <v>08</v>
+      </c>
+      <c r="C5" t="str">
+        <v>School of Social Policy</v>
+      </c>
+      <c r="D5" t="str">
+        <v>035</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Health Services Management Centre</v>
+      </c>
+      <c r="F5" t="str">
+        <v>122</v>
+      </c>
+      <c r="G5" t="str">
+        <v>12</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Implementation Science</v>
+      </c>
+      <c r="I5" t="str">
+        <v>LM Implementation Science Dub</v>
+      </c>
+      <c r="J5" t="str">
+        <v>LM Implementation Science</v>
+      </c>
+      <c r="K5" t="str">
+        <v>TBC</v>
+      </c>
+      <c r="L5" t="str">
+        <v>LM</v>
+      </c>
+      <c r="M5" t="str">
+        <v>20</v>
+      </c>
+      <c r="N5" t="str">
+        <v>GT</v>
+      </c>
+      <c r="O5" t="str">
+        <v>Z</v>
+      </c>
+      <c r="P5" t="str">
+        <v>131</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>B900</v>
+      </c>
+      <c r="R5" t="str">
+        <v>100260</v>
+      </c>
+      <c r="S5" t="str">
+        <v>MSc Global Health System Leadership (Dubai campus)PG Dip Global Health System Leadership (Dubai campus) (alternative qual)As an optional module (including any information about its grouping, if relevant):PG Cert Global Health System Leadership (Dubai campus) (alternative qual)</v>
+      </c>
+      <c r="T5" t="str">
         <v/>
       </c>
-      <c r="AV3" t="str">
+      <c r="U5" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="V5" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="W5" t="str">
+        <v>UoB Campus Dubai</v>
+      </c>
+      <c r="X5" t="str">
+        <v>U</v>
+      </c>
+      <c r="Y5" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="Z5">
+        <v>10</v>
+      </c>
+      <c r="AA5">
+        <v>10</v>
+      </c>
+      <c r="AB5">
+        <v>10</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>10</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>160</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5" t="str">
+        <v>Globally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region face many diverse conflict and instability and double burden of disease. &lt;br&gt;&lt;br&gt;The diversity of people and health situations requires, on the demand side, a solid understanding of the emerging socio-economic, epidemiologic and demographic patterns and trends at both aggregate as well as national and sub-national levels, with due sensitivity to disadvantaged populations and vulnerable segments of the society. On the supply side, it is equally crucial to have a solid understanding of the commonalities and divergences of the health systems, the circumstances and political economy under which they have evolved and operate and, more specifically, how these bear upon the way the health system stewardship function of health ministries is carried out. This module studies the systematic approach of the theory and practice of implementation science to recognise, understand and address health system and implementation bottlenecks, identifying, planning, managing, and evaluating optimal implementation options for a given setting to improve health system and examine long-term sustainability and resilience approaches to combat future shocks and establish the foundation for change, along the \"financing-governance-service delivery\" nexus. &lt;br&gt;&lt;br&gt;This module enables students to develop a health system strengthening intervention demonstrating implementation science skills applying a gender lens and one health approach promoting the uptake of research findings into policy and practice in the health system for health development to advance the UHC and SDG agenda. &lt;br&gt;&lt;br&gt;Topics include: Theory and practice of implementation Science, Implementation Science intervention: Research methods and data management, Planning and conducting implementation research, Communications and advocacy, Integrating implementation science into health systems, implementation science from an intersectional gender lens, implementation science and one-health approach.</v>
+      </c>
+      <c r="AM5" t="str">
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Demonstrate a systematic understanding of the theory and practice of implementation science. &lt;/li&gt;&lt;li&gt;Examine approaches to critically identify, assess, and evaluate health system bottlenecks and barriers to programme implementation. &lt;/li&gt;&lt;li&gt;Demonstrate the ability to design a health system strengthening intervention, monitoring and evaluation and communication and advocacy plan in order to promote uptake into health systems.&lt;/li&gt;&lt;li&gt;Critically analyse theory and concepts related to the study of implementation science from an inter-sectoral gender lens and apply these to develop a health system strengthening intervention. &lt;/li&gt;&lt;li&gt;Critically analyse theory and concepts related to the study of implementation science and one health approach and apply these to develop a health system strengthening intervention.&lt;/li&gt;&lt;/ul&gt;</v>
+      </c>
+      <c r="AN5" t="str">
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Social Policy[Health Services Management Centre𓏉Implementation Science`January 2025¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThis module studies the systematic approach of the theory and practice of implementation science to recognise, understand and address health system and implementation bottlenecks, identifying, planning, managing, and evaluating optimal implementation options for a given setting to improve health system and examine long-term sustainability and resilience approaches to combat future shocks and establish the foundation for change, along the “financing-governance-service delivery” nexus.  Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Resource implications have been arranged across Edgbaston and Dubai campuses.SFAre there any related programme modifications? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?YesB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryN/AQIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 10/08/2023Approving body: SEQC (Chair’s action)College (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC (Chair’s action)Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Social Policy[Health Services Management Centre] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)N/AʓImplementation Science#TBC=Masters - LM@20$, if relevantN/A⸮Semester 1ﱙAs a compulsory module (i.e. every student in the year should be ǕMSc Global Health System Leadership (Dubai campus)PG Dip Global Health System Leadership (Dubai campus) (alternative qual)As an optional module (including any information about its grouping, if relevant):PG Cert Global Health System Leadership (Dubai campus) (alternative qual)À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁN/A☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/AÂN/AÃUoB Campus DubaiÄÄ on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThis programme has been designed to be fully inclusive.  As a University/Department we are committed to ensuring that all our modules/programmes are inclusive and that we comply fully with the Equality Act of 2010. There are no barriers to applications, access, or progression.  The department always considers whether any parts of module delivery might prove disadvantageous to any group.  Module materials are designed to be fully accessible and are made available in advance to students electronically and, where requested, hard copy form. Further adjustments are made where appropriate to support students with SSAs/RAPs.Q ÅN/AÆ effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç10È 10É10ꮛꮜꮝ10ꮞꮟꮠꮡꮢ160ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥGlobally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region face many diverse conflict and instability and double burden of disease. The diversity of people and health situations requires, on the demand side, a solid understanding of the emerging socio-economic, epidemiologic and demographic patterns and trends at both aggregate as well as national and sub-national levels, with due sensitivity to disadvantaged populations and vulnerable segments of the society. On the supply side, it is equally crucial to have a solid understanding of the commonalities and divergences of the health systems, the circumstances and political economy under which they have evolved and operate and, more specifically, how these bear upon the way the health system stewardship function of health ministries is carried out. This module studies the systematic approach of the theory and practice of implementation science to recognise, understand and address health system and implementation bottlenecks, identifying, planning, managing, and evaluating optimal implementation options for a given setting to improve health system and examine long-term sustainability and resilience approaches to combat future shocks and establish the foundation for change, along the “financing-governance-service delivery” nexus.  This module enables students to develop a health system strengthening intervention demonstrating implementation science skills applying a gender lens and one health approach promoting the uptake of research findings into policy and practice in the health system for health development to advance the UHC and SDG agenda. Topics include: Theory and practice of implementation Science, Implementation Science intervention: Research methods and data management, Planning and conducting implementation research, Communications and advocacy, Integrating implementation science into health systems, implementation science from an intersectional gender lens, implementation science and one-health approach.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:Demonstrate a systematic understanding of the theory and practice of implementation science. Examine approaches to critically identify, assess, and evaluate health system bottlenecks and barriers to programme implementation.  Demonstrate the ability to design a health system strengthening intervention, monitoring and  evaluation and communication and advocacy plan in order to promote uptake into health systems.Critically analyse theory and concepts related to the study of implementation science from an inter-sectoral gender lens and apply these to develop a health system strengthening intervention. Critically analyse theory and concepts related to the study of implementation science and one health approach and apply these to develop a health system strengthening intervention.  ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+      </c>
+      <c r="AO5" t="str">
+        <v>&lt;br&gt;2,500-word assignment (60%)&lt;br&gt;&lt;br&gt;In module 10 minute group presentation (40%)&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="AP5" t="str">
+        <v>N/A - not examined</v>
+      </c>
+      <c r="AQ5" t="str">
+        <v>N/A - not examined</v>
+      </c>
+      <c r="AR5" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="AS5" t="str">
+        <v>Resubmission of failed component: 2,500-word assignment (60%); Individual assignment 1000 words reflective piece. (40%).</v>
+      </c>
+      <c r="AT5" t="str">
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;2,500-word assignment (60%)&lt;br&gt;&lt;br&gt;In module 10 minute group presentation (40%)&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of failed component: 2,500-word assignment (60%); Individual assignment 1000 words reflective piece. (40%).</v>
+      </c>
+      <c r="AU5" t="str">
+        <v>Semester 1</v>
+      </c>
+      <c r="AV5" t="str">
+        <v>5</v>
+      </c>
+      <c r="AW5" t="str">
+        <v>Dr. Ayat Abu Agla</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>002025</v>
+      </c>
+      <c r="B6" t="str">
+        <v>08</v>
+      </c>
+      <c r="C6" t="str">
+        <v>School of Social Policy</v>
+      </c>
+      <c r="D6" t="str">
+        <v>035</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Health Services Management Centre</v>
+      </c>
+      <c r="F6" t="str">
+        <v>122</v>
+      </c>
+      <c r="G6" t="str">
+        <v>12</v>
+      </c>
+      <c r="H6" t="str">
+        <v>Leadership and Management in Global Health</v>
+      </c>
+      <c r="I6" t="str">
+        <v>LM Leade &amp; Manage in Gl He Dub</v>
+      </c>
+      <c r="J6" t="str">
+        <v>LM Leadership and Management in Global Health</v>
+      </c>
+      <c r="K6" t="str">
+        <v>TBC</v>
+      </c>
+      <c r="L6" t="str">
+        <v>LM</v>
+      </c>
+      <c r="M6" t="str">
+        <v>20</v>
+      </c>
+      <c r="N6" t="str">
+        <v>GT</v>
+      </c>
+      <c r="O6" t="str">
+        <v>Z</v>
+      </c>
+      <c r="P6" t="str">
+        <v>131</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>B900</v>
+      </c>
+      <c r="R6" t="str">
+        <v>100260</v>
+      </c>
+      <c r="S6" t="str">
+        <v>MSc Global Health System Leadership (Dubai campus)As an optional module (including any information about its grouping, if relevant):</v>
+      </c>
+      <c r="T6" t="str">
         <v/>
       </c>
-      <c r="AW3" t="str">
-        <v>Dr Ioanna Katapidi</v>
+      <c r="U6" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="V6" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="W6" t="str">
+        <v>UoB Campus Dubai</v>
+      </c>
+      <c r="X6" t="str">
+        <v>U</v>
+      </c>
+      <c r="Y6" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="Z6">
+        <v>10</v>
+      </c>
+      <c r="AA6">
+        <v>10</v>
+      </c>
+      <c r="AB6">
+        <v>10</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>10</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>160</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6" t="str">
+        <v>Globally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region face many diverse conflict and instability and double burden of disease. &lt;br&gt;&lt;br&gt;This module examines issues relating to leadership and management in global health. It introduces theories, foundational concepts, and context in leadership and management of self, teams, and the organization including concepts of role, power, authority, change and resilience of leaders and managers to develop the knowledge and understanding needed to appraise and evaluate approaches within health systems, complex adaptive systems, and values-based leadership to combat future shocks and establish the foundation for change, along the \"financing-governance-service delivery\" nexus for health development to advance the UHC and SDG agenda. &lt;br&gt;&lt;br&gt;The module enables students to develop capabilities in health system leadership and management including skills and attributes needed to lead change including those related to power, ethics, decision-making, equality, diversity, and inclusion and work with multi-sectoral interdisciplinary teams, vulnerable groups. &lt;br&gt;&lt;br&gt;Topics include: Theories and models of leadership and management; concepts of role-power-authority and change; resilience of leaders and managers, complex adaptive systems, values-based leadership; Leadership and equality, diversity and inclusion; decision-making.</v>
+      </c>
+      <c r="AM6" t="str">
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Demonstrate an understanding of the evolution and range of theories and models in leadership and management.&lt;/li&gt;&lt;li&gt;Demonstrate an understanding of theories, foundational concepts for leaders and managers including those related to identity of role, power, authority, change, resilience and decision-making.&lt;/li&gt;&lt;li&gt;Demonstrate attributes and skills needed to critically appraise and evaluate approaches within health systems, complex adaptive systems, and values-based leadership and their implications for health and health care and apply these to different social and economic contexts.&lt;/li&gt;&lt;li&gt;Demonstrate capabilities in health system leadership and management including skills and attributes needed to lead change including those related to equality, diversity, and inclusion.&lt;/li&gt;&lt;li&gt;Examine approaches to work with multi-sectoral interdisciplinary teams, vulnerable groups.&lt;/li&gt;&lt;/ul&gt;</v>
+      </c>
+      <c r="AN6" t="str">
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Social Policy[Health Services Management Centre𓏉Leadership and Management in Global Health`January 2025¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFTo meet the pressing challenges facing global health systems, a range of calls have been made for improvements in leadership and management to advance the Universal Health Coverage (UHC) and Sustainable Development Goal (SGD) agendas.The module enables students to develop capabilities in health system leadership and management including skills and attributes needed to lead change including those related to equality, diversity, and inclusion and work with multi-sectoral interdisciplinary teams, vulnerable groups, power, and ethics and decision-making for health development to advance the UHC and SDG agenda.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Resource implications have been arranged across Edgbaston and Dubai campuses.SFAre there any related programme modifications? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?YesB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryN/AQIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 10/08/2023Approving body: SEQC (Chair’s action)College (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC (Chair’s action)Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Social Policy[Health Services Management Centre] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)N/AʓLeadership and Management in Global Health#TBC=Masters - LM@20$, if relevantN/A⸮Semester 1ﱙAs a compulsory module (i.e. every student in the year should be ǕMSc Global Health System Leadership (Dubai campus)As an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁN/A☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/AÂN/AÃUoB Campus DubaiÄÄ on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThis programme has been designed to be fully inclusive.  As a University/Department we are committed to ensuring that all our modules/programmes are inclusive and that we comply fully with the Equality Act of 2010. There are no barriers to applications, access, or progression.  The department always considers whether any parts of module delivery might prove disadvantageous to any group.  Module materials are designed to be fully accessible and are made available in advance to students electronically and, where requested, hard copy form. Further adjustments are made where appropriate to support students with SSAs/RAPs.Q ÅN/AÆ effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç10È 10É10ꮛꮜꮝ10ꮞꮟꮠꮡꮢ160ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥGlobally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region face many diverse conflict and instability and double burden of disease. This module examines issues relating to leadership and management in global health. It introduces theories, foundational concepts, and context in leadership and management of self, teams, and the organization including concepts of role, power, authority, change and resilience of leaders and managers to develop the knowledge and understanding needed to appraise and evaluate approaches within health systems, complex adaptive systems, and values-based leadership to combat future shocks and establish the foundation for change, along the “financing-governance-service delivery” nexus for health development to advance the UHC and SDG agenda.  The module enables students to develop capabilities in health system leadership and management including skills and attributes needed to lead change including those related to power, ethics, decision-making, equality, diversity, and inclusion and work with multi-sectoral interdisciplinary teams, vulnerable groups. Topics include: Theories and models of leadership and management; concepts of role-power-authority and change; resilience of leaders and managers, complex adaptive systems, values-based leadership; Leadership and equality, diversity and inclusion; decision-making.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:Demonstrate an understanding of the evolution and range of theories and models in leadership and management.Demonstrate an understanding of theories, foundational concepts for leaders and managers including those related to identity of role, power, authority, change, resilience and decision-making.Demonstrate attributes and skills needed to critically appraise and evaluate approaches within health systems, complex adaptive systems, and values-based leadership and their implications for health and health care and apply these to different social and economic contexts.Demonstrate capabilities in health system leadership and management including skills and attributes needed to lead change including those related to equality, diversity, and inclusion.Examine approaches to work with multi-sectoral interdisciplinary teams, vulnerable groups.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+      </c>
+      <c r="AO6" t="str">
+        <v>&lt;br&gt;2,500-word assignment (60%) &lt;br&gt;&lt;br&gt;In module 10 minute group-based presentation reflecting on a system leadership and management challenge (40%)&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="AP6" t="str">
+        <v>N/A - not examined</v>
+      </c>
+      <c r="AQ6" t="str">
+        <v>N/A - not examined</v>
+      </c>
+      <c r="AR6" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="AS6" t="str">
+        <v>&lt;br&gt;Resubmission of failed component: 2500-word assignment (60%); Individual assignment 1000 words reflective piece. (40%).</v>
+      </c>
+      <c r="AT6" t="str">
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;2,500-word assignment (60%) &lt;br&gt;&lt;br&gt;In module 10 minute group-based presentation reflecting on a system leadership and management challenge (40%)&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of failed component: 2500-word assignment (60%); Individual assignment 1000 words reflective piece. (40%).</v>
+      </c>
+      <c r="AU6" t="str">
+        <v>Semester 1</v>
+      </c>
+      <c r="AV6" t="str">
+        <v>5</v>
+      </c>
+      <c r="AW6" t="str">
+        <v>Dr. Ayat Abu-Agla</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>002025</v>
+      </c>
+      <c r="B7" t="str">
+        <v>08</v>
+      </c>
+      <c r="C7" t="str">
+        <v>School of Social Policy</v>
+      </c>
+      <c r="D7" t="str">
+        <v>035</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Health Services Management Centre</v>
+      </c>
+      <c r="F7" t="str">
+        <v>122</v>
+      </c>
+      <c r="G7" t="str">
+        <v>12</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Research Dissertation</v>
+      </c>
+      <c r="I7" t="str">
+        <v>LM Research Dissertation Dub</v>
+      </c>
+      <c r="J7" t="str">
+        <v>LM Research Dissertation</v>
+      </c>
+      <c r="K7" t="str">
+        <v>Dubai - TBC</v>
+      </c>
+      <c r="L7" t="str">
+        <v>LM</v>
+      </c>
+      <c r="M7" t="str">
+        <v>60</v>
+      </c>
+      <c r="N7" t="str">
+        <v>GT</v>
+      </c>
+      <c r="O7" t="str">
+        <v>Z</v>
+      </c>
+      <c r="P7" t="str">
+        <v>131</v>
+      </c>
+      <c r="Q7" t="str">
+        <v>B900</v>
+      </c>
+      <c r="R7" t="str">
+        <v>100260</v>
+      </c>
+      <c r="S7" t="str">
+        <v>MSc Global Health System LeadershipAs an optional module (including any information about its grouping, if relevant): N/A</v>
+      </c>
+      <c r="T7" t="str">
+        <v/>
+      </c>
+      <c r="U7" t="str">
+        <v>Students must have taken pre-requisite module Implementation Science in same or previous academic year</v>
+      </c>
+      <c r="V7" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="W7" t="str">
+        <v>UoB Campus Dubai</v>
+      </c>
+      <c r="X7" t="str">
+        <v>U</v>
+      </c>
+      <c r="Y7" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="Z7">
+        <v>6</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>10</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>584</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7" t="str">
+        <v>The Research Dissertation will demonstrate students' consolidation and application of global health&lt;br&gt;system leadership knowledge and skills by undertaking a research task relevant to the students' &lt;br&gt;current area of practice. It will build upon the proposal submitted for Implementation Science &lt;br&gt;(pre-requisite).&lt;br&gt;Students will undertake a research investigation under the guidance of a supervisor after determining&lt;br&gt;an appropriate methodology for the inquiry task, and subject to module lead approval.&lt;br&gt;&lt;br&gt;The investigation could take the form of a systematic review or thematic synthesis or project involving&lt;br&gt;fieldwork (subject to appropriate ethical and/or governance requirements). &lt;br&gt;&lt;br&gt;Outcomes of the study will be contextualised in terms of health system significance and potential for &lt;br&gt;transformation of services, or care delivery, or improving patient care or healthcare professional &lt;br&gt;education, leadership, or policy and promoting the uptake of research findings into policy and practice&lt;br&gt; in the health system.&lt;br&gt;</v>
+      </c>
+      <c r="AM7" t="str">
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Plan an inquiry relevant to their clinical area, research unit or educational institution pertaining to health and social care.&lt;/li&gt;&lt;li&gt;Review and critically analyse literature and current policy in this area to determine / refine and inform the focus and nature of the investigation.&lt;/li&gt;&lt;li&gt;Determine appropriate methods of investigation for the research task; providing rationale for the study, justifying the relevance to their field of practice, and recognising its limitations.&lt;/li&gt;&lt;li&gt;Collect or review and critically analyse data or information/data relevant to the subject.&lt;/li&gt;&lt;li&gt;Interpret the data collected and explain the significance, relevance, and implications for health system, health policy, service transformation for patient, population or professional, service delivery benefit.&lt;/li&gt;&lt;/ul&gt;</v>
+      </c>
+      <c r="AN7" t="str">
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Social Policy[Health Services Management Centre𓏉Research Dissertation`January 2025¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFThe Research Dissertation will demonstrate students’ consolidation and application of global health system leadership knowledge and skills by undertaking a research task relevant to the students’ current area of practice. It will build upon the proposal submitted for Implementation Science (pre-requisite). Students will undertake a research investigation under the guidance of a supervisor after determining an appropriate methodology for the inquiry task, and subject to module lead approval.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Resource implications have been arranged across Edgbaston and Dubai campuses.SFAre there any related programme modifications? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?YesB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryN/AQIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 10/08/2023Approving body: SEQC (Chair’s action)College (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC (Chair’s action)Module SpecificationThis form should be completed to accompany a module proposal form or revised to accompany a module modification form by using tracked changes.{School of Social Policy [Health Services Management Centre] module delivered in collaboration with another organisation? NoIf ‘yes’, please state the organisation’s name:B Q SFIs this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g., Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)N/AʓResearch Dissertation#Dubai - TBC=Masters - LM@60 credits$, if relevantN/A⸮Full TermﱙAs a compulsory module (i.e., every student in the year should be ǕMSc Global Health System LeadershipAs an optional module (including any information about its grouping, if relevant): N/AÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e., modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁStudents must have taken pre-requisite module Implementation Science in same or previous academic year☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/AÂN/AÃUoB Campus DubaiÄ The module will also be utilised as part of the MSc Global Health System Leadership in the Dubai CampusÄ on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access, or progression for any protected groupMSc Global Health System Leadership students will be allocated a Personal Academic tutor throughout the course and will have contact details for the Programme Director and administrative team. Students undertaking this module will be allocated a dissertation supervisor to support their individualised development during the module. Students will be provided with information, via canvas, regarding student services and the contact details for the allocated well-being advisors.  The well-being advisor will liaise with the School Welfare Officer to ensure that any additional support needs required are facilitated.  In addition to the services provided locally within the College of Social Sciences, when appropriate students will be signposted to other support services provided by the university.Working with the library and academic skills staff specific sessions aimed at supporting student learning will be incorporated as part of the module content.  The use of a range of learning and teaching strategies will ensure that a diverse range of learning styles are accommodated. The module does not pose any known barriers to access or progression for any protected group.Q ÅN/AÆ effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 600B Q Ç6 hoursÈ ÉꮛUp to 10 hours group or individual tutorial supportꮜꮝꮞꮟꮠꮡꮢ584 hoursꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g., is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThe Research Dissertation will demonstrate students’ consolidation and application of global healthsystem leadership knowledge and skills by undertaking a research task relevant to the students’ current area of practice. It will build upon the proposal submitted for Implementation Science (pre-requisite).Students will undertake a research investigation under the guidance of a supervisor after determiningan appropriate methodology for the inquiry task, and subject to module lead approval.The investigation could take the form of a systematic review or thematic synthesis or project involvingfieldwork (subject to appropriate ethical and/or governance requirements). Outcomes of the study will be contextualised in terms of health system significance and potential for transformation of services, or care delivery, or improving patient care or healthcare professional  education, leadership, or policy and promoting the uptake of research findings into policy and practice in the health system.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:Plan an inquiry relevant to their clinical area, research unit or educational institution pertaining to health and social care.Review and critically analyse literature and current policy in this area to determine / refine and inform the focus and nature of the investigation.Determine appropriate methods of investigation for the research task; providing rationale for the study, justifying the relevance to their field of practice, and recognising its limitations.Collect or review and critically analyse data or information/data relevant to the subject.Interpret the data collected and explain the significance, relevance, and implications for health system, health policy, service transformation for patient, population or professional, service delivery benefit. ꮨ(i.e., assessment that does not produce a mark that ꮩ</v>
+      </c>
+      <c r="AO7" t="str">
+        <v>["&lt;br&gt;&lt;br&gt; Significant module modifications can include any change resulting in the generation of a new module code (changes in title, level, or credits).&lt;br&gt; Consideration should be given to whether the proposed proposal/modification will impact on existing and/or prospective students. If so, they may need to be consulted. Please consult the guidance on making changes to programmes following the intervention of the Competition and Markets Authority and the Policy on Consultation with Students (PDF - 123KB) for more details. Additionally, it is good practice to seek students' views on changes to provision.&lt;br&gt; If the modification relates to all instances of a module, please include all locations and all semesters affected in sections 11 and 15 respectively.&lt;br&gt; Module attributes are relevant where it is useful to put modules into categories, e.g. putting modules into subject-based categories on a specialist programme, to indicate which modules can contribute to any specialist minors if not already obvious from the programme requirements; or putting modules into a themed category, such as 'Languages for All modules'. Otherwise please leave this section blank.&lt;br&gt; E.g. if the module is part of a particular subject theme or list of optional modules.&lt;br&gt; College of Arts and Law: 10 for all modules; College of Engineering and Physical Sciences: 10 for undergraduate modules, 5 for postgraduate modules; College of Life and Environmental Sciences: 10 for all modules; College of Medical and Dental Sciences: 10 for all modules; College of Social Sciences: 15 for all modules.&lt;br&gt; As a University we are committed to ensuring that our programmes and modules are inclusive of all students including international, part-time, mature, those from different socio-economic backgrounds and those with protected characteristics according to the Equality Act 2010. All programmes and modules should therefore seek to promote equality of opportunity through ensuring they pose no barriers to applications, access or progression for any student who meets the admissions criteria. Further guidance can be obtained from Student Services.&lt;br&gt; 'Coursework' includes written tasks, practical's, digital assets, oral presentations, portfolios, and locally scheduled in-course tests.&lt;br&gt; 'Examinations' are normally scheduled in the designated exam periods and include on-campus 'closed' and 'open book' exams, take-home exams, and online timed exams.&lt;br&gt; 5.5.3 of the Code of Practice on Taught Programme and Module Assessment and Feedback (PDF - 482KB) states that 'Where there is more than one assessment contributing to the module mark, principal academic units may specify that particular assessments must be passed in order to pass the module (known as 'internal hurdles'). The weighting of each assessment, or the requirement to pass a particular assessment, must be clearly stated as a percentage of the module mark in the approved module descriptions. &lt;br&gt;&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Proposal&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of Social Policy&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;Health Services Management Centre&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;Research Dissertation&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;January 2025&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The Research Dissertation will demonstrate students' consolidation and application of global health system leadership knowledge and skills by undertaking a research task relevant to the students' current area of practice. It will build upon the proposal submitted for Implementation Science (pre-requisite). Students will undertake a research investigation under the guidance of a supervisor after determining an appropriate methodology for the inquiry task, and subject to module lead approval.&lt;br&gt;&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;Resource implications have been arranged across Edgbaston and Dubai campuses.&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;Yes&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;Yes&lt;br&gt;&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;Please describe how, when, and with whom consultations occurred, and the outcomes&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 10/08/2023&lt;br&gt;Approving body: SEQC (Chair's action)&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC (Chair's action)&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form or revised to accompany a module modification form by using tracked changes.&lt;br&gt;&lt;br&gt;School/Institute that owns the module&lt;br&gt; School of Social Policy &lt;br&gt;&lt;br&gt;B&lt;br&gt;&lt;br&gt;Department (if applicable)&lt;br&gt;Health Services Management Centre&lt;br&gt;B&lt;br&gt;&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes', please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g., Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Module title &lt;br&gt;Research Dissertation&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;Module code(s) (if known)&lt;br&gt;Dubai - TBC&lt;br&gt;B&lt;br&gt;&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;Module credits &lt;br&gt;60 credits&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;Module attribute, if relevant&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;&lt;br&gt;Semester in which the module will run&lt;br&gt;Full Term&lt;br&gt;&lt;br&gt;&lt;br&gt;B&lt;br&gt;&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e., every student in the year should be registered on this module code):&lt;br&gt;&lt;br&gt;MSc Global Health System Leadership&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant): N/A&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e., modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;Students must have taken pre-requisite module Implementation Science in same or previous academic year&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Dubai&lt;br&gt;&lt;br&gt;If 'other' please state here: &lt;br&gt;&lt;br&gt;The module will also be utilised as part of the MSc Global Health System Leadership in the Dubai Campus&lt;br&gt;B Q SF&lt;br&gt;&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access, or progression for any protected group&lt;br&gt;MSc Global Health System Leadership students will be allocated a Personal Academic tutor throughout the course and will have contact details for the Programme Director and administrative team. &lt;br&gt;&lt;br&gt;Students undertaking this module will be allocated a dissertation supervisor to support their individualised development during the module. &lt;br&gt;&lt;br&gt;Students will be provided with information, via canvas, regarding student services and the contact details for the allocated well-being advisors. The well-being advisor will liaise with the School Welfare Officer to ensure that any additional support needs required are facilitated. In addition to the services provided locally within the College of Social Sciences, when appropriate students will be signposted to other support services provided by the university.&lt;br&gt;Working with the library and academic skills staff specific sessions aimed at supporting student learning will be incorporated as part of the module content. The use of a range of learning and teaching strategies will ensure that a diverse range of learning styles are accommodated. &lt;br&gt;&lt;br&gt;The module does not pose any known barriers to access or progression for any protected group.&lt;br&gt;Q &lt;br&gt;&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;600&lt;br&gt;B Q SF&lt;br&gt;&lt;br&gt;Lecture&lt;br&gt;6 hours&lt;br&gt;&lt;br&gt;&lt;br&gt;Seminar &lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Project supervision&lt;br&gt;Up to 10 hours group or individual tutorial support&lt;br&gt;&lt;br&gt;&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Guided independent study&lt;br&gt;584 hours&lt;br&gt;&lt;br&gt;&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g., is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥThe Research Dissertation will demonstrate students' consolidation and application of global health&lt;br&gt;system leadership knowledge and skills by undertaking a research task relevant to the students' &lt;br&gt;current area of practice. It will build upon the proposal submitted for Implementation Science &lt;br&gt;(pre-requisite).&lt;br&gt;Students will undertake a research investigation under the guidance of a supervisor after determining&lt;br&gt;an appropriate methodology for the inquiry task, and subject to module lead approval.&lt;br&gt;&lt;br&gt;The investigation could take the form of a systematic review or thematic synthesis or project involving&lt;br&gt;fieldwork (subject to appropriate ethical and/or governance requirements). &lt;br&gt;&lt;br&gt;Outcomes of the study will be contextualised in terms of health system significance and potential for &lt;br&gt;transformation of services, or care delivery, or improving patient care or healthcare professional &lt;br&gt;education, leadership, or policy and promoting the uptake of research findings into policy and practice&lt;br&gt; in the health system.&lt;br&gt;ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student's failure of the module. The QAA publish guidance related to 'levelness' in the Frameworks for Higher Education Qualifications and in their Subject Benchmark Statements. Schools/Institutes are also encouraged to refer to the Birmingham Graduate Attributes. &lt;br&gt;&lt;br&gt;ꮧPlan an inquiry relevant to their clinical area, research unit or educational institution pertaining to health and social care.&lt;br&gt;&lt;br&gt;Review and critically analyse literature and current policy in this area to determine / refine and inform the focus and nature of the investigation.&lt;br&gt;&lt;br&gt;Determine appropriate methods of investigation for the research task; providing rationale for the study, justifying the relevance to their field of practice, and recognising its limitations.&lt;br&gt;&lt;br&gt;Collect or review and critically analyse data or information/data relevant to the subject.&lt;br&gt;&lt;br&gt;Interpret the data collected and explain the significance, relevance, and implications for health system, health policy, service transformation for patient, population or professional, service delivery benefit. ꮨ(i.e., assessment that does not produce a mark that contributes to the overall module mark)&lt;br&gt;Students will submit a research dissertation proposal (building on feedback from Implementation Science) of up to 1000 words. Students will receive feedback on this proposal.&lt;br&gt;Students may present a first draft of their dissertation or part of, to their supervisor for feedback at least 3 weeks prior to submitting the final research dissertation. &lt;br&gt;Q&lt;br&gt;&lt;br&gt;Assessment category (multiple assessments should be included in the same category, e.g., a module with two written tasks and an oral presentation would be 'coursework 100%')&lt;br&gt;If the module is wholly or partly assessed by coursework, please state the overall weighting: 100%&lt;br&gt;&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;&lt;br&gt;If the module is wholly or partly assessed by examination, please state the overall weighting: N/A&lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;&lt;br&gt;Additional information on the method(s) of summative assessment and weighting, e.g., 1hr written unseen examination (50%), 500-word essay (10%), group presentation (40%), if required&lt;br&gt;2000-word research proposal assessment of methods to inform dissertation (15%)&lt;br&gt;&lt;br&gt;&lt;br&gt;Final Global Health System Leadership research dissertation: &lt;br&gt;Word count: 13,000 words. (85%)&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="AP7" t="str">
+        <v>N/A - not examinedIf ‘yes’, please specify the length of the examination:</v>
+      </c>
+      <c r="AQ7" t="str">
+        <v>N/A - not examined</v>
+      </c>
+      <c r="AR7" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="AS7" t="str">
+        <v>Reassessment: &lt;br&gt;Failure to achieve an overall average of at least 50% will require the student to improve and resubmit the work. &lt;br&gt;&lt;br&gt;Dissertation supervisor support will be offered to support the resubmission attempt.&lt;br&gt;</v>
+      </c>
+      <c r="AT7" t="str">
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;["&lt;br&gt;&lt;br&gt; Significant module modifications can include any change resulting in the generation of a new module code (changes in title, level, or credits).&lt;br&gt; Consideration should be given to whether the proposed proposal/modification will impact on existing and/or prospective students. If so, they may need to be consulted. Please consult the guidance on making changes to programmes following the intervention of the Competition and Markets Authority and the Policy on Consultation with Students (PDF - 123KB) for more details. Additionally, it is good practice to seek students' views on changes to provision.&lt;br&gt; If the modification relates to all instances of a module, please include all locations and all semesters affected in sections 11 and 15 respectively.&lt;br&gt; Module attributes are relevant where it is useful to put modules into categories, e.g. putting modules into subject-based categories on a specialist programme, to indicate which modules can contribute to any specialist minors if not already obvious from the programme requirements; or putting modules into a themed category, such as 'Languages for All modules'. Otherwise please leave this section blank.&lt;br&gt; E.g. if the module is part of a particular subject theme or list of optional modules.&lt;br&gt; College of Arts and Law: 10 for all modules; College of Engineering and Physical Sciences: 10 for undergraduate modules, 5 for postgraduate modules; College of Life and Environmental Sciences: 10 for all modules; College of Medical and Dental Sciences: 10 for all modules; College of Social Sciences: 15 for all modules.&lt;br&gt; As a University we are committed to ensuring that our programmes and modules are inclusive of all students including international, part-time, mature, those from different socio-economic backgrounds and those with protected characteristics according to the Equality Act 2010. All programmes and modules should therefore seek to promote equality of opportunity through ensuring they pose no barriers to applications, access or progression for any student who meets the admissions criteria. Further guidance can be obtained from Student Services.&lt;br&gt; 'Coursework' includes written tasks, practical's, digital assets, oral presentations, portfolios, and locally scheduled in-course tests.&lt;br&gt; 'Examinations' are normally scheduled in the designated exam periods and include on-campus 'closed' and 'open book' exams, take-home exams, and online timed exams.&lt;br&gt; 5.5.3 of the Code of Practice on Taught Programme and Module Assessment and Feedback (PDF - 482KB) states that 'Where there is more than one assessment contributing to the module mark, principal academic units may specify that particular assessments must be passed in order to pass the module (known as 'internal hurdles'). The weighting of each assessment, or the requirement to pass a particular assessment, must be clearly stated as a percentage of the module mark in the approved module descriptions. &lt;br&gt;&lt;br&gt;Form for Proposing or Modifying Modules&lt;br&gt;Module proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.&lt;br&gt;The final column in the below forms indicates why the different items of information are required, using the following codes:&lt;br&gt;B: Basic data used for information and programme modelling.&lt;br&gt;Q: Quality assurance processes and considerations.&lt;br&gt;SF: Alignment with the University's strategic aims and/or the financial risk:reward of the development.&lt;br&gt;&lt;br&gt;Is this a module proposal or modification?&lt;br&gt;Module Proposal&lt;br&gt;&lt;br&gt;If 'proposal', please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running&lt;br&gt;B&lt;br&gt;1&lt;br&gt;School/Institute that owns the module&lt;br&gt;School of Social Policy&lt;br&gt;&lt;br&gt;B&lt;br&gt;2&lt;br&gt;Department (if applicable)&lt;br&gt;Health Services Management Centre&lt;br&gt;B&lt;br&gt;3&lt;br&gt;Module title&lt;br&gt;Research Dissertation&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Date of implementation (in terms of academic sessions)&lt;br&gt;January 2025&lt;br&gt;B&lt;br&gt;&lt;br&gt;Rationale&lt;br&gt;&lt;br&gt;Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module. &lt;br&gt;SF&lt;br&gt;&lt;br&gt;The Research Dissertation will demonstrate students' consolidation and application of global health system leadership knowledge and skills by undertaking a research task relevant to the students' current area of practice. It will build upon the proposal submitted for Implementation Science (pre-requisite). Students will undertake a research investigation under the guidance of a supervisor after determining an appropriate methodology for the inquiry task, and subject to module lead approval.&lt;br&gt;&lt;br&gt;Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)&lt;br&gt;Resource implications have been arranged across Edgbaston and Dubai campuses.&lt;br&gt;SF&lt;br&gt;&lt;br&gt;Are there any related programme modifications? (for proposals and significant module modifications)&lt;br&gt;Yes&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If yes, have they been submitted for approval alongside this proposal?&lt;br&gt;Yes&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;7&lt;br&gt;Consultation (required for modifications, advised for proposals, where applicable)&lt;br&gt;Please describe how, when, and with whom consultations occurred, and the outcomes&lt;br&gt;&lt;br&gt;Prospective/existing students where necessary&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module/programme is subject to accreditation, please provide details of consultation with the professional body &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;If the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision &lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;8&lt;br&gt;Approval&lt;br&gt;&lt;br&gt;School/Institute&lt;br&gt;Date: 10/08/2023&lt;br&gt;Approving body: SEQC (Chair's action)&lt;br&gt;&lt;br&gt;College (mandatory for proposals only)&lt;br&gt;Date: 24/08/2023&lt;br&gt;Approving body: CQAAC (Chair's action)&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Module Specification&lt;br&gt;&lt;br&gt;This form should be completed to accompany a module proposal form or revised to accompany a module modification form by using tracked changes.&lt;br&gt;&lt;br&gt;School/Institute that owns the module&lt;br&gt; School of Social Policy &lt;br&gt;&lt;br&gt;B&lt;br&gt;&lt;br&gt;Department (if applicable)&lt;br&gt;Health Services Management Centre&lt;br&gt;B&lt;br&gt;&lt;br&gt;Is the module delivered in collaboration with another organisation? &lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes', please state the organisation's name:&lt;br&gt;B Q SF&lt;br&gt;&lt;br&gt;Is this module to be delivered by more than one School/Institute at UoB?&lt;br&gt;No&lt;br&gt;&lt;br&gt;If 'yes' state which Schools/Institutes they are and what the split will be, e.g., Mathematics 50%, Chemistry 50%:&lt;br&gt;B SF&lt;br&gt;&lt;br&gt;Accrediting body (if applicable)&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Module title &lt;br&gt;Research Dissertation&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;Module code(s) (if known)&lt;br&gt;Dubai - TBC&lt;br&gt;B&lt;br&gt;&lt;br&gt;Module level&lt;br&gt;Masters - LM&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;Module credits &lt;br&gt;60 credits&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;Module attribute, if relevant&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;&lt;br&gt;Semester in which the module will run&lt;br&gt;Full Term&lt;br&gt;&lt;br&gt;B&lt;br&gt;&lt;br&gt;Programmes on which the module is available (please state the programme title and code)&lt;br&gt;As a compulsory module (i.e., every student in the year should be registered on this module code):&lt;br&gt;&lt;br&gt;MSc Global Health System Leadership&lt;br&gt;&lt;br&gt;As an optional module (including any information about its grouping, if relevant): N/A&lt;br&gt;&lt;br&gt;Confirmation that module registrations (or numbers attending teaching events for this module) are expected to meet or exceed the relevant College's agreed threshold:&lt;br&gt;Yes&lt;br&gt;B&lt;br&gt;13.1&lt;br&gt;State the name and code of any pre-requisite modules, i.e., modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, as well as attempted&lt;br&gt;Students must have taken pre-requisite module Implementation Science in same or previous academic year&lt;br&gt;B&lt;br&gt;13.2&lt;br&gt;State if there is any other/prior knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicable&lt;br&gt;N/A&lt;br&gt;&lt;br&gt;State the name and code of any co-requisite modules on which students must also register in the same session&lt;br&gt;N/A&lt;br&gt;B&lt;br&gt;&lt;br&gt;Where will the teaching take place?&lt;br&gt; UoB Campus Dubai&lt;br&gt;&lt;br&gt;If 'other' please state here: &lt;br&gt;&lt;br&gt;The module will also be utilised as part of the MSc Global Health System Leadership in the Dubai Campus&lt;br&gt;B Q SF&lt;br&gt;&lt;br&gt;Comment briefly on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access, or progression for any protected group&lt;br&gt;MSc Global Health System Leadership students will be allocated a Personal Academic tutor throughout the course and will have contact details for the Programme Director and administrative team. &lt;br&gt;&lt;br&gt;Students undertaking this module will be allocated a dissertation supervisor to support their individualised development during the module. &lt;br&gt;&lt;br&gt;Students will be provided with information, via canvas, regarding student services and the contact details for the allocated well-being advisors. The well-being advisor will liaise with the School Welfare Officer to ensure that any additional support needs required are facilitated. In addition to the services provided locally within the College of Social Sciences, when appropriate students will be signposted to other support services provided by the university.&lt;br&gt;Working with the library and academic skills staff specific sessions aimed at supporting student learning will be incorporated as part of the module content. The use of a range of learning and teaching strategies will ensure that a diverse range of learning styles are accommodated. &lt;br&gt;&lt;br&gt;The module does not pose any known barriers to access or progression for any protected group.&lt;br&gt;Q &lt;br&gt;&lt;br&gt;Please detail any exemptions from Regulations&lt;br&gt;N/A&lt;br&gt;Q&lt;br&gt;&lt;br&gt;Total student effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to 'guided independent study'). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. &lt;br&gt;600&lt;br&gt;B Q SF&lt;br&gt;&lt;br&gt;Lecture&lt;br&gt;6 hours&lt;br&gt;&lt;br&gt;Seminar &lt;br&gt;&lt;br&gt;Tutorial&lt;br&gt;&lt;br&gt;Project supervision&lt;br&gt;Up to 10 hours group or individual tutorial support&lt;br&gt;&lt;br&gt;Demonstration&lt;br&gt;&lt;br&gt;Practical classes/workshops&lt;br&gt;&lt;br&gt;Supervised time in a studio/workshop/lab&lt;br&gt;&lt;br&gt;Fieldwork&lt;br&gt;&lt;br&gt;External visits&lt;br&gt;&lt;br&gt;Work based learning/placement&lt;br&gt;&lt;br&gt;Guided independent study&lt;br&gt;584 hours&lt;br&gt;&lt;br&gt;Study abroad&lt;br&gt;&lt;br&gt;Module description&lt;br&gt;&lt;br&gt;Recommended:&lt;br&gt;Providing a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.&lt;br&gt;Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.&lt;br&gt;Possibly noting what 'type' of module it is, e.g., is it a broad, introductory module or is it a more specialist module that builds on previous learning?&lt;br&gt;A module description should be approximately 150 words.&lt;br&gt;Not recommended:&lt;br&gt;Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.&lt;br&gt;Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.&lt;br&gt;Over-use of technical jargon, which makes the description less ꮥThe Research Dissertation will demonstrate students' consolidation and application of global health&lt;br&gt;system leadership knowledge and skills by undertaking a research task relevant to the students' &lt;br&gt;current area of practice. It will build upon the proposal submitted for Implementation Science &lt;br&gt;(pre-requisite).&lt;br&gt;Students will undertake a research investigation under the guidance of a supervisor after determining&lt;br&gt;an appropriate methodology for the inquiry task, and subject to module lead approval.&lt;br&gt;&lt;br&gt;The investigation could take the form of a systematic review or thematic synthesis or project involving&lt;br&gt;fieldwork (subject to appropriate ethical and/or governance requirements). &lt;br&gt;&lt;br&gt;Outcomes of the study will be contextualised in terms of health system significance and potential for &lt;br&gt;transformation of services, or care delivery, or improving patient care or healthcare professional &lt;br&gt;education, leadership, or policy and promoting the uptake of research findings into policy and practice&lt;br&gt; in the health system.&lt;br&gt;ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student's failure of the module. The QAA publish guidance related to 'levelness' in the Frameworks for Higher Education Qualifications and in their Subject Benchmark Statements. Schools/Institutes are also encouraged to refer to the Birmingham Graduate Attributes. &lt;br&gt;&lt;br&gt;ꮧPlan an inquiry relevant to their clinical area, research unit or educational institution pertaining to health and social care.&lt;br&gt;&lt;br&gt;Review and critically analyse literature and current policy in this area to determine / refine and inform the focus and nature of the investigation.&lt;br&gt;&lt;br&gt;Determine appropriate methods of investigation for the research task; providing rationale for the study, justifying the relevance to their field of practice, and recognising its limitations.&lt;br&gt;&lt;br&gt;Collect or review and critically analyse data or information/data relevant to the subject.&lt;br&gt;&lt;br&gt;Interpret the data collected and explain the significance, relevance, and implications for health system, health policy, service transformation for patient, population or professional, service delivery benefit. ꮨ(i.e., assessment that does not produce a mark that contributes to the overall module mark)&lt;br&gt;Students will submit a research dissertation proposal (building on feedback from Implementation Science) of up to 1000 words. Students will receive feedback on this proposal.&lt;br&gt;Students may present a first draft of their dissertation or part of, to their supervisor for feedback at least 3 weeks prior to submitting the final research dissertation. &lt;br&gt;Q&lt;br&gt;&lt;br&gt;Assessment category (multiple assessments should be included in the same category, e.g., a module with two written tasks and an oral presentation would be 'coursework 100%')&lt;br&gt;If the module is wholly or partly assessed by coursework, please state the overall weighting: 100%&lt;br&gt;&lt;br&gt;B Q&lt;br&gt;&lt;br&gt;If the module is wholly or partly assessed by examination, please state the overall weighting: N/A&lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;Additional information on the method(s) of summative assessment and weighting, e.g., 1hr written unseen examination (50%), 500-word essay (10%), group presentation (40%), if required&lt;br&gt;2000-word research proposal assessment of methods to inform dissertation (15%)&lt;br&gt;&lt;br&gt;Final Global Health System Leadership research dissertation: &lt;br&gt;Word count: 13,000 words. (85%)&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Reassessment: &lt;br&gt;Failure to achieve an overall average of at least 50% will require the student to improve and resubmit the work. &lt;br&gt;&lt;br&gt;Dissertation supervisor support will be offered to support the resubmission attempt.&lt;br&gt;</v>
+      </c>
+      <c r="AU7" t="str">
+        <v>Full Term</v>
+      </c>
+      <c r="AV7" t="str">
+        <v>1</v>
+      </c>
+      <c r="AW7" t="str">
+        <v>Dr Ayat Abu-Agla (Dubai)Dr Ross Millar (Edgbaston)</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>002025</v>
+      </c>
+      <c r="B8" t="str">
+        <v>08</v>
+      </c>
+      <c r="C8" t="str">
+        <v>School of Social Policy</v>
+      </c>
+      <c r="D8" t="str">
+        <v>035</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Health Services Management Centre</v>
+      </c>
+      <c r="F8" t="str">
+        <v>122</v>
+      </c>
+      <c r="G8" t="str">
+        <v>12</v>
+      </c>
+      <c r="H8" t="str">
+        <v>Strategic Planning</v>
+      </c>
+      <c r="I8" t="str">
+        <v>LM Strategic Planning Dub</v>
+      </c>
+      <c r="J8" t="str">
+        <v>LM Strategic Planning</v>
+      </c>
+      <c r="K8" t="str">
+        <v>TBC</v>
+      </c>
+      <c r="L8" t="str">
+        <v>LM</v>
+      </c>
+      <c r="M8" t="str">
+        <v>20</v>
+      </c>
+      <c r="N8" t="str">
+        <v>GT</v>
+      </c>
+      <c r="O8" t="str">
+        <v>Z</v>
+      </c>
+      <c r="P8" t="str">
+        <v>131</v>
+      </c>
+      <c r="Q8" t="str">
+        <v>B900</v>
+      </c>
+      <c r="R8" t="str">
+        <v>100260</v>
+      </c>
+      <c r="S8" t="str">
+        <v>MSc Global Health System Leadership (Dubai campus)PG Dip Global Health System Leadership (Dubai campus) (alternative qual)As an optional module (including any information about its grouping, if relevant):PG Cert Global Health System Leadership (Dubai campus) (alternative qual)</v>
+      </c>
+      <c r="T8" t="str">
+        <v/>
+      </c>
+      <c r="U8" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="V8" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="W8" t="str">
+        <v>UoB Campus Dubai</v>
+      </c>
+      <c r="X8" t="str">
+        <v>U</v>
+      </c>
+      <c r="Y8" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="Z8">
+        <v>10</v>
+      </c>
+      <c r="AA8">
+        <v>10</v>
+      </c>
+      <c r="AB8">
+        <v>10</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>10</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>160</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8" t="str">
+        <v>Globally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region face many diverse conflict and instability and double burden of disease. &lt;br&gt;&lt;br&gt;This module provides a systematic understanding of the basic principles and theories of strategic planning, implementation, monitoring and evaluation, conflict resolution, priority setting and resource mobilisation in relation to health policy and health system strategy and planning.&lt;br&gt;&lt;br&gt;The module enables students to develop a health strategy informed by evidence and tools demonstrating the integrated, theoretical and practical knowledge of strategic planning for health development to advance the UHC and SDG agenda.&lt;br&gt;&lt;br&gt;Topics include: Theories and principles of strategic planning; Monitoring and evaluation; Conflict resolution; Priority setting and; Resource mobilisation.</v>
+      </c>
+      <c r="AM8" t="str">
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Examine the complex range of tasks faced and roles undertaken by strategic health care leaders and managers. &lt;/li&gt;&lt;li&gt;Demonstrate an understanding of the evolution and range of theories and models in strategic planning, implementation, monitoring and evaluation in relation to health policy and health system strategy.&lt;/li&gt;&lt;li&gt;Understand the opportunities and challenges of achieving large scale strategic change in health systems.&lt;/li&gt;&lt;li&gt;Demonstrate a systematic understanding of the basic principles and theories of conflict resolution, priority setting and resource mobilisation in relation to health policy and health system strategy and planning.&lt;/li&gt;&lt;li&gt;Examine approaches to assessing need and opportunities in order to set priorities as part of the strategic planning process.&lt;/li&gt;&lt;li&gt;Develop capabilities in health strategy informed by evidence and tools demonstrating the integrated, theoretical and practical knowledge of strategic planning for health development to advance the UHC and SDG agenda.&lt;/li&gt;&lt;li&gt;Demonstrate the ability to synthesise and critically analyse theory and evidence from a variety of sources on a range of aspects of strategic planning including public involvement, strategic commissioning, decommissioning and integration.&lt;/li&gt;&lt;/ul&gt;</v>
+      </c>
+      <c r="AN8" t="str">
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Social Policy[Health Services Management Centre𓏉Strategic Planning`January 2025¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFGlobal health systems face difficult decisions about how best to allocate resources in an effective, efficient, and sustainable way. This module engages with key concepts, ideas and tools to promote strategic planning for success.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Resource implications have been arranged across Edgbaston and Dubai campuses.SFAre there any related programme modifications? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?YesB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryN/AQIf the module is/will be available to students from other Schools/Institutes/Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Collaborative Provision N/AQ8ApprovalSchool/InstituteDate: 10/08/2023Approving body: SEQC (Chair’s action)College (mandatory for proposals only)Date: 24/08/2023Approving body: CQAAC (Chair’s action)Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Social Policy[Health Services Management Centre] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School/Institute at UoB?NoIf ‘yes’ state which Schools/Institutes they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)N/AʓStrategic Planning#TBC=Masters - LM@20$, if relevantN/A⸮Semester 2ﱙAs a compulsory module (i.e. every student in the year should be ǕMSc Global Health System Leadership (Dubai campus)PG Dip Global Health System Leadership (Dubai campus) (alternative qual)As an optional module (including any information about its grouping, if relevant):PG Cert Global Health System Leadership (Dubai campus) (alternative qual)À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁN/A☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/AÂN/AÃUoB Campus DubaiÄÄ on how your School/Institute/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThis programme has been designed to be fully inclusive.  As a University/Department we are committed to ensuring that all our modules/programmes are inclusive and that we comply fully with the Equality Act of 2010. There are no barriers to applications, access, or progression.  The department always considers whether any parts of module delivery might prove disadvantageous to any group.  Module materials are designed to be fully accessible and are made available in advance to students electronically and, where requested, hard copy form. Further adjustments are made where appropriate to support students with SSAs/RAPs.Q ÅN/AÆ effort for the module (this should equal the total no. of hours in 18.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç10È 10É10ꮛꮜꮝ10ꮞꮟꮠꮡꮢ160ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥGlobally health systems have been at the frontline of the Covid-19 response, regularly experiencing major financial and operational stress. Furthermore, the Eastern Mediterranean Region face many diverse conflict and instability and double burden of disease. This module provides a systematic understanding of the basic principles and theories of strategic planning, implementation, monitoring and evaluation, conflict resolution, priority setting and resource mobilisation in relation to health policy and health system strategy and planning.The module enables students to develop a health strategy informed by evidence and tools demonstrating the integrated, theoretical and practical knowledge of strategic planning for health development to advance the UHC and SDG agenda.Topics include: Theories and principles of strategic planning; Monitoring and evaluation; Conflict resolution; Priority setting and; Resource mobilisation.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. The QAA publish guidance related to ‘levelness’ in the Frameworks for Higher Education Qualifications and in their ꮧBy the end of the module students should be able to:Examine the complex range of tasks faced and roles undertaken by strategic health care leaders and managers. Demonstrate an understanding of the evolution and range of theories and models in strategic planning, implementation, monitoring and evaluation in relation to health policy and health system strategy.Understand the opportunities and challenges of achieving large scale strategic change in health systems.Demonstrate a systematic understanding of the basic principles and theories of conflict resolution, priority setting and resource mobilisation in relation to health policy and health system strategy and planning.Examine approaches to assessing need and opportunities in order to set priorities as part of the strategic planning process.Develop capabilities in health strategy informed by evidence and tools demonstrating the integrated, theoretical and practical knowledge of strategic planning for health development to advance the UHC and SDG agenda.Demonstrate the ability to synthesise and critically analyse theory and evidence from a variety of sources on a range of aspects of strategic planning including public involvement, strategic commissioning, decommissioning and integration.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+      </c>
+      <c r="AO8" t="str">
+        <v>&lt;br&gt;One 4,000-word assignment (100%) strategic business proposal &lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+      </c>
+      <c r="AP8" t="str">
+        <v>N/A - not examined</v>
+      </c>
+      <c r="AQ8" t="str">
+        <v>N/A - not examined</v>
+      </c>
+      <c r="AR8" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="AS8" t="str">
+        <v>Resubmission of above assignment</v>
+      </c>
+      <c r="AT8" t="str">
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;One 4,000-word assignment (100%) strategic business proposal &lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of above assignment</v>
+      </c>
+      <c r="AU8" t="str">
+        <v>Semester 2</v>
+      </c>
+      <c r="AV8" t="str">
+        <v>6</v>
+      </c>
+      <c r="AW8" t="str">
+        <v>Dr Ayat Abu-Agla</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AW3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AW8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major UX overhaul and Tailwind CSS migration
Frontend:
- Migrate from Bootstrap to Tailwind CSS
- Single primary CTA button (Upload → Generate → Download)
- Add module filtering (All/Needs Attention/Ready) with Fix Next button
- Add searchable dropdowns for college/school/department selection
- Add inline field badges linking to fix controls
- Improve hierarchy mismatch UI with decision-oriented copy
- Add step progress indicator and status feedback
- Make success alerts less dominant with auto-dismiss
- Consolidate to single "Module Specification Reader" title

Backend:
- Add fuzzy department matching with suggestions
- Add college/school/department hierarchy validation
- Add cascading data updates (subject, cc, jacs, hecos)
- Add POST /api/download endpoint to use current state
- Add session-based file management
- Update mappings for new departments

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW12"/>
+  <dimension ref="A1:AW9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -553,88 +553,88 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2027/28</v>
+        <v>002026</v>
       </c>
       <c r="B2" t="str">
-        <v>04</v>
+        <v/>
       </c>
       <c r="C2" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>School of Health Sciences</v>
       </c>
       <c r="D2" t="str">
-        <v>056</v>
+        <v>084</v>
       </c>
       <c r="E2" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>Applied Health Sciences</v>
       </c>
       <c r="F2" t="str">
-        <v>013</v>
+        <v/>
       </c>
       <c r="G2" t="str">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="str">
-        <v>Energy Economics and Optimisation</v>
+        <v>Health Economics</v>
       </c>
       <c r="I2" t="str">
-        <v>LH Ener Economic &amp; Optimisatio</v>
+        <v>£1 fo a 20 cr mo La Po GT = £3</v>
       </c>
       <c r="J2" t="str">
-        <v>LH Energy Economics and Optimisation</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Health Economics#08157=LM Health Economics</v>
       </c>
       <c r="K2" t="str">
-        <v>TBC</v>
+        <v>= £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Health Economics#</v>
       </c>
       <c r="L2" t="str">
-        <v>LH</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Health Economics#08157=LM</v>
       </c>
       <c r="M2" t="str">
         <v>20</v>
       </c>
       <c r="N2" t="str">
-        <v>UG</v>
+        <v>GT</v>
       </c>
       <c r="O2" t="str">
         <v>Z</v>
       </c>
       <c r="P2" t="str">
-        <v>116</v>
+        <v/>
       </c>
       <c r="Q2" t="str">
-        <v>H810</v>
+        <v/>
       </c>
       <c r="R2" t="str">
-        <v>100143</v>
+        <v/>
       </c>
       <c r="S2" t="str">
-        <v>As an optional module (including any information about its grouping, if relevant):B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) UG in Chemical Engineering (all variants)</v>
+        <v>404I - PG MC Health Economics FTAs an optional module (including any information about its grouping, if relevant):1778 - PGDip Public Health PT1779 - Master of Public Health PT195B - MSc Health Research Methods FT196B - MSc Health Research Methods PT197B - MSc Health Research Meth Flex198B - PGDip Health Research Meth FT199B - PGDip Health Research Meth PT200B - PGDip Health Research Met Flex201B - PGCert Health Research Meth FT202B - PGCert Health Research Meth PT203B - PGCert Health Resear Meth Flex215E - Master of Public Health (I) FT218E - MSc (I) Health Rese Methods FT290A - MPH (SEAL) 15 month299E - PGDip Respiratory Medicine FT300E - PGDip Respiratory Medicine PT303E - MSc Respiratory Medicine FT304E - MSc Respiratory Medicine PT3231 - Master of Public Health FT4210 - PGCert Public Health PT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)481A - MSc Health Economi Economet FT482A - PGDip Health Econo Economet FT6706 - PGDip Public Health FT693B - PGCert Public Health FT755G - MSc Biomedical Innovation FT756G - MSc Biomedical Innovation PT758G - PGDip Biomedical Innovation FT759G - PGDip Biomedical Innovation PT8003 - PGCert Public Health (Flex)808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex814C - PGCert Pub Health (Glo Hea) FT815C - PGCert Pub Health (Glo Hea) PT9963 - MPH (SEAL) PT9965 - MPH (SEAL) Flex</v>
       </c>
       <c r="T2" t="str">
         <v/>
       </c>
       <c r="U2" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="V2" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="W2" t="str">
-        <v>UoB Campus Edgbaston</v>
+        <v>Birmingham</v>
       </c>
       <c r="X2" t="str">
         <v>B</v>
       </c>
       <c r="Y2" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="Z2">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="AA2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AB2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -658,37 +658,37 @@
         <v>0</v>
       </c>
       <c r="AJ2">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="AK2">
         <v>0</v>
       </c>
       <c r="AL2" t="str">
-        <v>Given the prominence of how energy is supplied and used globally, the course will examine how economics is shaping the policy agenda, and vice versa, considering the different technologies that will be part of the energy system.&lt;br&gt;&lt;br&gt;Students will need to consider a range of topics in economics, sufficient to allow them to understand the business and financial pages of a serious newspaper, and to appreciate the commercial context of engineering decisions that they will make in their subsequent careers, and become aware of the main features of government economic policies.&lt;br&gt;&lt;br&gt;The specific aim is to introduce students to economic issues in energy, and in particular to electricity system economics, since this will greatly influence the future success or failure of different low-carbon technologies.&lt;br&gt;&lt;br&gt;To allow for certain quantitative analysis and decision making optimisation strategies for energy economic situations and energy systems will be investigated.</v>
+        <v>This module introduces the basic principles of health economics and the role of health economics in decision making. It will also equip students with the knowledge needed to interpret and critique applied health economics studies. It covers the different methods of economic evaluation and decision modelling, knowledge of public health and health care systems, the roles and limitations of markets, equity analysis, and incentives in public health systems. It covers the interface between health economics and public health policy.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AM2" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Understand the economic context for decision making by companies and governments, with particular reference to issues concerning energy and carbon emissions.&lt;/li&gt;&lt;li&gt;Apply the economic tools of supply and demand analysis, game theory, and investment appraisal.&lt;/li&gt;&lt;li&gt;Select and use suitable optimisation and other techniques in analysing energy investment and pricing decisions.&lt;/li&gt;&lt;/ul&gt;</v>
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Demonstrate a critical understanding of the principles of economic analysis and health economics applicable to health and public health decision making&lt;/li&gt;&lt;li&gt;Demonstrate a critical understanding of different approaches to economic evaluation and how these are used in public health, i.&lt;/li&gt;&lt;li&gt;Critically appraise a published economic analysis of public health interventions&lt;/li&gt;&lt;li&gt;Demonstrate an understanding of the techniques used to measure both costs and benefits in the evaluation of public health interventions. &lt;/li&gt;&lt;li&gt;Demonstrate a critical understanding of the ethical issues surrounding health economics&lt;/li&gt;&lt;/ul&gt;</v>
       </c>
       <c r="AN2" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Chemical Engineering* (if applicable)Choose an item.BXEnergy Economics and Optimisation`2027/28¬¬ for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFNew programme BEng/MEng in Energy Engineering … and to combine aspects of two existing 10 credits modules, 04 21169 Energy Economics and 04 26506 Plant Optimisation, into one 20 credit module.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Additional resources are not anticipated, as this module will replace existing modules in the School. SFAre there any related programme paperwork? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?Yes. New programme proposalB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryn/a. part of new programme and rolled out to new cohorts of UG provisionQIf the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)n/aQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Accreditation to be sought from the Energy Institute once programme is running and the IChemEQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsN/aQWill the change fit into the partial block structure timetabling approach?                                                                                                                                 N/AIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.It is replacing two existing 10 credits with one 20 credit module, so no additional timetabling of rooms etc is required.8ApprovalSchoolDate: 03/12/2024Approving body: School Programmes and Modules Committee, Chair’s actionsCollege (mandatory for proposals only)Date: 13/12/2024Approving body: CQAACModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Chemical Engineering[Choose an item.] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)ʓEnergy Economics and Optimisation#TBC=Honours - LH@20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.ﱙAs a compulsory module (i.e. every student in the year should be ǕAs an optional module (including any information about its grouping, if relevant):B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) UG in Chemical Engineering (all variants)À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Án/a☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicablen/aÂn/aÃUoB Campus EdgbastonÄÄ on how your School /Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe School is committed to ensuring an inclusive curriculum and actively promotes equality of opportunity to all. The School adheres to all Student Support agreements. There are no barriers to registration for this module when selected as part of the relevant programme offering.The module will seek to promote equality of opportunity through ensuring that no barriers are posed to students who would like to participate.  The module will also seek to ensure there are no barriers to students progressing through it.Scrutiny of EDI issues will be explicitly carried out by Education Committee within the School.Q Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).The module and programme are based on sustainability.This module is directly linked to the Education for Sustainability. In the context of energy transitions, it is directly linked to a number of Sustainable Development Goals, SDG 7 Affordable and Clean energy, SDG 12 Responsible Consumption and Production, and SDG 13 Climate Action.SFÅn/aÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç30È 6É10ꮛꮜꮝ10ꮞꮟꮠꮡꮢ144ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥGiven the prominence of how energy is supplied and used globally, the course will examine how economics is shaping the policy agenda, and vice versa, considering the different technologies that will be part of the energy system.Students will need to consider a range of topics in economics, sufficient to allow them to understand the business and financial pages of a serious newspaper, and to appreciate the commercial context of engineering decisions that they will make in their subsequent careers, and become aware of the main features of government economic policies.The specific aim is to introduce students to economic issues in energy, and in particular to electricity system economics, since this will greatly influence the future success or failure of different low-carbon technologies.To allow for certain quantitative analysis and decision making optimisation strategies for energy economic situations and energy systems will be investigated.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Understand the economic context for decision making by companies and governments, with particular reference to issues concerning energy and carbon emissions.Apply the economic tools of supply and demand analysis, game theory, and investment appraisal.Select and use suitable optimisation and other techniques in analysing energy investment and pricing decisions.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running!School of Health Sciences* (if applicable)Applied Health SciencesXHealth Economics (08157)`2026/27¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  Removal of 10 credit modules was required by College. On review and discussion with module leads, it was apparent that this module already provided sufficient teaching and depth of coverage for a 20-credit module, but there was an opportunity to expand the assessment to include an examination (MCQ) that focuses on key concepts and application of health economics. Inclusion of an unseen examination will also be a positive step to ensuring the module assessment remains robust in the context of generative AI technologies.The new fee for the microcredential version (404I) will be: Home: Ladder Point 1 = £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Health Economics#08157=LM@ 20 $, if relevant⸮Semester 2 ﱙ please state how frequently and when they will be delivered.Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ404I - PG MC Health Economics FTAs an optional module (including any information about its grouping, if relevant):1778 - PGDip Public Health PT1779 - Master of Public Health PT195B - MSc Health Research Methods FT196B - MSc Health Research Methods PT197B - MSc Health Research Meth Flex198B - PGDip Health Research Meth FT199B - PGDip Health Research Meth PT200B - PGDip Health Research Met Flex201B - PGCert Health Research Meth FT202B - PGCert Health Research Meth PT203B - PGCert Health Resear Meth Flex215E - Master of Public Health (I) FT218E - MSc (I) Health Rese Methods FT290A - MPH (SEAL) 15 month299E - PGDip Respiratory Medicine FT300E - PGDip Respiratory Medicine PT303E - MSc Respiratory Medicine FT304E - MSc Respiratory Medicine PT3231 - Master of Public Health FT4210 - PGCert Public Health PT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)481A - MSc Health Economi Economet FT482A - PGDip Health Econo Economet FT6706 - PGDip Public Health FT693B - PGCert Public Health FT755G - MSc Biomedical Innovation FT756G - MSc Biomedical Innovation PT758G - PGDip Biomedical Innovation FT759G - PGDip Biomedical Innovation PT8003 - PGCert Public Health (Flex)808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex814C - PGCert Pub Health (Glo Hea) FT815C - PGCert Pub Health (Glo Hea) PT9963 - MPH (SEAL) PT9965 - MPH (SEAL) FlexÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:Choose an item.13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Á☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableÂÃBirminghamÄComment briefly on how your School/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupPlease briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).ÅÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. Ç18È 3É0ꮛ0ꮜ0ꮝ10ꮞ0ꮟ0ꮠ0ꮡ0ꮢ 169ꮣ0ꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis module introduces the basic principles of health economics and the role of health economics in decision making. It will also equip students with the knowledge needed to interpret and critique applied health economics studies. It covers the different methods of economic evaluation and decision modelling, knowledge of public health and health care systems, the roles and limitations of markets, equity analysis, and incentives in public health systems.  It covers the interface between health economics and public health policy.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:21.1Demonstrate a critical understanding of the principles of economic analysis and health economics applicable to health and public health decision making21.2Demonstrate a critical understanding of different approaches to economic evaluation and how these are used in public health, i.21.3Critically appraise a published economic analysis of public health interventions21.4Demonstrate an understanding of the techniques used to measure both costs and benefits in the evaluation of public health interventions. 21.5Demonstrate a critical understanding of the ethical issues surrounding health economicsꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
       </c>
       <c r="AO2" t="str">
-        <v>&lt;br&gt;&lt;br&gt;Computer based Class test (50%) 2 hrs&lt;br&gt;&lt;br&gt;Unseen Written exam (50%), 2 hrs&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+        <v>&lt;br&gt;Assessment:&lt;br&gt;One written assignment of 2,000 words (60%), and&lt;br&gt;&lt;br&gt;One unseen multiple-choice examination (MCQ) lasting 1 hour and 30 minutes (organised by the School) (40%)&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AP2" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="AQ2" t="str">
-        <v>Summer Exam Period</v>
+        <v>Summer</v>
       </c>
       <c r="AR2" t="str">
-        <v>n/a</v>
+        <v>None</v>
       </c>
       <c r="AS2" t="str">
-        <v>&lt;br&gt;Retake of failed components.</v>
+        <v>Repeat of the failed component(s), i.e. resubmission of an amended 2,000 word assignment and/or MCQ examination, both following individualised feedback.&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AT2" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Computer based Class test (50%) 2 hrs&lt;br&gt;&lt;br&gt;Unseen Written exam (50%), 2 hrs&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Retake of failed components.</v>
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Assessment:&lt;br&gt;One written assignment of 2,000 words (60%), and&lt;br&gt;&lt;br&gt;One unseen multiple-choice examination (MCQ) lasting 1 hour and 30 minutes (organised by the School) (40%)&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Repeat of the failed component(s), i.e. resubmission of an amended 2,000 word assignment and/or MCQ examination, both following individualised feedback.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AU2" t="str">
         <v>Semester 2</v>
@@ -697,102 +697,102 @@
         <v>6</v>
       </c>
       <c r="AW2" t="str">
-        <v>Prof Jonathan Radcliffe</v>
+        <v>Emma Frew / Irina Pokhilenko</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2027/28</v>
+        <v>002026</v>
       </c>
       <c r="B3" t="str">
-        <v>04</v>
+        <v/>
       </c>
       <c r="C3" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>School of Health Sciences</v>
       </c>
       <c r="D3" t="str">
-        <v>056</v>
+        <v>084</v>
       </c>
       <c r="E3" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>Applied Health Sciences</v>
       </c>
       <c r="F3" t="str">
-        <v>013</v>
+        <v/>
       </c>
       <c r="G3" t="str">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" t="str">
-        <v>Energy efficiency and sustainability</v>
+        <v>Sociology and Social Policy</v>
       </c>
       <c r="I3" t="str">
-        <v>LH Ene efficien &amp; sustainabili</v>
+        <v>£1 fo a 20 cr mo La Po GT = £3</v>
       </c>
       <c r="J3" t="str">
-        <v>LH Energy efficiency and sustainability</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Sociology and Social Policy#08158=LM Sociology and Social Policy</v>
       </c>
       <c r="K3" t="str">
-        <v>TBC</v>
+        <v>= £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Sociology and Social Policy#</v>
       </c>
       <c r="L3" t="str">
-        <v>LH</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Sociology and Social Policy#08158=LM</v>
       </c>
       <c r="M3" t="str">
         <v>20</v>
       </c>
       <c r="N3" t="str">
-        <v>UG</v>
+        <v>GT</v>
       </c>
       <c r="O3" t="str">
         <v>Z</v>
       </c>
       <c r="P3" t="str">
-        <v>116</v>
+        <v/>
       </c>
       <c r="Q3" t="str">
-        <v>H810</v>
+        <v/>
       </c>
       <c r="R3" t="str">
-        <v>100143</v>
+        <v/>
       </c>
       <c r="S3" t="str">
-        <v>As an optional module (including any information about its grouping, if relevant):B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) UG Chem Eng programmes plus variants</v>
+        <v>408I - PG MC Sociol &amp; Social Pol FTAs an optional module (including any information about its grouping, if relevant):1778 - PGDip Public Health PT1779 - Master of Public Health PT215E - Master of Public Health (I) FT290A - MPH (SEAL) 15 month3231 - Master of Public Health FT4210 - PGCert Public Health PT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)481A - MSc Health Economi Economet FT482A - PGDip Health Econo Economet FT6706 - PGDip Public Health FT693B - PGCert Public Health FT8003 - PGCert Public Health (Flex)808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex814C - PGCert Pub Health (Glo Hea) FT815C - PGCert Pub Health (Glo Hea) PT9963 - MPH (SEAL) PT9965 - MPH (SEAL) Flex</v>
       </c>
       <c r="T3" t="str">
         <v/>
       </c>
       <c r="U3" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="V3" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="W3" t="str">
-        <v>UoB Campus Edgbaston</v>
+        <v>Birmingham</v>
       </c>
       <c r="X3" t="str">
         <v>B</v>
       </c>
       <c r="Y3" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="Z3">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="AA3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AB3">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AC3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AD3">
         <v>0</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AF3">
         <v>0</v>
@@ -807,37 +807,37 @@
         <v>0</v>
       </c>
       <c r="AJ3">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="AK3">
         <v>0</v>
       </c>
       <c r="AL3" t="str">
-        <v>This module will provide students with a firm and hands-on understanding of the science and engineering behind effective and efficient use of energy technologies, particularly related to conventional energy (e.g. fossil fuels).&lt;br&gt;&lt;br&gt;It will consider how resources can be minimised by reducing energy consumption, specifically by increasing efficiency of use.&lt;br&gt;&lt;br&gt;Additionally, the module will focus on how efficient use of energy can lead to reduction in greenhouse gas emissions and other environmental impacts through the application of life cycle assessment. Life cycle assessment is a standard method used for measuring environmental impacts of products, processes and systems in accordance with ISO 14040/14044:2006. &lt;br&gt;&lt;br&gt;This will be underpinned by extensive coursework and experimental work in which the students will attempt to reduce their own home energy use by 70%. In doing so they will be instructed on energy technology, the economic environment they operate in, environmental sustainability impacts and also the socio-political issues such as tackling energy poverty. &lt;br&gt;</v>
+        <v>&lt;br&gt;The Sociology and Social Policy module aims firstly, to develop knowledge and understanding of sociology as applied to medicine and public health; and secondly, to enable students to understand and critique health policy within a social science framework. While students will be able to introduce and discuss examples of health policy from different countries, teaching on the module will mainly focus on a UK context.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AM3" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Analyse and compare energy use in the built environment.&lt;/li&gt;&lt;li&gt;Categorise and solve problems relating to energy efficiency enhancement.&lt;/li&gt;&lt;li&gt;Conduct life cycle assessment studies.&lt;/li&gt;&lt;li&gt;Evaluate environmental impacts of different energy efficiency and use scenarios.&lt;/li&gt;&lt;li&gt;Compose a business plan for energy saving scheme, explaining technical, environmental and socio-political needs.&lt;/li&gt;&lt;/ul&gt;</v>
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Demonstrate an understanding of the principles of sociology as applied to medicine and health-related behaviour&lt;/li&gt;&lt;li&gt; Critically engage with the relevant sociological and policy literature&lt;/li&gt;&lt;li&gt; Critically engage with examples of policy, applying concepts from the literature&lt;/li&gt;&lt;li&gt; Make connections between health policy and wider developments in society&lt;/li&gt;&lt;/ul&gt;</v>
       </c>
       <c r="AN3" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Chemical Engineering* (if applicable)Choose an item.BXEnergy efficiency and sustainability`2027/28¬¬ for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFNew programme BEng/MEng in Energy Engineering, and extension/expansion of existing 10cr module (04 32463 Efficient Use of Energy which it will replace in the existing progs) to align with UoB’s intention to have minimum of 20cr taught modules. Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Additional resources are not anticipated, as this module will draw on materials already available for existing modules in the School. Focusing on the software use: Life cycle assessment software (Granta) is available to all EPS students through the Apps Anywhere System/Remote cluster groups SFAre there any related programme paperwork? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?Yes. New programme proposalB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryn/a. part of new programme and rolled out to cohorts on UG provisionQIf the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)n/aQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Accreditation to be sought from the Energy Institute &amp; IChemE (for this module) once programme is running. QIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsN/aQWill the change fit into the partial block structure timetabling approach?                                                                                                                                 N/AIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 03/12/2024Approving body: School Programmes and Modules Committee, Chair’s actionsCollege (mandatory for proposals only)Date: 13/12/2024Approving body: CQAACModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Chemical Engineering[Choose an item.] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)ʓEnergy efficiency and sustainability#TBC=Honours - LH@20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.ﱙAs a compulsory module (i.e. every student in the year should be ǕAs an optional module (including any information about its grouping, if relevant):B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) UG Chem Eng programmes plus variantsÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Án/a☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicablen/aÂn/aÃUoB Campus EdgbastonÄÄ on how your School /Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe School is committed to ensuring an inclusive curriculum and actively promotes equality of opportunity to all. The School adheres to all Student Support agreements. There are no barriers to registration for this module when selected as part of the relevant programme offering.The module will seek to promote equality of opportunity through ensuring that no barriers are posed to students who would like to participate.  The module will also seek to ensure there are no barriers to students progressing through it.Scrutiny of EDI issues will be explicitly carried out by Education Committee within the School.Q Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).The module and programme are based on sustainability.This module is directly linked to the Education for Sustainability. In the context of energy transitions, it is directly linked to a number of Sustainable Development Goals, SDG 7 Affordable and Clean energy, SDG 12 Responsible Consumption and Production, and SDG 13 Climate Action.SFÅn/aÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç28È 4É12ꮛ4ꮜꮝꮞꮟꮠꮡꮢ152ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis module will provide students with a firm and hands-on understanding of the science and engineering behind effective and efficient use of energy technologies, particularly related to conventional energy (e.g. fossil fuels).It will consider how resources can be minimised by reducing energy consumption, specifically by increasing efficiency of use.Additionally, the module will focus on how efficient use of energy can lead to reduction in greenhouse gas emissions and other environmental impacts through the application of life cycle assessment. Life cycle assessment is a standard method used for measuring environmental impacts of products, processes and systems in accordance with ISO 14040/14044:2006. This will be underpinned by extensive coursework and experimental work in which the students will attempt to reduce their own home energy use by 70%. In doing so they will be instructed on energy technology, the economic environment they operate in, environmental sustainability impacts and also the socio-political issues such as tackling energy poverty. ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Analyse and compare energy use in the built environment.Categorise and solve problems relating to energy efficiency enhancement.Conduct life cycle assessment studies.Evaluate environmental impacts of different energy efficiency and use scenarios.Compose a business plan for energy saving scheme, explaining technical, environmental and socio-political needs.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running!School of Health Sciences* (if applicable)Applied Health SciencesXSociology and Social Policy (08158)`2026/27¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  Removal of 10 credit modules was required by College. On review and discussion with module leads, it was apparent that this module already provided sufficient teaching and depth of coverage for a 20-credit module, but there was an opportunity to expand the assessment by including a standardised viva-type assessment alongside the written assignment to assess student understanding of the relevant concepts and application of these in their essays. Inclusion of an individual in-person assessment will also be a positive step to ensuring the module assessment remains robust in the context of generative AI technologies.The new fee for the microcredential version (408I) will be: Home: Ladder Point 1 = £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Sociology and Social Policy#08158=LM@ 20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ408I - PG MC Sociol &amp; Social Pol FTAs an optional module (including any information about its grouping, if relevant):1778 - PGDip Public Health PT1779 - Master of Public Health PT215E - Master of Public Health (I) FT290A - MPH (SEAL) 15 month3231 - Master of Public Health FT4210 - PGCert Public Health PT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)481A - MSc Health Economi Economet FT482A - PGDip Health Econo Economet FT6706 - PGDip Public Health FT693B - PGCert Public Health FT8003 - PGCert Public Health (Flex)808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex814C - PGCert Pub Health (Glo Hea) FT815C - PGCert Pub Health (Glo Hea) PT9963 - MPH (SEAL) PT9965 - MPH (SEAL) FlexÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:Choose an item.13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Á☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableÂÃBirminghamÄComment briefly on how your School/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupPlease briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).ÅÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. Ç 17È 0É0ꮛ 0ꮜ0ꮝ13ꮞ0ꮟ0ꮠ0ꮡ0ꮢ 170ꮣ0ꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThe Sociology and Social Policy module aims firstly, to develop knowledge and understanding of sociology as applied to medicine and public health; and secondly, to enable students to understand and critique health policy within a social science framework. While students will be able to introduce and discuss examples of health policy from different countries, teaching on the module will mainly focus on a UK context.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:21.1Demonstrate an understanding of the principles of sociology as applied to medicine and health-related behaviour21.2 Critically engage with the relevant sociological and policy literature21.3 Critically engage with examples of policy, applying concepts from the literature21.4 Make connections between health policy and wider developments in societyꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
       </c>
       <c r="AO3" t="str">
-        <v>&lt;br&gt;&lt;br&gt;&lt;br&gt;Written coursework (80%), max 2500 words &lt;br&gt;Group presentation (20%, 10 mins including Q&amp;A)&lt;br&gt;</v>
+        <v>&lt;br&gt;One written assignment, 2500 words, on a topic of the student's choice agreed in person or in writing with the module lead(s) (50%).&lt;br&gt;&lt;br&gt;15-minute standardised viva examination on the same topic as the written assignment (50%).&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AP3" t="str">
         <v>No</v>
       </c>
       <c r="AQ3" t="str">
-        <v>N/A - not examined</v>
+        <v>N/A – not examined</v>
       </c>
       <c r="AR3" t="str">
-        <v>n/a</v>
+        <v>None</v>
       </c>
       <c r="AS3" t="str">
-        <v>&lt;br&gt;Resubmission of written report to cover all LOs (100% reassessment)&lt;br&gt;</v>
+        <v>Repeat of the failed component(s), i.e. resubmission of failed assignment and/or repeat viva, both following individualised feedback.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AT3" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Written coursework (80%), max 2500 words &lt;br&gt;Group presentation (20%, 10 mins including Q&amp;A)&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of written report to cover all LOs (100% reassessment)&lt;br&gt;</v>
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;One written assignment, 2500 words, on a topic of the student's choice agreed in person or in writing with the module lead(s) (50%).&lt;br&gt;&lt;br&gt;15-minute standardised viva examination on the same topic as the written assignment (50%).&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Repeat of the failed component(s), i.e. resubmission of failed assignment and/or repeat viva, both following individualised feedback.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AU3" t="str">
         <v>Semester 2</v>
@@ -846,93 +846,93 @@
         <v>6</v>
       </c>
       <c r="AW3" t="str">
-        <v>Neha Mehta</v>
+        <v>Antje Lindenmeyer and Ian Litchfield</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>January 2028</v>
+        <v>002026</v>
       </c>
       <c r="B4" t="str">
-        <v>04</v>
+        <v/>
       </c>
       <c r="C4" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>School of Health Sciences</v>
       </c>
       <c r="D4" t="str">
-        <v>056</v>
+        <v>084</v>
       </c>
       <c r="E4" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>Applied Health Sciences</v>
       </c>
       <c r="F4" t="str">
-        <v>013</v>
+        <v/>
       </c>
       <c r="G4" t="str">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" t="str">
-        <v>Energy Systems, Policy, Markets and Regulation</v>
+        <v>Advanced Statistical Methods</v>
       </c>
       <c r="I4" t="str">
-        <v>LI En Syst Poli Mark &amp; Regulat</v>
+        <v>£1 fo a 20 cr mo La Po GT = £3</v>
       </c>
       <c r="J4" t="str">
-        <v>LI Energy Systems, Policy, Markets and Regulation</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Advanced Statistical Methods#19251=LM Advanced Statistical Methods</v>
       </c>
       <c r="K4" t="str">
-        <v>TBC</v>
+        <v>= £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Advanced Statistical Methods#</v>
       </c>
       <c r="L4" t="str">
-        <v>LI</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Advanced Statistical Methods#19251=LM</v>
       </c>
       <c r="M4" t="str">
         <v>20</v>
       </c>
       <c r="N4" t="str">
-        <v>UG</v>
+        <v>GT</v>
       </c>
       <c r="O4" t="str">
         <v>Z</v>
       </c>
       <c r="P4" t="str">
-        <v>116</v>
+        <v/>
       </c>
       <c r="Q4" t="str">
-        <v>H810</v>
+        <v/>
       </c>
       <c r="R4" t="str">
-        <v>100143</v>
+        <v/>
       </c>
       <c r="S4" t="str">
-        <v>B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant): n/a</v>
+        <v>414I - PG MC Adv Stat Methods FTAs an optional module (including any information about its grouping, if relevant):1778 - PGDip Public Health PT1779 - Master of Public Health PT195B - MSc Health Research Methods FT196B - MSc Health Research Methods PT197B - MSc Health Research Meth Flex198B - PGDip Health Research Meth FT199B - PGDip Health Research Meth PT200B - PGDip Health Research Met Flex201B - PGCert Health Research Meth FT202B - PGCert Health Research Meth PT203B - PGCert Health Resear Meth Flex215E - Master of Public Health (I) FT218E - MSc (I) Health Rese Methods FT290A - MPH (SEAL) 15 month3231 - Master of Public Health FT4210 - PGCert Public Health PT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)481A - MSc Health Economi Economet FT482A - PGDip Health Econo Economet FT6706 - PGDip Public Health FT693B - PGCert Public Health FT8003 - PGCert Public Health (Flex)808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex814C - PGCert Pub Health (Glo Hea) FT815C - PGCert Pub Health (Glo Hea) PT9963 - MPH (SEAL) PT9965 - MPH (SEAL) Flex</v>
       </c>
       <c r="T4" t="str">
         <v/>
       </c>
       <c r="U4" t="str">
-        <v>Year 1 Chemical Engineering or Year 1 Energy Engineering would need to be successfully passed.</v>
+        <v/>
       </c>
       <c r="V4" t="str">
-        <v>none</v>
+        <v/>
       </c>
       <c r="W4" t="str">
-        <v>UoB Campus Edgbaston</v>
+        <v>Birmingham</v>
       </c>
       <c r="X4" t="str">
         <v>B</v>
       </c>
       <c r="Y4" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="Z4">
-        <v>NaN</v>
+        <v>15</v>
       </c>
       <c r="AA4">
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>NaN</v>
+        <v>0</v>
       </c>
       <c r="AC4">
         <v>0</v>
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="AE4">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -950,43 +950,43 @@
         <v>0</v>
       </c>
       <c r="AH4">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AI4">
         <v>0</v>
       </c>
       <c r="AJ4">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="AK4">
         <v>0</v>
       </c>
       <c r="AL4" t="str">
-        <v>The module is intended to convey the regulatory and market environment energy systems exist in. It will provide a link between engineering approaches to energy production and distribution infrastructure, key environmental and sustainability issues of energy supply and demand, and the economic and political side of the energy economy. This also includes the decisions and boundary conditions set by policies, roadmaps, and business strategies, within which energy delivery takes place, and which might well conflict with each other.&lt;br&gt;&lt;br&gt;The module will cover domestic and international developments and scenarios for the future development of the national and global energy systems, as well as covering the regulatory environment. This includes technical standardisation, as well as the economic and operational framework different countries and regions choose to set, including the functioning and procedures of international energy markets.&lt;br&gt;&lt;br&gt;Besides the lecture cum tutorial format, students will be offered a seminar/workshop and a field trip to collect first-hand experience with and insight into the procedures and hardware of the energy system.</v>
+        <v>This module will build on student's learning about statistical principles and methods gained in previous modules. Through the use of data sets, students will have the opportunity to develop their knowledge of and skills in of data methods related to the analysis of individual epidemiological studies.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AM4" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Understand the framework(s) energy infrastructure and supply operate under.&lt;/li&gt;&lt;li&gt;Understand the procedures and infrastructure of global energy markets.&lt;/li&gt;&lt;li&gt;Describe to an expert person the function of regulation in the energy infrastructure and markets.&lt;/li&gt;&lt;li&gt;Present to an expert and/or lay audience selected details of energy policies.&lt;/li&gt;&lt;li&gt;Explain how different energy policies and roadmaps influence the sustainability of global energy supply, as well as global energy prices.&lt;/li&gt;&lt;/ul&gt;</v>
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Propose a statistical analysis plan based on the design and aims of a given study &lt;/li&gt;&lt;li&gt;Evaluate data using statistical analysis plans &lt;/li&gt;&lt;li&gt;Differentiate between types of research question and the appropriate analyses required&lt;/li&gt;&lt;li&gt;Critique and understand advanced statistical concepts&lt;/li&gt;&lt;/ul&gt;</v>
       </c>
       <c r="AN4" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Chemical Engineering* (if applicable)Choose an item.BXEnergy Systems, Policy, Markets and Regulation`January 2028¬¬ for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFNew module relevant specifically to Energy Engineers to understand the framework and regulatory environment energy supply systems work in.  It is required for the new Energy Engineering programme and prepares the UG students for taking the Year 4 and/or MSc SEE modules.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Though these are new modules, they build on some existing material from the MSc SEE, with components added by existing staff on the module.SFAre there any related programme paperwork? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?Yes, there is a new Energy Engineering UG programme that this module proposal is part of.B Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryNone – part of new programmeQIf the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body  Energy Institute accreditation will be applied for once the programme is runningQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and Partnershipsn/aQWill the change fit into the partial block structure timetabling approach?                                                                                                                                 N/AIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.Chemical Engineering as it stands is not part of the partial block approach.  No significant impact expected with timetabling as replacing similar existing content.8ApprovalSchoolDate: 29/11/2024Approving body: Chairs action from School Education CommitteeCollege (mandatory for proposals only)Date: 13/12/2024Approving body: CQAACModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Chemical Engineering[Choose an item.] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)ʓEnergy Systems, Policy, Markets and Regulation#TBC=Intermediate - LI@20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.ﱙAs a compulsory module (i.e. every student in the year should be Ǖ B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant): n/aÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁYear 1 Chemical Engineering or Year 1 Energy Engineering would need to be successfully passed.☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableNoneÂnoneÃUoB Campus EdgbastonÄÄ on how your School /Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe School is committed to ensuring an inclusive curriculum and actively promotes equality of opportunity to all. The School adheres to all Student Support agreements. There are no barriers to registration for this module when selected as part of the relevant programme offering.  The module will seek to promote equality of opportunity through ensuring that no barriers are posed to students who would like to participate.  The module will also seek to ensure there are no barriers to students progressing through it.  Scrutiny of EDI issues will be explicitly carried out by Education Committee within the School. Q Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).The whole Energy UG programme is based on principles of sustainability.SFÅn/aÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200 hoursB Q Ç20 hours (2 x 10 weeks)È É20 hours (2 x 10 weeks)ꮛꮜꮝ4 hoursꮞꮟꮠ12 hoursꮡꮢ144 hoursꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThe module is intended to convey the regulatory and market environment energy systems exist in. It will provide a link between engineering approaches to energy production and distribution infrastructure, key environmental and sustainability issues of energy supply and demand, and the economic and political side of the energy economy. This also includes the decisions and boundary conditions set by policies, roadmaps, and business strategies, within which energy delivery takes place, and which might well conflict with each other.The module will cover domestic and international developments and scenarios for the future development of the national and global energy systems, as well as covering the regulatory environment. This includes technical standardisation, as well as the economic and operational framework different countries and regions choose to set, including the functioning and procedures of international energy markets.Besides the lecture cum tutorial format, students will be offered a seminar/workshop and a field trip to collect first-hand experience with and insight into the procedures and hardware of the energy system.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Understand the framework(s) energy infrastructure and supply operate under.Understand the procedures and infrastructure of global energy markets.Describe to an expert person the function of regulation in the energy infrastructure and markets.Present to an expert and/or lay audience selected details of energy policies.Explain how different energy policies and roadmaps influence the sustainability of global energy supply, as well as global energy prices.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running!School of Health Sciences* (if applicable)Applied Health SciencesXAdvanced Statistical Methods (19251)`2026/27¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  Removal of 10 credit modules was required by College. On review and discussion with module leads, it was apparent that this module would benefit from covering an increased range of currently used statistical approaches and a change in the assessment task to increase the complexity of the task (though this does not require a change in module specification).The new fee for the microcredential version (414I) will be: Home: Ladder Point 1 = £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Advanced Statistical Methods#19251=LM@ 20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ414I - PG MC Adv Stat Methods FTAs an optional module (including any information about its grouping, if relevant):1778 - PGDip Public Health PT1779 - Master of Public Health PT195B - MSc Health Research Methods FT196B - MSc Health Research Methods PT197B - MSc Health Research Meth Flex198B - PGDip Health Research Meth FT199B - PGDip Health Research Meth PT200B - PGDip Health Research Met Flex201B - PGCert Health Research Meth FT202B - PGCert Health Research Meth PT203B - PGCert Health Resear Meth Flex215E - Master of Public Health (I) FT218E - MSc (I) Health Rese Methods FT290A - MPH (SEAL) 15 month3231 - Master of Public Health FT4210 - PGCert Public Health PT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)481A - MSc Health Economi Economet FT482A - PGDip Health Econo Economet FT6706 - PGDip Public Health FT693B - PGCert Public Health FT8003 - PGCert Public Health (Flex)808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex814C - PGCert Pub Health (Glo Hea) FT815C - PGCert Pub Health (Glo Hea) PT9963 - MPH (SEAL) PT9965 - MPH (SEAL) FlexÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:Choose an item.13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Á☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableÂÃBirminghamÄComment briefly on how your School/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupPlease briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).ÅÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. Ç15È 0É0ꮛ0ꮜ0ꮝ15ꮞ0ꮟ0ꮠ0ꮡ0ꮢ170ꮣ0ꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis module will build on student's learning about statistical principles and methods gained in previous modules.  Through the use of data sets, students will have the opportunity to develop their knowledge of and skills in of data methods related to the analysis of individual epidemiological studies.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:21.1Propose a statistical analysis plan based on the design and aims of a given study 21.2Evaluate data using statistical analysis plans 21.3Differentiate between types of research question and the appropriate analyses required21.4Critique and understand advanced statistical conceptsꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
       </c>
       <c r="AO4" t="str">
-        <v>&lt;br&gt;50% coursework (individual report 2000 words)&lt;br&gt;&lt;br&gt;30% group presentation (10 mins to include Q&amp;A)&lt;br&gt;20% Year 2 Portfolio work&lt;br&gt;&lt;br&gt;</v>
+        <v>&lt;br&gt; Single written assignment of up to 1,000 words total. (100%)&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AP4" t="str">
         <v>No</v>
       </c>
       <c r="AQ4" t="str">
-        <v>Other (please state below)n/a</v>
+        <v>N/A – not examined</v>
       </c>
       <c r="AR4" t="str">
-        <v>none</v>
+        <v/>
       </c>
       <c r="AS4" t="str">
-        <v>Resubmission of failed element(s)&lt;br&gt;&lt;br&gt;Re-assessment of group work element (if required) will be replaced by a separate piece of written individual work</v>
+        <v>Repeat of the assessment following individual feedback&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AT4" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;50% coursework (individual report 2000 words)&lt;br&gt;&lt;br&gt;30% group presentation (10 mins to include Q&amp;A)&lt;br&gt;20% Year 2 Portfolio work&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of failed element(s)&lt;br&gt;&lt;br&gt;Re-assessment of group work element (if required) will be replaced by a separate piece of written individual work</v>
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt; Single written assignment of up to 1,000 words total. (100%)&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Repeat of the assessment following individual feedback&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AU4" t="str">
         <v>Semester 2</v>
@@ -995,93 +995,93 @@
         <v>6</v>
       </c>
       <c r="AW4" t="str">
-        <v>Prof Robert Steinberger-Wilckens</v>
+        <v>Prof Karla Hemming and Dr Laura Quinn</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2028/29</v>
+        <v>002026</v>
       </c>
       <c r="B5" t="str">
-        <v>04</v>
+        <v/>
       </c>
       <c r="C5" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>School of Health Sciences</v>
       </c>
       <c r="D5" t="str">
-        <v>056</v>
+        <v>084</v>
       </c>
       <c r="E5" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>Applied Health Sciences</v>
       </c>
       <c r="F5" t="str">
-        <v>013</v>
+        <v/>
       </c>
       <c r="G5" t="str">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" t="str">
-        <v>Energy Data and Analytics</v>
+        <v>Health Information and Health Informatics</v>
       </c>
       <c r="I5" t="str">
-        <v>LH Energy Data &amp; Analytics</v>
+        <v>£1 fo a 20 cr mo La Po GT = £3</v>
       </c>
       <c r="J5" t="str">
-        <v>LH Energy Data and Analytics</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ LM Health Information and Health Informatics#25714Equivalent modules: =LM Health Information and Health Informatics</v>
       </c>
       <c r="K5" t="str">
-        <v>TBC</v>
+        <v>= £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ LM Health Information and Health Informatics#</v>
       </c>
       <c r="L5" t="str">
-        <v>LH</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ LM Health Information and Health Informatics#25714Equivalent modules: =LM</v>
       </c>
       <c r="M5" t="str">
         <v>20</v>
       </c>
       <c r="N5" t="str">
-        <v>UG</v>
+        <v>GT</v>
       </c>
       <c r="O5" t="str">
         <v>Z</v>
       </c>
       <c r="P5" t="str">
-        <v>116</v>
+        <v/>
       </c>
       <c r="Q5" t="str">
-        <v>H810</v>
+        <v/>
       </c>
       <c r="R5" t="str">
-        <v>100143</v>
+        <v/>
       </c>
       <c r="S5" t="str">
-        <v>B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant):</v>
+        <v>1778 - PGDip Public Health PT1779 - Master of Public Health PT215E - Master of Public Health (I) FT290A - MPH (SEAL) 15 month3231 - Master of Public Health FT403I - PG MC Heal Info &amp; Heal Info FT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)6706 - PGDip Public Health FT808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex9963 - MPH (SEAL) PT9965 - MPH (SEAL) FlexAs an optional module (including any information about its grouping, if relevant):178E - PhD Integ St Life Sci MDS FT180E - PhD Integ St Life Sci LES FT195B - MSc Health Research Methods FT196B - MSc Health Research Methods PT197B - MSc Health Research Meth Flex198B - PGDip Health Research Meth FT199B - PGDip Health Research Meth PT200B - PGDip Health Research Met Flex201B - PGCert Health Research Meth FT202B - PGCert Health Research Meth PT203B - PGCert Health Resear Meth Flex218E - MSc (I) Health Rese Methods FT299E - PGDip Respiratory Medicine FT300E - PGDip Respiratory Medicine PT303E - MSc Respiratory Medicine FT304E - MSc Respiratory Medicine PT733H - MSc Prim Care Rese &amp; Leader FT871H - PGDip Prim Care Res &amp; Lead FT872H - PGDip Prim Care Res &amp;amp; Lead PT</v>
       </c>
       <c r="T5" t="str">
         <v/>
       </c>
       <c r="U5" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="V5" t="str">
-        <v>n/a</v>
+        <v>02 21812 LM Epid Stat + Res Meth (Epid)02 27286 LM Pract Epidemiology Stat</v>
       </c>
       <c r="W5" t="str">
-        <v>UoB Campus Edgbaston</v>
+        <v>Birmingham</v>
       </c>
       <c r="X5" t="str">
         <v>B</v>
       </c>
       <c r="Y5" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="Z5">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AA5">
         <v>0</v>
       </c>
       <c r="AB5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -1105,132 +1105,132 @@
         <v>0</v>
       </c>
       <c r="AJ5">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="AK5">
         <v>0</v>
       </c>
       <c r="AL5" t="str">
-        <v>This 20-credit module provides foundational skills applicable across the energy sector, preparing students with transferable skills for a focus on energy management, consulting, and sustainability analysis.&lt;br&gt;&lt;br&gt;The module provides a practical introduction to energy data analysis, emphasising hands-on experience with real-world datasets. Students develop analytical capabilities using Python programming, moving beyond the limitations of traditional spreadsheet software to handle complex energy data sources. The curriculum covers essential data sources including electrical grid data that covers both spatial and time-series and building category data. Students to critically evaluate data quality and in techniques for exploratory data analysis.&lt;br&gt;&lt;br&gt;Technical skills development centres on Python programming fundamentals for data analysis, with students gaining experience in data cleaning, preprocessing, and time series analysis techniques specific to energy data. The module emphasises the integration of multiple data sources and statistical analysis methods particularly relevant to energy consumption patterns. Students learn to analyse load profiles, identify peak demand, and better understand renewable energy generation and energy consumption patterns through hands-on exercises. Introductory examples will be extended into various types of near-casting.&lt;br&gt;&lt;br&gt;Assessment focuses on practical application through project work, where students analyse real energy datasets and present their findings using industry-standard methods.</v>
+        <v>The module introduces students to population level health information and to principles of health informatics.&lt;br&gt;&lt;br&gt;The aim of the module is to provide students with a detailed understanding of: why health information is important; how to identify and critique valid sources of health information; health information systems in the UK and elsewhere, and how these are integrated; the governance structures for health information; the role of computerised decision support systems; and emerging information related technologies in delivering health care.&lt;br&gt;&lt;br&gt;The module enables students to: appreciate the vast amount of accessible health information available; value the impact of high-quality health intelligence in shaping public health policies and interventions, and understand the role of health informatics in delivering health care in an efficient way.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AM5" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Critically evaluate the quality and limitations of energy datasets while applying appropriate data cleaning and preprocessing techniques&lt;/li&gt;&lt;li&gt;Explain the main datetime formats found in energy datasets, and their advantages and disadvantages&lt;/li&gt;&lt;li&gt;Explain the main geospatial formats found in energy datasets, and their advantages and disadvantages&lt;/li&gt;&lt;li&gt;Demonstrate proficiency in analysing time-series energy data, including the ability to integrate multiple data sources effectively&lt;/li&gt;&lt;li&gt;Apply statistical methods to analyse energy consumption patterns and develop near-casting predictions from real-world or synthetic datasets&lt;/li&gt;&lt;li&gt;Design and execute data analysis workflows that combine multiple energy datasets to address specific analytical challenges&lt;/li&gt;&lt;li&gt;Evaluate and implement appropriate error detection and data imputation strategies for energy datasets&lt;/li&gt;&lt;/ul&gt;</v>
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Develop, collate and critically appraise suitable health information data and systems to describe given health conditions;&lt;/li&gt;&lt;li&gt;Understand and interpret current trends and future developments in population health data collection and storage;&lt;/li&gt;&lt;li&gt;Critically analyse governance structures in handling health information related data;&lt;/li&gt;&lt;li&gt;Understand the principles of the role of computerised decision support tools in the management of health conditions at a population level.&lt;/li&gt;&lt;/ul&gt;</v>
       </c>
       <c r="AN5" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Chemical Engineering* (if applicable)Choose an item.BXEnergy Data and Analytics`2028/29¬¬ for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFNew programme BEng/MEng in Energy Engineering. This module will provides a practical introduction to energy data analysis, emphasising hands-on experience with real-world datasets, the critically evaluation of data quality and in techniques for exploratory data analysis. Thus, providing foundational skills applicable across the energy sector, preparing students with transferable skills for a focus on energy management, consulting, and sustainability analysis.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Additional resources are not anticipated, as this module will draw on materials already available for existing modules in the School. SFAre there any related programme paperwork? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?Yes. New programme proposalB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryn/a. part of new programmeQIf the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)n/aQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Accreditation to be sought from the Energy Institute once programme is running. QIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsN/aQWill the change fit into the partial block structure timetabling approach?                                                                                                                                 N/AIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 03/12/2024Approving body: School Programmes and Modules Committee, Chair’s actionsCollege (mandatory for proposals only)Date: 13/12/2024Approving body: CQAACModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Chemical Engineering[Choose an item.] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)ʓEnergy Data and Analytics#TBC=Honours - LH@20$, if relevant⸮Semester 1ﱙ please state how frequently and when they will be delivered.ﱙAs a compulsory module (i.e. every student in the year should be ǕB.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Án/a☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicablen/aÂn/aÃUoB Campus EdgbastonÄÄ on how your School /Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe School is committed to ensuring an inclusive curriculum and actively promotes equality of opportunity to all. The School adheres to all Student Support agreements. There are no barriers to registration for this module when selected as part of the relevant programme offering.The module will seek to promote equality of opportunity through ensuring that no barriers are posed to students who would like to participate.  The module will also seek to ensure there are no barriers to students progressing through it.Scrutiny of EDI issues will be explicitly carried out by Education Committee within the School.Q Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).The module and programme are based on sustainability.This module is directly linked to the Education for Sustainability. In the context of energy transitions, it is directly linked to a number of Sustainable Development Goals, SDG 7 Affordable and Clean energy, SDG 12 Responsible Consumption and Production, and SDG 13 Climate Action.SFÅn/aÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç30È É20ꮛꮜꮝꮞꮟꮠꮡꮢ150ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis 20-credit module provides foundational skills applicable across the energy sector, preparing students with transferable skills for a focus on energy management, consulting, and sustainability analysis.The module provides a practical introduction to energy data analysis, emphasising hands-on experience with real-world datasets. Students develop analytical capabilities using Python programming, moving beyond the limitations of traditional spreadsheet software to handle complex energy data sources. The curriculum covers essential data sources including electrical grid data that covers both spatial and time-series and building category data. Students to critically evaluate data quality and in techniques for exploratory data analysis.Technical skills development centres on Python programming fundamentals for data analysis, with students gaining experience in data cleaning, preprocessing, and time series analysis techniques specific to energy data. The module emphasises the integration of multiple data sources and statistical analysis methods particularly relevant to energy consumption patterns. Students learn to analyse load profiles, identify peak demand, and better understand renewable energy generation and energy consumption patterns through hands-on exercises. Introductory examples will be extended into various types of near-casting.Assessment focuses on practical application through project work, where students analyse real energy datasets and present their findings using industry-standard methods.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Critically evaluate the quality and limitations of energy datasets while applying appropriate data cleaning and preprocessing techniquesExplain the main datetime formats found in energy datasets, and their advantages and disadvantagesExplain the main geospatial formats found in energy datasets, and their advantages and disadvantagesDemonstrate proficiency in analysing time-series energy data, including the ability to integrate multiple data sources effectivelyApply statistical methods to analyse energy consumption patterns and develop near-casting predictions from real-world or synthetic datasetsDesign and execute data analysis workflows that combine multiple energy datasets to address specific analytical challengesEvaluate and implement appropriate error detection and data imputation strategies for energy datasetsꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running!School of Health Sciences* (if applicable)Applied Health SciencesXLM Health Information and Health Informatics (25714)`2026/27¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  Removal of 10 credit modules was required by College. On review and discussion with module leads, it was apparent that this module already provided sufficient teaching and depth of coverage for a 20-credit module, but there was an opportunity to expand and increase the size and complexity of the written assignment, so that it better tests key concepts and includes a real-world type task. The revised assignment will also be more rigorous in design to ensure the module assessment remains robust in the context of generative AI technologies.The new fee for the microcredential version (403I) will be: Home: Ladder Point 1 = £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ LM Health Information and Health Informatics#25714Equivalent modules: =LM@ 20$, if relevant⸮Semester  1ﱙ please state how frequently and when they will be delivered.Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ1778 - PGDip Public Health PT1779 - Master of Public Health PT215E - Master of Public Health (I) FT290A - MPH (SEAL) 15 month3231 - Master of Public Health FT403I - PG MC Heal Info &amp; Heal Info FT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)6706 - PGDip Public Health FT808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex9963 - MPH (SEAL) PT9965 - MPH (SEAL) FlexAs an optional module (including any information about its grouping, if relevant):178E - PhD Integ St Life Sci MDS FT180E - PhD Integ St Life Sci LES FT195B - MSc Health Research Methods FT196B - MSc Health Research Methods PT197B - MSc Health Research Meth Flex198B - PGDip Health Research Meth FT199B - PGDip Health Research Meth PT200B - PGDip Health Research Met Flex201B - PGCert Health Research Meth FT202B - PGCert Health Research Meth PT203B - PGCert Health Resear Meth Flex218E - MSc (I) Health Rese Methods FT299E - PGDip Respiratory Medicine FT300E - PGDip Respiratory Medicine PT303E - MSc Respiratory Medicine FT304E - MSc Respiratory Medicine PT733H - MSc Prim Care Rese &amp; Leader FT871H - PGDip Prim Care Res &amp; Lead FT872H - PGDip Prim Care Res &amp;amp; Lead PTÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:Choose an item.13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Á☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableÂ02 21812 LM Epid Stat + Res Meth (Epid)02 27286 LM Pract Epidemiology StatÃBirminghamÄComment briefly on how your School/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupPlease briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).ÅÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. Ç34È 0É0ꮛ0ꮜ0ꮝ0ꮞ0ꮟ0ꮠ0ꮡ0ꮢ 166ꮣ0ꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThe module introduces students to population level health information and to principles of health informatics.The aim of the module is to provide students with a detailed understanding of: why health information is important; how to identify and critique valid sources of health information; health information systems in the UK and elsewhere, and how these are integrated; the governance structures for health information; the role of computerised decision support systems; and emerging information related technologies in delivering health care.The module enables students to: appreciate the vast amount of accessible health information available; value the impact of high-quality health intelligence in shaping public health policies and interventions, and understand the role of health informatics in delivering health care in an efficient way.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:21.1Develop, collate and critically appraise suitable health information data and systems to describe given health conditions;21.2Understand and interpret current trends and future developments in population health data collection and storage;21.3Critically analyse governance structures in handling health information related data;21.4Understand the principles of the role of computerised decision support tools in the management of health conditions at a population level.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
       </c>
       <c r="AO5" t="str">
-        <v>&lt;br&gt;&lt;br&gt;Written coursework 2500 words (50%)&lt;br&gt;&lt;br&gt;90-minute written unseen examination (50%)&lt;br&gt;&lt;br&gt;</v>
+        <v>&lt;br&gt;One 3000 word written assignment to investigate the epidemiology of a given health condition and analyse aspects of a health information system related to that subject&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AP5" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="AQ5" t="str">
-        <v>N/A - not examined</v>
+        <v>N/A – not examined</v>
       </c>
       <c r="AR5" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="AS5" t="str">
-        <v>&lt;br&gt;Resubmission of failed component(s)</v>
+        <v>Resubmission of written assignment following individualised feedback.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AT5" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Written coursework 2500 words (50%)&lt;br&gt;&lt;br&gt;90-minute written unseen examination (50%)&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of failed component(s)</v>
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;One 3000 word written assignment to investigate the epidemiology of a given health condition and analyse aspects of a health information system related to that subject&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of written assignment following individualised feedback.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AU5" t="str">
-        <v>Semester 1</v>
+        <v>Semester  1</v>
       </c>
       <c r="AV5" t="str">
-        <v>5</v>
+        <v/>
       </c>
       <c r="AW5" t="str">
-        <v>Grant Wilson</v>
+        <v>Nicola Adderley and Zhaonan Wang</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2027/28</v>
+        <v>002026</v>
       </c>
       <c r="B6" t="str">
-        <v>04</v>
+        <v/>
       </c>
       <c r="C6" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>School of Health Sciences</v>
       </c>
       <c r="D6" t="str">
-        <v>056</v>
+        <v>084</v>
       </c>
       <c r="E6" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>Applied Health Sciences</v>
       </c>
       <c r="F6" t="str">
-        <v>013</v>
+        <v/>
       </c>
       <c r="G6" t="str">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" t="str">
-        <v>Low Carbon Processes</v>
+        <v>Introduction to Leadership and Management for Health</v>
       </c>
       <c r="I6" t="str">
-        <v>LH Low Carbon Processes</v>
+        <v>£1 fo a 20 cr mo La Po GT = £3</v>
       </c>
       <c r="J6" t="str">
-        <v>LH Low Carbon Processes</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Introduction to Leadership and Management for Health#26552=LM Introduction to Leadership and Management for Health</v>
       </c>
       <c r="K6" t="str">
-        <v>TBC</v>
+        <v>= £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Introduction to Leadership and Management for Health#</v>
       </c>
       <c r="L6" t="str">
-        <v>LH</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Introduction to Leadership and Management for Health#26552=LM</v>
       </c>
       <c r="M6" t="str">
         <v>20</v>
       </c>
       <c r="N6" t="str">
-        <v>UG</v>
+        <v>GT</v>
       </c>
       <c r="O6" t="str">
         <v>Z</v>
       </c>
       <c r="P6" t="str">
-        <v>116</v>
+        <v/>
       </c>
       <c r="Q6" t="str">
-        <v>H810</v>
+        <v/>
       </c>
       <c r="R6" t="str">
-        <v>100143</v>
+        <v/>
       </c>
       <c r="S6" t="str">
-        <v>As an optional module (including any information about its grouping, if relevant):B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) UG in Chemical Engineering (all variants)</v>
+        <v>405I - PG MC Int to Lead &amp; Man Hea FTAs an optional module (including any information about its grouping, if relevant):1778 - PGDip Public Health PT1779 - Master of Public Health PT215E - Master of Public Health (I) FT290A - MPH (SEAL) 15 month299E - PGDip Respiratory Medicine FT300E - PGDip Respiratory Medicine PT303E - MSc Respiratory Medicine FT304E - MSc Respiratory Medicine PT3231 - Master of Public Health FT4210 - PGCert Public Health PT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)481A - MSc Health Economi Economet FT482A - PGDip Health Econo Economet FT6706 - PGDip Public Health FT693B - PGCert Public Health FT8003 - PGCert Public Health (Flex)808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex814C - PGCert Pub Health (Glo Hea) FT815C - PGCert Pub Health (Glo Hea) PT9963 - MPH (SEAL) PT9965 - MPH (SEAL) Flex</v>
       </c>
       <c r="T6" t="str">
         <v/>
       </c>
       <c r="U6" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="V6" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="W6" t="str">
-        <v>UoB Campus Edgbaston</v>
+        <v>Birmingham</v>
       </c>
       <c r="X6" t="str">
         <v>B</v>
       </c>
       <c r="Y6" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="Z6">
         <v>25</v>
       </c>
       <c r="AA6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AB6">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="AC6">
         <v>0</v>
@@ -1254,37 +1254,37 @@
         <v>0</v>
       </c>
       <c r="AJ6">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="AK6">
         <v>0</v>
       </c>
       <c r="AL6" t="str">
-        <v>The low-carbon transition of the chemical and energy industry – either by modifying existing products or expanding their operations to include low-carbon technologies – are seen as crucial to achieving net zero targets, and this requires future engineers to be equipped with the knowledge and skills required to drive the transition and innovation.&lt;br&gt;Given as a society, we are likely facing irreversible effects of climate change, we must also ensure that designs are robust and able to withstand a changing climate (e.g. ambient temperature changes and wider more frequent and substantial flooding).&lt;br&gt;The module will consider aspects of how to modify existing and design new process and systems from both a technological and societal perspective.&lt;br&gt;</v>
+        <v>This module provides an introduction to management for students from a range of professional and academic backgrounds. Its aim is to examine the main components of management in a way that is accessible to students with different levels of experience of working in organisations. Using health care organisations as a focus it explores the key elements of managing self, managing teams and managing organisations to enable students to develop a critical perspective on organisation. It focuses on the use of theory and research to build an understanding of management and leadership in organisations.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AM6" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Acquire core knowledge and understanding of a breath of zero or low-carbon fuels, chemical and energy process technologies/concepts and underlying low-carbon engineering principles&lt;/li&gt;&lt;li&gt;Develop critical awareness around the limits of low-carbon chemical/energy processes and of the potential of new and emerging technologies/concepts and appreciate the potential societal challenges to implementation.&lt;/li&gt;&lt;li&gt;Apply the principles of sustainability, economics, and ethics via cost-benefit analysis for the selection of processes, energy products and plant with the environment and minimising of adverse impacts.&lt;/li&gt;&lt;li&gt;Demonstrate understanding of Management of Change procedures and thus how they can be implemented for both system technology changes but also within society.&lt;/li&gt;&lt;li&gt;Critically assess design choices specifically relating to functional and efficient system selection for robust and resilient operation in different and varying climates.&lt;/li&gt;&lt;/ul&gt;</v>
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Discuss broad conceptual approaches to the study of management&lt;/li&gt;&lt;li&gt;Examine management of self; management of teams; management of the organisation as a framework for the practice of management.&lt;/li&gt;&lt;li&gt;Analyse critically specific theories of management and leadership and their utility in increasing understanding of organisations&lt;/li&gt;&lt;li&gt;Examine the rationale for and effectiveness of change strategies utilised in health care organisations.&lt;/li&gt;&lt;li&gt;Evaluate critically the concept of organisational culture and its applications in managing health care.&lt;/li&gt;&lt;li&gt;Critique relevant research to inform an analysis of health care organisations&lt;/li&gt;&lt;li&gt;Critically analyse and understand global leadership challenges and opportunities in public health&lt;/li&gt;&lt;/ul&gt;</v>
       </c>
       <c r="AN6" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Chemical Engineering* (if applicable)Choose an item.BXLow Carbon Processes`2027/28¬¬ for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFNew programme BEng/MEng in Energy Engineering. This module is a combination of two existing 10 credit options, 04 40404 Designing for Climate Change and 04 40405 Low Carbon Chemical and Energy Processes.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Additional resources are not anticipated, as this module will be replacing two existing modules. SFAre there any related programme paperwork? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?Yes. New programme proposalB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryn/a. part of new programme and rolled out to cohorts on the UG provisionQIf the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)n/aQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Accreditation to be sought from the Energy Institute once programme is running and IChemEQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsN/aQWill the change fit into the partial block structure timetabling approach?                                                                                                                                 N/AIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.None replacing two existing 10 credit modules.8ApprovalSchoolDate: 03/12/2024Approving body: School Programmes and Modules Committee, Chair’s actionsCollege (mandatory for proposals only)Date: 13/12/2024Approving body: CQAACModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Chemical Engineering[Choose an item.] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)ʓLow Carbon Processes#TBC=Honours - LH@20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.ﱙAs a compulsory module (i.e. every student in the year should be ǕAs an optional module (including any information about its grouping, if relevant):B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) UG in Chemical Engineering (all variants)À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Án/a☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicablen/aÂn/aÃUoB Campus EdgbastonÄÄ on how your School /Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe School is committed to ensuring an inclusive curriculum and actively promotes equality of opportunity to all. The School adheres to all Student Support agreements. There are no barriers to registration for this module when selected as part of the relevant programme offering.The module will seek to promote equality of opportunity through ensuring that no barriers are posed to students who would like to participate.  The module will also seek to ensure there are no barriers to students progressing through it.Scrutiny of EDI issues will be explicitly carried out by Education Committee within the School.Q Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).The module and programme are based on sustainability.This module is directly linked to the Education for Sustainability. In the context of energy transitions, it is directly linked to a number of Sustainable Development Goals, SDG 7 Affordable and Clean energy, SDG 12 Responsible Consumption and Production, and SDG 13 Climate Action.SFÅn/aÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç25È 10É17ꮛꮜꮝꮞꮟꮠꮡꮢ148ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThe low-carbon transition of the chemical and energy industry – either by modifying existing products or expanding their operations to include low-carbon technologies – are seen as crucial to achieving net zero targets, and this requires future engineers to be equipped with the knowledge and skills required to drive the transition and innovation.Given as a society, we are likely facing irreversible effects of climate change, we must also ensure that designs are robust and able to withstand a changing climate (e.g. ambient temperature changes and wider more frequent and substantial flooding).The module will consider aspects of how to modify existing and design new process and systems from both a technological and societal perspective.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Acquire core knowledge and understanding of a breath of zero or low-carbon fuels, chemical and energy process technologies/concepts and underlying low-carbon engineering principlesDevelop critical awareness around the limits of low-carbon chemical/energy processes and of the potential of new and emerging technologies/concepts and appreciate the potential societal challenges to implementation.Apply the principles of sustainability, economics, and ethics via cost-benefit analysis for the selection of processes, energy products and plant with the environment and minimising of adverse impacts.Demonstrate understanding of Management of Change procedures and thus how they can be implemented for both system technology changes but also within society.Critically assess design choices specifically relating to functional and efficient system selection for robust and resilient operation in different and varying climates.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running!School of Health Sciences* (if applicable)Applied Health SciencesXIntroduction to Leadership and Management for Health (26552)`2026/27¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  Removal of 10 credit modules was required by College. On review and discussion with module leads, it was apparent that this module already provided sufficient teaching and depth of coverage for a 20-credit module, but there was an opportunity to include a learning outcome that took an explicitly global focus, and expand the assessment to introduce a group based presentation and include an element of personal reflection. Inclusion of classroom-based group-presentation will also be a positive step to ensuring the module assessment remains robust in the context of generative AI technologies.The new fee for the microcredential version (405I) will be: Home: Ladder Point 1 = £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Introduction to Leadership and Management for Health#26552=LM@ 20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ405I - PG MC Int to Lead &amp; Man Hea FTAs an optional module (including any information about its grouping, if relevant):1778 - PGDip Public Health PT1779 - Master of Public Health PT215E - Master of Public Health (I) FT290A - MPH (SEAL) 15 month299E - PGDip Respiratory Medicine FT300E - PGDip Respiratory Medicine PT303E - MSc Respiratory Medicine FT304E - MSc Respiratory Medicine PT3231 - Master of Public Health FT4210 - PGCert Public Health PT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)481A - MSc Health Economi Economet FT482A - PGDip Health Econo Economet FT6706 - PGDip Public Health FT693B - PGCert Public Health FT8003 - PGCert Public Health (Flex)808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex814C - PGCert Pub Health (Glo Hea) FT815C - PGCert Pub Health (Glo Hea) PT9963 - MPH (SEAL) PT9965 - MPH (SEAL) FlexÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:Choose an item.13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Á☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableÂÃBirminghamÄComment briefly on how your School/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupPlease briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).ÅÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. Ç25È 5É0ꮛ0ꮜ0ꮝ0ꮞ0ꮟ0ꮠ0ꮡ0ꮢ 170ꮣ0ꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis module provides an introduction to management for students from a range of professional and academic backgrounds.  Its aim is to examine the main components of management in a way that is accessible to students with different levels of experience of working in organisations.  Using health care organisations as a focus it explores the key elements of managing self, managing teams and managing organisations to enable students to develop a critical perspective on organisation.  It focuses on the use of theory and research to build an understanding of management and leadership in organisations.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:21.1Discuss broad conceptual approaches to the study of management21.2Examine management of self; management of teams; management of the organisation as a framework for the practice of management.21.3Analyse critically specific theories of management and leadership  and  their utility in increasing understanding of organisations21.4Examine the rationale for and effectiveness of change strategies utilised in health care organisations.21.5Evaluate critically the concept of organisational culture and its applications in managing health care.21.6Critique relevant research to inform an analysis of health care organisations21.7Critically analyse and understand global leadership challenges and opportunities in public healthꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
       </c>
       <c r="AO6" t="str">
-        <v>&lt;br&gt;Written coursework (50%), individual 2000 words&lt;br&gt;&lt;br&gt;Unseen written exam (50%), 2hrs&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+        <v>&lt;br&gt;10-minute group presentation followed by questions (10%), and&lt;br&gt;&lt;br&gt;500-word individual reflection on working in the group (20%), and&lt;br&gt;&lt;br&gt;Individual 2000-word critical written assignment (70%)&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AP6" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="AQ6" t="str">
-        <v>Summer Exam Period</v>
+        <v>N/A – not examined</v>
       </c>
       <c r="AR6" t="str">
-        <v/>
+        <v>None</v>
       </c>
       <c r="AS6" t="str">
-        <v>Resubmission and/or retaking of failed components.&lt;br&gt;(Resit exam would be in Supplementary period)</v>
+        <v>Repeat of the failed component following individual feedback (or group feedback for the group presentation), i.e. repeat of the group presentation and/or resubmission of the individual reflection and/or resubmission of the critical written assignment.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AT6" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Written coursework (50%), individual 2000 words&lt;br&gt;&lt;br&gt;Unseen written exam (50%), 2hrs&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission and/or retaking of failed components.&lt;br&gt;(Resit exam would be in Supplementary period)</v>
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;10-minute group presentation followed by questions (10%), and&lt;br&gt;&lt;br&gt;500-word individual reflection on working in the group (20%), and&lt;br&gt;&lt;br&gt;Individual 2000-word critical written assignment (70%)&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Repeat of the failed component following individual feedback (or group feedback for the group presentation), i.e. repeat of the group presentation and/or resubmission of the individual reflection and/or resubmission of the critical written assignment.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AU6" t="str">
         <v>Semester 2</v>
@@ -1293,93 +1293,93 @@
         <v>6</v>
       </c>
       <c r="AW6" t="str">
-        <v>Dr Matt Keith</v>
+        <v>A Neath and Marisza Hijryana</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2027/28</v>
+        <v>002026</v>
       </c>
       <c r="B7" t="str">
-        <v>04</v>
+        <v/>
       </c>
       <c r="C7" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>School of Health Sciences</v>
       </c>
       <c r="D7" t="str">
-        <v>056</v>
+        <v>084</v>
       </c>
       <c r="E7" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>Applied Health Sciences</v>
       </c>
       <c r="F7" t="str">
-        <v>013</v>
+        <v/>
       </c>
       <c r="G7" t="str">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" t="str">
-        <v>Petrochemical Engineering and Process Optimisation</v>
+        <v>Healthcare Public Health</v>
       </c>
       <c r="I7" t="str">
-        <v>LH Petroch Engine &amp; Pr Optimis</v>
+        <v>£1 fo a 20 cr mo La Po GT = £3</v>
       </c>
       <c r="J7" t="str">
-        <v>LH Petrochemical Engineering and Process Optimisation</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ LM Healthcare Public Health#37682Equivalent modules: =LM Healthcare Public Health</v>
       </c>
       <c r="K7" t="str">
-        <v>TBC</v>
+        <v>= £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ LM Healthcare Public Health#</v>
       </c>
       <c r="L7" t="str">
-        <v>LH</v>
+        <v>£1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ LM Healthcare Public Health#37682Equivalent modules: =LM</v>
       </c>
       <c r="M7" t="str">
         <v>20</v>
       </c>
       <c r="N7" t="str">
-        <v>UG</v>
+        <v>GT</v>
       </c>
       <c r="O7" t="str">
         <v>Z</v>
       </c>
       <c r="P7" t="str">
-        <v>116</v>
+        <v/>
       </c>
       <c r="Q7" t="str">
-        <v>H810</v>
+        <v/>
       </c>
       <c r="R7" t="str">
-        <v>100143</v>
+        <v/>
       </c>
       <c r="S7" t="str">
-        <v>As an optional module (including any information about its grouping, if relevant):B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) UG in Chemical Engineering (all variants)</v>
+        <v>406I - PG MC Healthcare Pub Health FTAs an optional module (including any information about its grouping, if relevant):1778 - PGDip Public Health PT1779 - Master of Public Health PT197B - MSc Health Research Meth Flex198B - PGDip Health Research Meth FT199B - PGDip Health Research Meth PT200B - PGDip Health Research Met Flex201B - PGCert Health Research Meth FT202B - PGCert Health Research Meth PT203B - PGCert Health Resear Meth Flex215E - Master of Public Health (I) FT290A - MPH (SEAL) 15 month299E - PGDip Respiratory Medicine FT300E - PGDip Respiratory Medicine PT303E - MSc Respiratory Medicine FT304E - MSc Respiratory Medicine PT3231 - Master of Public Health FT4210 - PGCert Public Health PT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)481A - MSc Health Economi Economet FT482A - PGDip Health Econo Economet FT6706 - PGDip Public Health FT693B - PGCert Public Health FT733H - MSc Prim Care Rese &amp; Leader FT8003 - PGCert Public Health (Flex)808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex814C - PGCert Pub Health (Glo Hea) FT815C - PGCert Pub Health (Glo Hea) PT871H - PGDip Prim Care Res &amp; Lead FT872H - PGDip Prim Care Res &amp; Lead PT9963 - MPH (SEAL) PT9965 - MPH (SEAL) Flex</v>
       </c>
       <c r="T7" t="str">
         <v/>
       </c>
       <c r="U7" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="V7" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="W7" t="str">
-        <v>UoB Campus Edgbaston</v>
+        <v>Birmingham</v>
       </c>
       <c r="X7" t="str">
         <v>B</v>
       </c>
       <c r="Y7" t="str">
-        <v>n/a</v>
+        <v/>
       </c>
       <c r="Z7">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="AA7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AB7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -1388,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="AE7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AF7">
         <v>0</v>
@@ -1403,114 +1403,114 @@
         <v>0</v>
       </c>
       <c r="AJ7">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="AK7">
         <v>0</v>
       </c>
       <c r="AL7" t="str">
-        <v>Industry is rapidly changing to adjust to a range of complex and often conflicting needs while aiming to maximize a range of benefits. Understanding of optimisation techniques and the tools necessary to undertake analysis of these situations is important. &lt;br&gt;&lt;br&gt;The module will consider some general aspects of process optimisation and then look specifically at PetroChemical applications particularly the main unit operations associated with transforming crude oil to gasoline.</v>
+        <v>The module takes the planning cycle used in many health care systems as its focus (called the commissioning cycle in UK health services). It will introduce students to the three key areas of planning, procuring and monitoring health care services. The module is underpinned by teaching on the critical appraisal of evidence and the use of economic appraisal in health settings. Particular emphasis is placed on healthcare needs assessment and the ways in which this can be carried out. Students are exposed in particular to these concepts as they apply to health care delivery. The module is delivered by a mixture of internal academic experts and external experts experienced in service delivery.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AM7" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Understand and carry out key calculations associated with the main unit operations of a typical PetroChemical process.&lt;/li&gt;&lt;li&gt;Use optimisation and other process and system analysis to make suitably informed and justified decisions on refinery (PetroChemical) processes.&lt;/li&gt;&lt;li&gt;Select and use suitable optimisation techniques in a process (associated with the Chemical/Energy industry sector).&lt;/li&gt;&lt;/ul&gt;</v>
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Describe the planning cycle in the context of the provision and funding of health care&lt;/li&gt;&lt;li&gt;Demonstrate an understanding of the principles and practice of health care needs assessment and its application in public health practice&lt;/li&gt;&lt;li&gt;Demonstrate an understanding of the principles of economic appraisal of health care&lt;/li&gt;&lt;li&gt;Critically analyse health care policy implementation, in particular through the prioritisation of services and interventions&lt;/li&gt;&lt;li&gt;Demonstrate an understanding of and be able to analyse critical steps in service design or redesign such as service specifications, care pathways and models of care&lt;/li&gt;&lt;li&gt;Evaluate and audit health services to assure and improve quality&lt;/li&gt;&lt;li&gt;Demonstrate practical skills in the planning of health services, implementing changes in health services, and in the evaluation and quality improvement of health services.&lt;/li&gt;&lt;/ul&gt;</v>
       </c>
       <c r="AN7" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Chemical Engineering* (if applicable)Choose an item.BXPetrochemical Engineering and Process Optimisation`2027/28¬¬ for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFNew programme BEng/MEng in Energy Engineering This module is to combine aspects of two existing 10 credits modules, 04 26504 Petrochemical Engineering and 04 26506 Plant Optimisation, into one 20 credit module.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)Additional resources are not anticipated, as this module will replace existing modules in the School. SFAre there any related programme paperwork? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?Yes. New programme proposalB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryn/a. part of new programme and rolled out to existing cohorts on UG provisionQIf the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)n/aQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Accreditation to be sought from the Energy Institute once programme is running and the IChemEQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsN/aQWill the change fit into the partial block structure timetabling approach?                                                                                                                                 N/AIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.It is replacing two existing 10 credits with one 20 credit.8ApprovalSchoolDate: 03/12/2024Approving body: School Programmes and Modules Committee, Chair’s actionsCollege (mandatory for proposals only)Date: 13/12/2024Approving body: CQAACModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Chemical Engineering[Choose an item.] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)ʓPetrochemical Engineering and Process Optimisation#TBC=Honours - LH@20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.ﱙAs a compulsory module (i.e. every student in the year should be ǕAs an optional module (including any information about its grouping, if relevant):B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) UG in Chemical Engineering (all variants)À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Án/a☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicablen/aÂn/aÃUoB Campus EdgbastonÄÄ on how your School /Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe School is committed to ensuring an inclusive curriculum and actively promotes equality of opportunity to all. The School adheres to all Student Support agreements. There are no barriers to registration for this module when selected as part of the relevant programme offering.The module will seek to promote equality of opportunity through ensuring that no barriers are posed to students who would like to participate.  The module will also seek to ensure there are no barriers to students progressing through it.Scrutiny of EDI issues will be explicitly carried out by Education Committee within the School.Q Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).The module and programme are based on sustainability.This module is directly linked to the Education for Sustainability. In the context of energy transitions, it is directly linked to a number of Sustainable Development Goals, SDG 7 Affordable and Clean energy, SDG 12 Responsible Consumption and Production, and SDG 13 Climate Action.SFÅn/aÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç38È 10É10ꮛꮜ0ꮝ10ꮞꮟꮠꮡꮢ132ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥIndustry is rapidly changing to adjust to a range of complex and often conflicting needs while aiming to maximize a range of benefits.  Understanding of optimisation techniques and the tools necessary to undertake analysis of these situations is important. The module will consider some general aspects of process optimisation and then look specifically at PetroChemical applications particularly the main unit operations associated with transforming crude oil to gasoline.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Understand and carry out key calculations associated with the main unit operations of a typical PetroChemical process.Use optimisation and other process and system analysis to make suitably informed and justified decisions on refinery (PetroChemical) processes.Select and use suitable optimisation techniques in a process (associated with the Chemical/Energy industry sector).ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.Is this a module proposal or modification?Module ModificationIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running!School of Health Sciences* (if applicable)Applied Health SciencesXLM Healthcare Public Health (37682)`2026/27¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  Removal of 10 credit modules was required by College. On review and discussion with module leads, it was apparent that this module already provided sufficient teaching and depth of coverage for a 20-credit module, but there was an opportunity to expand the practical application of skills provided by the module (reflected in the additional learning outcome and group task assessment). Inclusion of classroom-based assessment and a group-submission will also be a positive step to ensuring the module assessment remains robust in the context of generative AI technologies.The new fee for the microcredential version (406I) will be: Home: Ladder Point 1 = £1260 for a 20 credit moduleOverseas: Ladder Point GT3a = £3380 for a 20 credit modulePlease describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)NoneAre there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessarySee comments in the Programme Modification form, which apply to a set of changes to individual modules (change from 10 to 20 credits).If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)Not applicableIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Not applicableIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsNot applicableWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 08/09/2025Approving body: Prof Louise Jackson, Joint School Head of EducationCollege (mandatory for proposals only)Date: Click here to enter a date.Approving body:Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Health Sciences[Applied Health Sciences] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ LM Healthcare Public Health#37682Equivalent modules: =LM@ 20$, if relevant⸮Semester 1ﱙ please state how frequently and when they will be delivered.Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ406I - PG MC Healthcare Pub Health FTAs an optional module (including any information about its grouping, if relevant):1778 - PGDip Public Health PT1779 - Master of Public Health PT197B - MSc Health Research Meth Flex198B - PGDip Health Research Meth FT199B - PGDip Health Research Meth PT200B - PGDip Health Research Met Flex201B - PGCert Health Research Meth FT202B - PGCert Health Research Meth PT203B - PGCert Health Resear Meth Flex215E - Master of Public Health (I) FT290A - MPH (SEAL) 15 month299E - PGDip Respiratory Medicine FT300E - PGDip Respiratory Medicine PT303E - MSc Respiratory Medicine FT304E - MSc Respiratory Medicine PT3231 - Master of Public Health FT4210 - PGCert Public Health PT4616 - Master of Public Health (Flex)4638 - Dip Public Health (Flex)481A - MSc Health Economi Economet FT482A - PGDip Health Econo Economet FT6706 - PGDip Public Health FT693B - PGCert Public Health FT733H - MSc Prim Care Rese &amp; Leader FT8003 - PGCert Public Health (Flex)808C - MPH (Global Health) FT809C - MPH (Global Health) PT810C - MPH (Global Health) Flex811C - PGDip Pub Health (Glob Hea) FT812C - PGDip Pub Health (Glob Hea) PT813C - PGDip Pub Heal (Glob Hea) Flex814C - PGCert Pub Health (Glo Hea) FT815C - PGCert Pub Health (Glo Hea) PT871H - PGDip Prim Care Res &amp; Lead FT872H - PGDip Prim Care Res &amp; Lead PT9963 - MPH (SEAL) PT9965 - MPH (SEAL) FlexÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:Choose an item.13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Á☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableÂÃBirminghamÄComment briefly on how your School/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupPlease briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).ÅÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. Ç30È 0É0ꮛ0ꮜ0ꮝ0ꮞ0ꮟ0ꮠ0ꮡ0ꮢ 170ꮣ0ꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThe module takes the planning cycle used in many health care systems as its focus (called the commissioning cycle in UK health services).  It will introduce students to the three key areas of planning, procuring and monitoring health care services.  The module is underpinned by teaching on the critical appraisal of evidence and the use of economic appraisal in health settings.  Particular emphasis is placed on healthcare needs assessment and the ways in which this can be carried out.  Students are exposed in particular to these concepts as they apply to health care delivery.  The module is delivered by a mixture of internal academic experts and external experts experienced in service delivery.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:21.1Describe the planning cycle in the context of the provision and funding of health care21.2Demonstrate an understanding of the principles and practice of health care needs assessment and its application in public health practice21.3Demonstrate an understanding of the principles of economic appraisal of health care21.4Critically analyse health care policy implementation, in particular through the prioritisation of services and interventions21.5Demonstrate an understanding of and be able to analyse critical steps in service design or redesign such as service specifications, care pathways and models of care21.6Evaluate and audit health services to assure and improve quality21.7Demonstrate practical skills in the planning of health services, implementing changes in health services, and in the evaluation and quality improvement of health services.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
       </c>
       <c r="AO7" t="str">
-        <v>&lt;br&gt;&lt;br&gt;Computer based Class test (50%) 2 hrs&lt;br&gt;&lt;br&gt;Unseen Written exam (50%), 2 hrs&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+        <v>&lt;br&gt;Assessment:&lt;br&gt;1. Assignment of 2,500 words (50%)&lt;br&gt;2. Group project: structured group-work, reflection and group report (50%)&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AP7" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="AQ7" t="str">
-        <v>Summer Exam Period</v>
+        <v>N/A – not examined</v>
       </c>
       <c r="AR7" t="str">
-        <v>n/a</v>
+        <v>N/A</v>
       </c>
       <c r="AS7" t="str">
-        <v>&lt;br&gt;Retake of failed components.</v>
+        <v>Resubmission of failed component(s), i.e. an amended 2,500 word assignment and/or revised group assignment, both following individualised feedback.&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AT7" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Computer based Class test (50%) 2 hrs&lt;br&gt;&lt;br&gt;Unseen Written exam (50%), 2 hrs&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Retake of failed components.</v>
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Assessment:&lt;br&gt;1. Assignment of 2,500 words (50%)&lt;br&gt;2. Group project: structured group-work, reflection and group report (50%)&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of failed component(s), i.e. an amended 2,500 word assignment and/or revised group assignment, both following individualised feedback.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AU7" t="str">
-        <v>Semester 2</v>
+        <v>Semester 1</v>
       </c>
       <c r="AV7" t="str">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AW7" t="str">
-        <v>Prof Bushra Al-Duri</v>
+        <v>Tom Marshall / Agnieszka Ignatowicz</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>January 2028</v>
+        <v>002027</v>
       </c>
       <c r="B8" t="str">
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="C8" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>Social Policy and Society</v>
       </c>
       <c r="D8" t="str">
-        <v>056</v>
+        <v/>
       </c>
       <c r="E8" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>Social Policy, Sociology and Criminology</v>
       </c>
       <c r="F8" t="str">
-        <v>013</v>
+        <v>262</v>
       </c>
       <c r="G8" t="str">
-        <v>13</v>
+        <v/>
       </c>
       <c r="H8" t="str">
-        <v>Process Design Exercise</v>
+        <v>Health and Cultures of Healing: Global Perspectives</v>
       </c>
       <c r="I8" t="str">
-        <v>LI Process Design Exercise</v>
+        <v>LM He &amp; Cul of Hea Gl Perspect</v>
       </c>
       <c r="J8" t="str">
-        <v>LI Process Design Exercise</v>
+        <v>LM Health and Cultures of Healing: Global Perspectives</v>
       </c>
       <c r="K8" t="str">
-        <v>TBC</v>
+        <v/>
       </c>
       <c r="L8" t="str">
-        <v>LI</v>
+        <v>LM</v>
       </c>
       <c r="M8" t="str">
         <v>20</v>
       </c>
       <c r="N8" t="str">
-        <v>UG</v>
+        <v>GT</v>
       </c>
       <c r="O8" t="str">
         <v>Z</v>
       </c>
       <c r="P8" t="str">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="Q8" t="str">
-        <v>H810</v>
+        <v>L400</v>
       </c>
       <c r="R8" t="str">
-        <v>100143</v>
+        <v>100502</v>
       </c>
       <c r="S8" t="str">
-        <v>part of new programme proposalB.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant): n/a</v>
+        <v>As an optional module (including any information about its grouping, if relevant):MA Sociology 571DMA Social Policy 2227/2228MA Global Public Policy 979DMA Global Criminology and Criminal Justice 877IMSc Health Care Policy and Management 2355/2356MA Culture, Power and Citizenship (programme proposed for 2027/28)</v>
       </c>
       <c r="T8" t="str">
         <v/>
       </c>
       <c r="U8" t="str">
-        <v>Year 1 Chemical Engineering or Year 1 Energy Engineering would need to be successfully passed.</v>
+        <v>N/A</v>
       </c>
       <c r="V8" t="str">
-        <v>none</v>
+        <v>N/A</v>
       </c>
       <c r="W8" t="str">
         <v>UoB Campus Edgbaston</v>
@@ -1519,13 +1519,13 @@
         <v>B</v>
       </c>
       <c r="Y8" t="str">
-        <v>n/a</v>
+        <v>N/A</v>
       </c>
       <c r="Z8">
-        <v>NaN</v>
+        <v>0</v>
       </c>
       <c r="AA8">
-        <v>NaN</v>
+        <v>20</v>
       </c>
       <c r="AB8">
         <v>0</v>
@@ -1537,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="AE8">
-        <v>NaN</v>
+        <v>0</v>
       </c>
       <c r="AF8">
         <v>0</v>
@@ -1552,37 +1552,37 @@
         <v>0</v>
       </c>
       <c r="AJ8">
-        <v>142</v>
+        <v>180</v>
       </c>
       <c r="AK8">
         <v>0</v>
       </c>
       <c r="AL8" t="str">
-        <v>The module is intended to emphasise the creative aspects of process design (for Chemical and Energy Engineers) and provide a link to simulation and computation to support with the delivery of a complex process design. It delivers the message that imagination and responsibility are essential attributes for successful professional engineers who are required to interface with many other business sectors.&lt;br&gt;&lt;br&gt;Working in groups, students use brainstorming techniques to generate ideas for new products and/or processes, while considering ethical, economic, and societal implications of proposed innovations. Each group then filters these ideas and develops one or more to the point of producing a business/development plan for its realisation.&lt;br&gt;&lt;br&gt;Groups are required to give attention to both commercial and ethical aspects of the project, and the engineering and process technology involved. As well as experiencing group operation in a broad, open-ended ideas generating environment, the students written and oral presentational skills and ethical reasoning capabilities are enhanced and tested.&lt;br&gt;&lt;br&gt;The module will also help to develop student skills in relevant software tools (e.g. Matlab, Excel, Python, AVEVA Pro II, AspenPlus) in generating quantitative values for processes to help with economic and other relevant analysis.</v>
+        <v>This interdisciplinary module explores diverse understandings of health, medicine, illness and healing across global contexts, and how culture shapes health and healing practices over time and space. Using embodied, reflective, and participatory learning, students will critically engage with healing traditions from ancient animist practices to contemporary medical pluralism. The module invites students to interrogate dominant biomedical paradigms and explore alternative and anti-colonial approaches to physical, mental, emotional, spiritual, and social wellbeing.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AM8" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Understand the circumstances which make the use of software design tools appropriate and necessary, and choose the appropriate tool for a given task&lt;/li&gt;&lt;li&gt;Solve engineering problems by programming/flowsheeting in the appropriate program&lt;/li&gt;&lt;li&gt;Understand how teams can operate effectively when addressing open-ended tasks requiring creative and entrepreneurial input.&lt;/li&gt;&lt;li&gt;Understand the importance of defining target customers, conducting market analysis, and consideration of intellectual property for engineering ventures.&lt;/li&gt;&lt;li&gt;Write a business plan, including finance and marketing strategy that can be defended ethically and in terms of health and safety&lt;/li&gt;&lt;li&gt;Use engineering skills and ethical reasoning to make a process/product with unique selling points that may be produced in a socially and environmentally beneficial way.&lt;/li&gt;&lt;/ul&gt;</v>
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Critically analyse diverse cultural and historical approaches to health and healing.&lt;/li&gt;&lt;li&gt;Reflect on personal and collective experiences of wellbeing through creative and embodied methods.&lt;/li&gt;&lt;li&gt;Co-create and present a multimedia project that connects personal health challenges with broader socio-cultural dynamics.&lt;/li&gt;&lt;li&gt;Engage in peer learning and provide/interpret constructive feedback to support collective and critical knowledge-building.&lt;/li&gt;&lt;/ul&gt;</v>
       </c>
       <c r="AN8" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Chemical Engineering* (if applicable)Choose an item.BXProcess Design Exercise`January 2028¬¬ for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFAlthough a new module proposal, in practice it will be a combination of two existing modules (Product Design Exercise 04 17128 and Computing for Chemical Engineers 04 33607) tweaked to be relevant to both Chemical Engineers and Energy Engineers.  It is required for the new Energy Engineering programme and the move to 20 credit modules.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)None (as in practice combining existing modules)SFAre there any related programme paperwork? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?Yes, there is a new Energy Engineering UG programme that this module proposal is part of.B Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryNone, required due to college request to develop programme and University request to move to 20 credit modules.QIf the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body IChemE – as combining existing content, no direct consultation is required.Energy Institute accreditation will be applied for once the programme is runningQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and Partnershipsn/aQWill the change fit into the partial block structure timetabling approach?                                                                                                                                 N/AIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.Chemical Engineering as it stands is not part of the partial block approach.  No significant impact expected with timetabling as replacing similar existing content.8ApprovalSchoolDate: 29/11/2024Approving body: Chairs action from School Education CommitteeCollege (mandatory for proposals only)Date: 13/12/2024Approving body: CQAACModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Chemical Engineering[Choose an item.] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)IChemEʓProcess Design Exercise#TBC=Intermediate - LI@20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.ﱙAs a compulsory module (i.e. every student in the year should be Ǖ part of new programme proposalB.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant): n/aÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁYear 1 Chemical Engineering or Year 1 Energy Engineering would need to be successfully passed.☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableNoneÂnoneÃUoB Campus EdgbastonÄÄ on how your School /Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe School is committed to ensuring an inclusive curriculum and actively promotes equality of opportunity to all. The School adheres to all Student Support agreements. There are no barriers to registration for this module when selected as part of the relevant programme offering.  The module will seek to promote equality of opportunity through ensuring that no barriers are posed to students who would like to participate.  The module will also seek to ensure there are no barriers to students progressing through it.  Scrutiny of EDI issues will be explicitly carried out by Education Committee within the School. Q Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).The whole Energy UG programme is based on principles of sustainability.SFÅn/aÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200 hoursB Q Ç20 hours (2 x 10 weeks)È 20 hours (2 x 10 weeks)Éꮛꮜꮝ18 hours (3 x 6 weeks) PC based classesꮞꮟꮠꮡꮢ142 hoursꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThe module is intended to emphasise the creative aspects of process design (for Chemical and Energy Engineers) and provide a link to simulation and computation to support with the delivery of a complex process design. It delivers the message that imagination and responsibility are essential attributes for successful professional engineers who are required to interface with many other business sectors.Working in groups, students use brainstorming techniques to generate ideas for new products and/or processes, while considering ethical, economic, and societal implications of proposed innovations. Each group then filters these ideas and develops one or more to the point of producing a business/development plan for its realisation.Groups are required to give attention to both commercial and ethical aspects of the project, and the engineering and process technology involved. As well as experiencing group operation in a broad, open-ended ideas generating environment, the students written and oral presentational skills and ethical reasoning capabilities are enhanced and tested.The module will also help to develop student skills in relevant software tools (e.g. Matlab, Excel, Python, AVEVA Pro II, AspenPlus) in generating quantitative values for processes to help with economic and other relevant analysis.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Understand the circumstances which make the use of software design tools appropriate and necessary, and choose the appropriate tool for a given taskSolve engineering problems by programming/flowsheeting in the appropriate programUnderstand how teams can operate effectively when addressing open-ended tasks requiring creative and entrepreneurial input.Understand the importance of defining target customers, conducting market analysis, and consideration of intellectual property for engineering ventures.Write a business plan, including finance and marketing strategy that can be defended ethically and in terms of health and safetyUse engineering skills and ethical reasoning to make a process/product with unique selling points that may be produced in a socially and environmentally beneficial way.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running!Social Policy and Society* (if applicable)Social Policy, Sociology and CriminologyXLM Health and Cultures of Healing: Global Perspectives`2027-28¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  This is being introduced as part of the review of the MA Sociology. Planning have identified that we are underrecruiting on this programme, and given our rise up the QS rankings for sociology, we feel that there is a strong case that if we can update and diversify the curriculum we can recruit more effectively from an international market. We offer an undergraduate LI ‘sociology of health and illness’ and LH ‘mental health and society’, so this module will extend and diversify this specialism at PGT level. It will have a strong cultural sociology theme, and so will also be suitable for our planned MA Culture, Power and Citizenship. It can also function as an attractive optional module for the MSc Health Care Policy and Management, MA Social Policy, MA Global Public Policy and MA Global Criminology and Criminal Justice.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)A module lead will be required (from existing resource). Due to the delivery methods, the module lead(s) would deliver all the content. (Capacity has been identified in existing workloads, and without detriment to other income-generating activity)Are there any related programme paperwork? (for proposals and significant module modifications)YesIf yes, have they been submitted for approval alongside this proposal?Yes7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryThe module represents an extension of choice on the current suite of MAs and does not affect existing provision. At UG HSMC have developed popular LI Sociology of Health and Illness and LI Mental Health and Society modules for sociology and JH students: this module extends and broadens that offer at LM.If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsN/AWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.8ApprovalSchoolDate: 28/11/2025Approving body: SEQCCollege (mandatory for proposals only)Date: 10/12/2025Approving body: CQAAC Chair’s ActionModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{Social Policy and Society[Social Policy, Sociology and Criminology] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ LM Health and Cultures of Healing: Global Perspectives#=Masters - LM@20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be ǕAs an optional module (including any information about its grouping, if relevant):MA Sociology 571DMA Social Policy 2227/2228MA Global Public Policy 979DMA Global Criminology and Criminal Justice 877IMSc Health Care Policy and Management 2355/2356MA Culture, Power and Citizenship (programme proposed for 2027/28) À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:Yes13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁN/A☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/AÂN/AÃ UoB Campus EdgbastonÄComment briefly on how your School/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe module will follow established School procedures for promoting transparent equality of access to and participation in the module, and pay due attention to EDB matters in design, delivery and assessment of the material. Oversight comes from standing School Education and EDB committees.Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).This interdisciplinary module directly addressesSDG 3 – Good health and wellbeing with a sustained examination of how we (historically and contemporaneously) understand these phenomena in diverse global contexts. In so doing, it also necessarily foregrounds issues of SDG10 – Reduced inequalities and, to a lesser extent (e.g. in specific case examples) SDG 6 – Clean water and sanitation.ÅN/AÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200 hoursÇÈ 20Éꮛꮜꮝꮞꮟꮠꮡꮢ180ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThis interdisciplinary module explores diverse understandings of health, medicine, illness and healing across global contexts, and how culture shapes health and healing practices over time and space. Using embodied, reflective, and participatory learning, students will critically engage with healing traditions from ancient animist practices to contemporary medical pluralism. The module invites students to interrogate dominant biomedical paradigms and explore alternative and anti-colonial approaches to physical, mental, emotional, spiritual, and social wellbeing.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Critically analyse diverse cultural and historical approaches to health and healing.Reflect on personal and collective experiences of wellbeing through creative and embodied methods.Co-create and present a multimedia project that connects personal health challenges with broader socio-cultural dynamics.Engage in peer learning and provide/interpret constructive feedback to support collective and critical knowledge-building.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
       </c>
       <c r="AO8" t="str">
-        <v>&lt;br&gt;80% coursework &lt;br&gt;(40% individual report (2000 words), 30% group presentation, 10% individual reflection exercise)&lt;br&gt;&lt;br&gt;20% class test (2 hr PC based set of exercises to complete).&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
+        <v>&lt;br&gt;Portfolio Project (3000 words) (80%)&lt;br&gt;Viva (15 mins) (20%) – discussing how learning and feedback on the module informed the portfolio project, including engagement with peer learning&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AP8" t="str">
         <v>No</v>
       </c>
       <c r="AQ8" t="str">
-        <v>Other (please state below)There is a class test, but this will be arranged by the school.</v>
+        <v>N/A - not examined</v>
       </c>
       <c r="AR8" t="str">
-        <v>none</v>
+        <v/>
       </c>
       <c r="AS8" t="str">
-        <v>&lt;br&gt;Resubmission of failed element(s) &lt;br&gt;Re-assessment of group work element (if required) will be replaced by a separate piece of written individual work&lt;br&gt;</v>
+        <v>Portfolio component – if failed, resubmitted in supplementary period to achieve pass standard.&lt;br&gt;&lt;br&gt;Viva component – if failed, in supplementary period submit a 1000-word reflection on how learning and feedback on the module informed the portfolio project (i.e. meets the objectives of the viva but in a written format).&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AT8" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;80% coursework &lt;br&gt;(40% individual report (2000 words), 30% group presentation, 10% individual reflection exercise)&lt;br&gt;&lt;br&gt;20% class test (2 hr PC based set of exercises to complete).&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission of failed element(s) &lt;br&gt;Re-assessment of group work element (if required) will be replaced by a separate piece of written individual work&lt;br&gt;</v>
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Portfolio Project (3000 words) (80%)&lt;br&gt;Viva (15 mins) (20%) – discussing how learning and feedback on the module informed the portfolio project, including engagement with peer learning&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Portfolio component – if failed, resubmitted in supplementary period to achieve pass standard.&lt;br&gt;&lt;br&gt;Viva component – if failed, in supplementary period submit a 1000-word reflection on how learning and feedback on the module informed the portfolio project (i.e. meets the objectives of the viva but in a written format).&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AU8" t="str">
         <v>Semester 2</v>
@@ -1591,75 +1591,75 @@
         <v>6</v>
       </c>
       <c r="AW8" t="str">
-        <v>Dr Tom Robinson</v>
+        <v>Prof Nicola Gale</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2026/27</v>
+        <v>002027</v>
       </c>
       <c r="B9" t="str">
-        <v>04</v>
+        <v>08</v>
       </c>
       <c r="C9" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>Social Policy and Society</v>
       </c>
       <c r="D9" t="str">
-        <v>056</v>
+        <v/>
       </c>
       <c r="E9" t="str">
-        <v>School of Chemical Engineering</v>
+        <v>Social Policy, Sociology and Criminology</v>
       </c>
       <c r="F9" t="str">
-        <v>013</v>
+        <v>262</v>
       </c>
       <c r="G9" t="str">
-        <v>13</v>
+        <v/>
       </c>
       <c r="H9" t="str">
-        <v>Science for Energy Engineering 1</v>
+        <v>Advanced Studies in the Sociology of Gender</v>
       </c>
       <c r="I9" t="str">
-        <v>LC Scien fo Energ Engineerin 1</v>
+        <v>LM Adva Stu in th Socio of Gen</v>
       </c>
       <c r="J9" t="str">
-        <v>LC Science for Energy Engineering 1</v>
+        <v>LM Advanced Studies in the Sociology of Gender</v>
       </c>
       <c r="K9" t="str">
-        <v>TBC</v>
+        <v/>
       </c>
       <c r="L9" t="str">
-        <v>LC</v>
+        <v>LM</v>
       </c>
       <c r="M9" t="str">
         <v>20</v>
       </c>
       <c r="N9" t="str">
-        <v>UG</v>
+        <v>GT</v>
       </c>
       <c r="O9" t="str">
         <v>Z</v>
       </c>
       <c r="P9" t="str">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="Q9" t="str">
-        <v>H810</v>
+        <v>L400</v>
       </c>
       <c r="R9" t="str">
-        <v>100143</v>
+        <v>100502</v>
       </c>
       <c r="S9" t="str">
-        <v>B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant):</v>
+        <v>N/AAs an optional module (including any information about its grouping, if relevant): MA Sociology 571DMA Global Criminology and Criminal Justice 877IMA Social Policy 2227/2228MA Global Public Policy 979DMA in Culture, Power and Citizenship (programme proposed for 2027/28 launch).</v>
       </c>
       <c r="T9" t="str">
         <v/>
       </c>
       <c r="U9" t="str">
-        <v>n/a</v>
+        <v>N/A</v>
       </c>
       <c r="V9" t="str">
-        <v>n/a</v>
+        <v>N/A</v>
       </c>
       <c r="W9" t="str">
         <v>UoB Campus Edgbaston</v>
@@ -1668,16 +1668,16 @@
         <v>B</v>
       </c>
       <c r="Y9" t="str">
-        <v>n/a</v>
+        <v>N/A</v>
       </c>
       <c r="Z9">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="AA9">
-        <v>15</v>
+        <v>NaN</v>
       </c>
       <c r="AB9">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -1698,40 +1698,40 @@
         <v>0</v>
       </c>
       <c r="AI9">
-        <v>0</v>
+        <v>NaN</v>
       </c>
       <c r="AJ9">
-        <v>140</v>
+        <v>NaN</v>
       </c>
       <c r="AK9">
         <v>0</v>
       </c>
       <c r="AL9" t="str">
-        <v>The module will introduce key research areas in the Energy area and explain the role of the underpinning engineering science required to be able to investigate these topics.&lt;br&gt;&lt;br&gt;Areas will include&lt;br&gt;Mechanics (e.g. work, power and energy, momentum, section analysis)&lt;br&gt;Thermodynamics (e.g. zeroth, first and second laws, Heat Engines and thermodynamic cycles)&lt;br&gt;Electrical Systems (e.g. basic analogue and digital circuits, magnetic fields, DC motors, three phase)&lt;br&gt;</v>
+        <v>What is gender? How does gender shape the social world we live in? In what ways are gender and power&lt;br&gt;relations constructed, reproduced, contested, and challenged in social interactions and within institutions? In&lt;br&gt;this module, we will examine these fundamental questions of feminist sociology through a series of empirical&lt;br&gt;case studies, while exploring the different methodological approaches feminist sociologists have used to&lt;br&gt;address these questions. Students will read and engage with both classic works that have been central to&lt;br&gt;the development of feminist sociology, as well as contemporary scholarship that represents the state-of-the-art in major substantive topics within the sociology of gender. &lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AM9" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Demonstrate knowledge and understanding of principles of mechanics and methodology necessary to underpin their education in mechanics, to enable appreciation of its scientific and engineering context and to support their understanding of future developments and technologies.&lt;/li&gt;&lt;li&gt;Explain using mathematical arguments the origin and nature of the physical laws and design rules required for the analysis and design of analogue and digital circuits and electrical machines.&lt;/li&gt;&lt;li&gt;Demonstrate knowledge and understanding of thermodynamic, mechanic and electrical principles necessary to underpin their education in related engineering disciplines and to enable them to apply mathematical methods, tools and notations proficiently in the analysis and solution of engineering problems.&lt;/li&gt;&lt;/ul&gt;</v>
+        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Apply core theoretical perspectives in feminist sociology to a range of substantive areas.&lt;/li&gt;&lt;li&gt;Identify the interactional processes and mechanisms through which gender difference and inequality are (re)produced and challenged.&lt;/li&gt;&lt;li&gt;Critically evaluate contemporary feminist scholarship both theoretically and methodologically.&lt;/li&gt;&lt;li&gt;Acquire the theoretical and empirical tools to be able to develop their own future research/practice in the analysis of gender.&lt;/li&gt;&lt;/ul&gt;</v>
       </c>
       <c r="AN9" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Chemical Engineering* (if applicable)Choose an item.BXScience for Energy Engineering 1`2026/27¬¬ for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFNew module relevant specifically to Energy Engineers to understand the underpinning physical and engineering science.  It is required for the new Energy Engineering programme and builds as a theme throughout Years 1-3, providing the fundamental principles on which the rest of the course rests.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)The module will be new and will have a staff load implications, however recent expansion of the energy theme related staff was made in part due to the expectation that specific energy theme related teaching would be required to expand the taught student numbers in this area.SFAre there any related programme paperwork? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?Yes. New programme proposalB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryn/a. part of new programmeQIf the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)n/aQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Accreditation to be sought from the Energy Institute once programme is running. QIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsN/aQWill the change fit into the partial block structure timetabling approach?                                                                                                                                 N/AIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.The expectation is that this would track the reaction and thermodynamics theme within Chemical engineering (other year 1 modules are shared with the Chem Eng programme).  So there will be a requirement to be able to house the module in a room.8ApprovalSchoolDate: 03/12/2024Approving body: School Programmes and Modules Committee, Chair’s actionsCollege (mandatory for proposals only)Date: 13/12/2024Approving body: CQAACModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Chemical Engineering[Choose an item.] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)ʓScience for Energy Engineering 1#TBC=Certificate - LC@20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.ﱙAs a compulsory module (i.e. every student in the year should be ǕB.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Án/a☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicablen/aÂn/aÃUoB Campus EdgbastonÄÄ on how your School /Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe School is committed to ensuring an inclusive curriculum and actively promotes equality of opportunity to all. The School adheres to all Student Support agreements. There are no barriers to registration for this module when selected as part of the relevant programme offering.The module will seek to promote equality of opportunity through ensuring that no barriers are posed to students who would like to participate.  The module will also seek to ensure there are no barriers to students progressing through it.Scrutiny of EDI issues will be explicitly carried out by Education Committee within the School.Q Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).The module and programme are based on sustainability.This module is directly linked to the Education for Sustainability. In the context of energy transitions, it is directly linked to a number of Sustainable Development Goals, SDG 7 Affordable and Clean energy, SDG 12 Responsible Consumption and Production, and SDG 13 Climate Action.SFÅn/aÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç25È 15É20ꮛꮜꮝꮞꮟꮠꮡꮢ140ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThe module will introduce key research areas in the Energy area and explain the role of the underpinning engineering science required to be able to investigate these topics.Areas will includeMechanics (e.g. work, power and energy, momentum, section analysis)Thermodynamics (e.g. zeroth, first and second laws, Heat Engines and thermodynamic cycles)Electrical Systems (e.g. basic analogue and digital circuits, magnetic fields, DC motors, three phase)ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Demonstrate knowledge and understanding of principles of mechanics and methodology necessary to underpin their education in mechanics, to enable appreciation of its scientific and engineering context and to support their understanding of future developments and technologies.Explain using mathematical arguments the origin and nature of the physical laws and design rules required for the analysis and design of analogue and digital circuits and electrical machines.Demonstrate knowledge and understanding of thermodynamic, mechanic and electrical principles necessary to underpin their education in related engineering disciplines and to enable them to apply mathematical methods, tools and notations proficiently in the analysis and solution of engineering problems.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
+        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running!Social Policy and Society* (if applicable)Social Policy, Sociology and CriminologyXLM Advanced Studies in the Sociology of Gender`2027–28 (Semester 2)¬Rationale for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  The sociology of gender is one of the largest subfields in contemporary sociology. But currently, there is no module on the topic of gender in SPSC at the PGT level, and this is a striking omission in our MA Sociology offer in particular. Considering that the School is also proposing to launch an MA in Culture, Power and Citizenship for 2027/28, a new module on “Advanced Studies in the Sociology of Gender” will not only enhance our MA Sociology (and Social Policy and Criminology) offer, but also contribute to the proposed new MA.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)The module will be staffed from within current capacity in SPSC. The staff members have capacity and there is no displacement of other income activity. Given gender is a core topic across multiple disciplines, significant additional library resource is not envisaged. Are there any related programme paperwork? (for proposals and significant module modifications)NoIf yes, have they been submitted for approval alongside this proposal?N/A7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryWe have not consulted directly with students on this, but our LI gender module is consistently the most popular in SPSC, with regular recruitment of over 150 students, indicating the strong demand in this sub-field. There is currently a gap at PGT with no offer in gender, and this weakens our overall offer for prospective PGT students (including our own UG students who are looking to continue their studies). If the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AIf the module/programme is subject to accreditation, please provide details of consultation with the professional body N/AIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsN/AWill the change fit into the partial block structure timetabling approach?                                                                                                                                 YesIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.N/A8ApprovalSchoolDate: 28/11/2025Approving body: SEQCCollege (mandatory for proposals only)Date: 10/12/2025Approving body: CQAAC Chair’s Action Module SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{Social Policy and Society[Social Policy, Sociology and Criminology] in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:Is this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:Accrediting body (if applicable)ʓ Advanced Studies in the Sociology of Gender#=Masters - LM@20$, if relevantN/A⸮Semester 2ﱙ please state how frequently and when they will be delivered.Programmes on which the module is available (please state the programme title and code)As a compulsory module (i.e. every student in the year should be Ǖ N/AAs an optional module (including any information about its grouping, if relevant): MA Sociology 571DMA Global Criminology and Criminal Justice 877IMA Social Policy 2227/2228MA Global Public Policy 979DMA in Culture, Power and Citizenship (programme proposed for 2027/28 launch).À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:Yes13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁN/A☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableN/AÂN/AÃ UoB Campus EdgbastonÄComment briefly on how your School/Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe module will follow School procedures for promoting transparent equality of access to the module, and pay due attention to EDB matters in design, delivery and assessment of the material. Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).Because this module will examine topics such as gender inequality, patriarchy, and heteronormativity through a sociological lens, it is well-aligned with SDG5: Gender Equality and SDDG10: Reduced Inequality.ÅN/AÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. Çs: 10 hoursÈs: 9 hoursꮢ: 181 hoursTotal: 200 hoursLecture10 Seminar 9É0ꮛ0ꮜ0ꮝ0ꮞ0ꮟ0ꮠ0ꮡ0Guided independent study181ꮣ0ꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥWhat is gender? How does gender shape the social world we live in? In what ways are gender and powerrelations constructed, reproduced, contested, and challenged in social interactions and within institutions? Inthis module, we will examine these fundamental questions of feminist sociology through a series of empiricalcase studies, while exploring the different methodological approaches feminist sociologists have used toaddress these questions. Students will read and engage with both classic works that have been central tothe development of feminist sociology, as well as contemporary scholarship that represents the state-of-the-art in major substantive topics within the sociology of gender. ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Apply core theoretical perspectives in feminist sociology to a range of substantive areas.Identify the interactional processes and mechanisms through which gender difference and inequality are (re)produced and challenged.Critically evaluate contemporary feminist scholarship both theoretically and methodologically.Acquire the theoretical and empirical tools to be able to develop their own future research/practice in the analysis of gender.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
       </c>
       <c r="AO9" t="str">
-        <v>&lt;br&gt;&lt;br&gt;Class test (20%) 1 hr&lt;br&gt;&lt;br&gt;Unseen Written exam (80%), 3 hrs &lt;br&gt;&lt;br&gt;</v>
+        <v>&lt;br&gt;&lt;br&gt;40%: 1000-word critical response piece in the form of EITHER i) a book review of a recent book publication in gender studies OR ii) a gender-focused response to a cultural artefact (e.g. film, exhibition, advertising campaign).&lt;br&gt;&lt;br&gt;60%: 2,500-word analysis in the form of either i) critical academic essay (chosen from topics provided) OR ii) a gender-focused piece of policy analysis. &lt;br&gt;&lt;br&gt;For all assessments, key literature and concepts from the module must be drawn on. &lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AP9" t="str">
-        <v>Yes</v>
+        <v>N/A - not examined</v>
       </c>
       <c r="AQ9" t="str">
-        <v>Summer Exam Period</v>
+        <v>N/A - not examined</v>
       </c>
       <c r="AR9" t="str">
-        <v>n/a</v>
+        <v>N/A</v>
       </c>
       <c r="AS9" t="str">
-        <v>Supplementary exam (100%, unseen 3 hrs)</v>
+        <v>Students will be able to resubmit failed components in the supplementary period.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AT9" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Class test (20%) 1 hr&lt;br&gt;&lt;br&gt;Unseen Written exam (80%), 3 hrs &lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Supplementary exam (100%, unseen 3 hrs)</v>
+        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;40%: 1000-word critical response piece in the form of EITHER i) a book review of a recent book publication in gender studies OR ii) a gender-focused response to a cultural artefact (e.g. film, exhibition, advertising campaign).&lt;br&gt;&lt;br&gt;60%: 2,500-word analysis in the form of either i) critical academic essay (chosen from topics provided) OR ii) a gender-focused piece of policy analysis. &lt;br&gt;&lt;br&gt;For all assessments, key literature and concepts from the module must be drawn on. &lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Students will be able to resubmit failed components in the supplementary period.&lt;br&gt;&lt;br&gt;</v>
       </c>
       <c r="AU9" t="str">
         <v>Semester 2</v>
@@ -1740,459 +1740,12 @@
         <v>6</v>
       </c>
       <c r="AW9" t="str">
-        <v>Dr Renaldi Renaldi</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>2027/28</v>
-      </c>
-      <c r="B10" t="str">
-        <v>04</v>
-      </c>
-      <c r="C10" t="str">
-        <v>School of Chemical Engineering</v>
-      </c>
-      <c r="D10" t="str">
-        <v>056</v>
-      </c>
-      <c r="E10" t="str">
-        <v>School of Chemical Engineering</v>
-      </c>
-      <c r="F10" t="str">
-        <v>013</v>
-      </c>
-      <c r="G10" t="str">
-        <v>13</v>
-      </c>
-      <c r="H10" t="str">
-        <v>Science for Energy Engineering 2</v>
-      </c>
-      <c r="I10" t="str">
-        <v>LI Scien fo Energ Engineerin 2</v>
-      </c>
-      <c r="J10" t="str">
-        <v>LI Science for Energy Engineering 2</v>
-      </c>
-      <c r="K10" t="str">
-        <v>TBC</v>
-      </c>
-      <c r="L10" t="str">
-        <v>LI</v>
-      </c>
-      <c r="M10" t="str">
-        <v>20</v>
-      </c>
-      <c r="N10" t="str">
-        <v>UG</v>
-      </c>
-      <c r="O10" t="str">
-        <v>Z</v>
-      </c>
-      <c r="P10" t="str">
-        <v>116</v>
-      </c>
-      <c r="Q10" t="str">
-        <v>H810</v>
-      </c>
-      <c r="R10" t="str">
-        <v>100143</v>
-      </c>
-      <c r="S10" t="str">
-        <v>B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant):</v>
-      </c>
-      <c r="T10" t="str">
-        <v/>
-      </c>
-      <c r="U10" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="V10" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="W10" t="str">
-        <v>UoB Campus Edgbaston</v>
-      </c>
-      <c r="X10" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y10" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="Z10">
-        <v>25</v>
-      </c>
-      <c r="AA10">
-        <v>15</v>
-      </c>
-      <c r="AB10">
-        <v>20</v>
-      </c>
-      <c r="AC10">
-        <v>0</v>
-      </c>
-      <c r="AD10">
-        <v>0</v>
-      </c>
-      <c r="AE10">
-        <v>0</v>
-      </c>
-      <c r="AF10">
-        <v>0</v>
-      </c>
-      <c r="AG10">
-        <v>0</v>
-      </c>
-      <c r="AH10">
-        <v>0</v>
-      </c>
-      <c r="AI10">
-        <v>0</v>
-      </c>
-      <c r="AJ10">
-        <v>140</v>
-      </c>
-      <c r="AK10">
-        <v>0</v>
-      </c>
-      <c r="AL10" t="str">
-        <v>The module will build on Science for Energy Engineers 1, expanding and going further into the topics and research areas covered in year 1. This module will continue to use the same approach of introducing key research areas in the Energy area and explaining the role of the underpinning engineering science required to be able to investigate these topics.&lt;br&gt;&lt;br&gt;Areas will include&lt;br&gt;Mechanics (e.g. vector analysis of rigid body systems (mainly 2D), static analysis of stress)&lt;br&gt;Thermodynamics (e.g. ideal and actual power generation cycles)&lt;br&gt;Electrical Systems (e.g. AC/DC conversion and induction)&lt;br&gt;</v>
-      </c>
-      <c r="AM10" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Apply principles of power transfer and voltage control, and power systems&lt;/li&gt;&lt;li&gt;Demonstrate knowledge and understanding of the mathematical and scientific principles that underpin static analysis of stress in solid mechanics and vector analysis of the dynamics (both kinematics and kinetics) of two-dimensional rigid body systems.&lt;/li&gt;&lt;li&gt;Demonstrate the ability to use the results of mechanical, electrical and thermodynamic analysis to solve engineering problems and to recommend appropriate action.&lt;/li&gt;&lt;/ul&gt;</v>
-      </c>
-      <c r="AN10" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Chemical Engineering* (if applicable)Choose an item.BXScience for Energy Engineering 2`2027/28¬¬ for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFNew module relevant specifically to Energy Engineers to understand the underpinning physical and engineering science.  It is required for the new Energy Engineering programme and builds as a theme throughout Years 1-3, providing the fundamental principles on which the rest of the course rests.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)The module will be new and will have a staff load implication, however recent expansion of the energy theme related staff was made in part due to the expectation that specific energy theme related teaching would be required to expand the taught student numbers in this area.SFAre there any related programme paperwork? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?Yes. New programme proposalB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryn/a. part of new programmeQIf the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)n/aQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Accreditation to be sought from the Energy Institute once programme is running. QIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsN/aQWill the change fit into the partial block structure timetabling approach?                                                                                                                                 N/AIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.The expectation is that this would track the reaction and thermodynamics theme within Chemical engineering (other year 2 module are shared with the Chem Eng programme).  So there will be a requirement to be able to house the module in a room.8ApprovalSchoolDate: 03/12/2024Approving body: School Programmes and Modules Committee, Chair’s actionsCollege (mandatory for proposals only)Date: 13/12/2024Approving body: CQAACModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Chemical Engineering[Choose an item.] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)ʓScience for Energy Engineering 2#TBC=Intermediate - LI@20$, if relevant⸮Semester 2ﱙ please state how frequently and when they will be delivered.ﱙAs a compulsory module (i.e. every student in the year should be ǕB.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Án/a☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicablen/aÂn/aÃUoB Campus EdgbastonÄÄ on how your School /Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe School is committed to ensuring an inclusive curriculum and actively promotes equality of opportunity to all. The School adheres to all Student Support agreements. There are no barriers to registration for this module when selected as part of the relevant programme offering.The module will seek to promote equality of opportunity through ensuring that no barriers are posed to students who would like to participate.  The module will also seek to ensure there are no barriers to students progressing through it.Scrutiny of EDI issues will be explicitly carried out by Education Committee within the School.Q Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).The module and programme are based on sustainability.This module is directly linked to the Education for Sustainability. In the context of energy transitions, it is directly linked to a number of Sustainable Development Goals, SDG 7 Affordable and Clean energy, SDG 12 Responsible Consumption and Production, and SDG 13 Climate Action.SFÅn/aÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç25È 15É20ꮛꮜꮝꮞꮟꮠꮡꮢ140ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThe module will build on Science for Energy Engineers 1, expanding and going further into the topics and research areas covered in year 1. This module will continue to use the same approach of introducing key research areas in the Energy area and explaining the role of the underpinning engineering science required to be able to investigate these topics.Areas will includeMechanics (e.g. vector analysis of rigid body systems (mainly 2D), static analysis of stress)Thermodynamics (e.g. ideal and actual power generation cycles)Electrical Systems (e.g. AC/DC conversion and induction)ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Apply principles of power transfer and voltage control, and power systemsDemonstrate knowledge and understanding of the mathematical and scientific principles that underpin static analysis of stress in solid mechanics and vector analysis of the dynamics (both kinematics and kinetics) of two-dimensional rigid body systems.Demonstrate the ability to use the results of mechanical, electrical and thermodynamic analysis to solve engineering problems and to recommend appropriate action.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
-      </c>
-      <c r="AO10" t="str">
-        <v>&lt;br&gt;&lt;br&gt;Coursework: Year 2 portfolio work (20%) &lt;br&gt;&lt;br&gt;Unseen Written exam (80%), 3 hrs &lt;br&gt;&lt;br&gt;</v>
-      </c>
-      <c r="AP10" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="AQ10" t="str">
-        <v>Summer Exam Period</v>
-      </c>
-      <c r="AR10" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="AS10" t="str">
-        <v>Supplementary exam (unseen 3 hrs)</v>
-      </c>
-      <c r="AT10" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Coursework: Year 2 portfolio work (20%) &lt;br&gt;&lt;br&gt;Unseen Written exam (80%), 3 hrs &lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Supplementary exam (unseen 3 hrs)</v>
-      </c>
-      <c r="AU10" t="str">
-        <v>Semester 2</v>
-      </c>
-      <c r="AV10" t="str">
-        <v>6</v>
-      </c>
-      <c r="AW10" t="str">
-        <v>Dr Jian Song</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>2028/29</v>
-      </c>
-      <c r="B11" t="str">
-        <v>04</v>
-      </c>
-      <c r="C11" t="str">
-        <v>School of Chemical Engineering</v>
-      </c>
-      <c r="D11" t="str">
-        <v>056</v>
-      </c>
-      <c r="E11" t="str">
-        <v>School of Chemical Engineering</v>
-      </c>
-      <c r="F11" t="str">
-        <v>013</v>
-      </c>
-      <c r="G11" t="str">
-        <v>13</v>
-      </c>
-      <c r="H11" t="str">
-        <v>Science for Energy Engineering 3</v>
-      </c>
-      <c r="I11" t="str">
-        <v>LH Scien fo Energ Engineerin 3</v>
-      </c>
-      <c r="J11" t="str">
-        <v>LH Science for Energy Engineering 3</v>
-      </c>
-      <c r="K11" t="str">
-        <v>TBC</v>
-      </c>
-      <c r="L11" t="str">
-        <v>LH</v>
-      </c>
-      <c r="M11" t="str">
-        <v>20</v>
-      </c>
-      <c r="N11" t="str">
-        <v>UG</v>
-      </c>
-      <c r="O11" t="str">
-        <v>Z</v>
-      </c>
-      <c r="P11" t="str">
-        <v>116</v>
-      </c>
-      <c r="Q11" t="str">
-        <v>H810</v>
-      </c>
-      <c r="R11" t="str">
-        <v>100143</v>
-      </c>
-      <c r="S11" t="str">
-        <v>B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant):</v>
-      </c>
-      <c r="T11" t="str">
-        <v/>
-      </c>
-      <c r="U11" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="V11" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="W11" t="str">
-        <v>UoB Campus Edgbaston</v>
-      </c>
-      <c r="X11" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y11" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="Z11">
-        <v>25</v>
-      </c>
-      <c r="AA11">
-        <v>15</v>
-      </c>
-      <c r="AB11">
-        <v>20</v>
-      </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
-      </c>
-      <c r="AH11">
-        <v>0</v>
-      </c>
-      <c r="AI11">
-        <v>0</v>
-      </c>
-      <c r="AJ11">
-        <v>140</v>
-      </c>
-      <c r="AK11">
-        <v>0</v>
-      </c>
-      <c r="AL11" t="str">
-        <v>The module will build on Science for Energy Engineers 1 and 2, expanding and going further into the topics and research areas covered in years 1 and 2. This module will continue to use the same approach of introducing key research areas in the Energy area and explaining the role of the underpinning engineering science required to be able to investigate these topics&lt;br&gt;&lt;br&gt;Areas will include&lt;br&gt;Mechanics (e.g. dynamic analysis of systems, engine types and operation)&lt;br&gt;Thermodynamics (e.g. sustainable energy systems)&lt;br&gt;Electrical Systems (e.g. power conversion and distribution systems)&lt;br&gt;&lt;br&gt;</v>
-      </c>
-      <c r="AM11" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;Evaluate steady state performance and variable-speed operations of electrical machines.&lt;/li&gt;&lt;li&gt;Explain the techniques for operation and control of electrical power transmission &amp; distribution systems&lt;/li&gt;&lt;li&gt;Demonstrate knowledge and understanding of mathematical and scientific principles necessary to underpin the dynamics of systems.&lt;/li&gt;&lt;li&gt;Demonstrate knowledge and understanding of scientific principles and methodology necessary to underpin efficient and sustainable energy systems across the mechanical engineering discipline.&lt;/li&gt;&lt;/ul&gt;</v>
-      </c>
-      <c r="AN11" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Chemical Engineering* (if applicable)Choose an item.BXScience for Energy Engineering 3`2028/29¬¬ for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFNew module relevant specifically to Energy Engineers to understand the underpinning physical and engineering science.  It is required for the new Energy Engineering programme and builds as a theme throughout Years 1-3, providing the fundamental principles on which the rest of the course rests.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)The module will be new and will have a staff load implication, however recent expansion of the energy theme related staff was made in part due to the expectation that specific energy theme related teaching would be required to expand the taught student numbers in this area.SFAre there any related programme paperwork? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?Yes. New programme proposalB Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryn/a. part of new programmeQIf the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)n/aQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body Accreditation to be sought from the Energy Institute once programme is running. QIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and PartnershipsN/aQWill the change fit into the partial block structure timetabling approach?                                                                                                                                 N/AIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.The expectation is that this would track the reaction and thermodynamics theme within Chemical engineering (other year 3 modules are shared with the Chem Eng programme).  So there will be a requirement to be able to house the module in a room.8ApprovalSchoolDate: 03/12/2024Approving body: School Programmes and Modules Committee, Chair’s actionsCollege (mandatory for proposals only)Date: 13/12/2024Approving body: CQAACModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Chemical Engineering[Choose an item.] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)ʓScience for Energy Engineering 3#TBC=Honours - LH@20$, if relevant⸮Semester 1ﱙ please state how frequently and when they will be delivered.ﱙAs a compulsory module (i.e. every student in the year should be ǕB.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant):À(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, Án/a☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicablen/aÂn/aÃUoB Campus EdgbastonÄÄ on how your School /Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe School is committed to ensuring an inclusive curriculum and actively promotes equality of opportunity to all. The School adheres to all Student Support agreements. There are no barriers to registration for this module when selected as part of the relevant programme offering.The module will seek to promote equality of opportunity through ensuring that no barriers are posed to students who would like to participate.  The module will also seek to ensure there are no barriers to students progressing through it.Scrutiny of EDI issues will be explicitly carried out by Education Committee within the School.Q Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).The module and programme are based on sustainability.This module is directly linked to the Education for Sustainability. In the context of energy transitions, it is directly linked to a number of Sustainable Development Goals, SDG 7 Affordable and Clean energy, SDG 12 Responsible Consumption and Production, and SDG 13 Climate Action.SFÅn/aÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200B Q Ç25È 15É20ꮛꮜꮝꮞꮟꮠꮡꮢ140ꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThe module will build on Science for Energy Engineers 1 and 2, expanding and going further into the topics and research areas covered in years 1 and 2. This module will continue to use the same approach of introducing key research areas in the Energy area and explaining the role of the underpinning engineering science required to be able to investigate these topicsAreas will includeMechanics (e.g. dynamic analysis of systems, engine types and operation)Thermodynamics (e.g. sustainable energy systems)Electrical Systems (e.g. power conversion and distribution systems)ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:Evaluate steady‐state performance and variable-speed operations of electrical machines.Explain the techniques for operation and control of electrical power transmission &amp; distribution systemsDemonstrate knowledge and understanding of mathematical and scientific principles necessary to underpin the dynamics of systems.Demonstrate knowledge and understanding of scientific principles and methodology necessary to underpin efficient and sustainable energy systems across the mechanical engineering discipline.ꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
-      </c>
-      <c r="AO11" t="str">
-        <v>&lt;br&gt;&lt;br&gt;Class test (20%) 1 hr&lt;br&gt;&lt;br&gt;Unseen Written exam (80%), 3 hrs &lt;br&gt;&lt;br&gt;</v>
-      </c>
-      <c r="AP11" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="AQ11" t="str">
-        <v>Summer Exam Period</v>
-      </c>
-      <c r="AR11" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="AS11" t="str">
-        <v>Supplementary exam (unseen 3 hrs)</v>
-      </c>
-      <c r="AT11" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Class test (20%) 1 hr&lt;br&gt;&lt;br&gt;Unseen Written exam (80%), 3 hrs &lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Supplementary exam (unseen 3 hrs)</v>
-      </c>
-      <c r="AU11" t="str">
-        <v>Semester 1</v>
-      </c>
-      <c r="AV11" t="str">
-        <v>5</v>
-      </c>
-      <c r="AW11" t="str">
-        <v>Dr Tongtong Zhang</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>September 2027</v>
-      </c>
-      <c r="B12" t="str">
-        <v>04</v>
-      </c>
-      <c r="C12" t="str">
-        <v>School of Chemical Engineering</v>
-      </c>
-      <c r="D12" t="str">
-        <v>056</v>
-      </c>
-      <c r="E12" t="str">
-        <v>School of Chemical Engineering</v>
-      </c>
-      <c r="F12" t="str">
-        <v>013</v>
-      </c>
-      <c r="G12" t="str">
-        <v>13</v>
-      </c>
-      <c r="H12" t="str">
-        <v>Systems Design and Control</v>
-      </c>
-      <c r="I12" t="str">
-        <v>LI Systems Design &amp; Control</v>
-      </c>
-      <c r="J12" t="str">
-        <v>LI Systems Design and Control</v>
-      </c>
-      <c r="K12" t="str">
-        <v>TBC</v>
-      </c>
-      <c r="L12" t="str">
-        <v>LI</v>
-      </c>
-      <c r="M12" t="str">
-        <v>20</v>
-      </c>
-      <c r="N12" t="str">
-        <v>UG</v>
-      </c>
-      <c r="O12" t="str">
-        <v>Z</v>
-      </c>
-      <c r="P12" t="str">
-        <v>116</v>
-      </c>
-      <c r="Q12" t="str">
-        <v>H810</v>
-      </c>
-      <c r="R12" t="str">
-        <v>100143</v>
-      </c>
-      <c r="S12" t="str">
-        <v>B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant): n/a</v>
-      </c>
-      <c r="T12" t="str">
-        <v/>
-      </c>
-      <c r="U12" t="str">
-        <v>Year 1 Chemical Engineering or Year 1 Energy Engineering would need to be successfully passed.</v>
-      </c>
-      <c r="V12" t="str">
-        <v>none</v>
-      </c>
-      <c r="W12" t="str">
-        <v>UoB Campus Edgbaston</v>
-      </c>
-      <c r="X12" t="str">
-        <v>B</v>
-      </c>
-      <c r="Y12" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="Z12">
-        <v>NaN</v>
-      </c>
-      <c r="AA12">
-        <v>NaN</v>
-      </c>
-      <c r="AB12">
-        <v>NaN</v>
-      </c>
-      <c r="AC12">
-        <v>0</v>
-      </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
-      <c r="AE12">
-        <v>NaN</v>
-      </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
-      <c r="AG12">
-        <v>0</v>
-      </c>
-      <c r="AH12">
-        <v>0</v>
-      </c>
-      <c r="AI12">
-        <v>0</v>
-      </c>
-      <c r="AJ12">
-        <v>140</v>
-      </c>
-      <c r="AK12">
-        <v>0</v>
-      </c>
-      <c r="AL12" t="str">
-        <v>The module will develop the modelling and dynamic system analysis skills required for monitoring and control of complex systems. This will include both paper and software based techniques.&lt;br&gt;&lt;br&gt;The fundamentals of engineering system relevant measurements will be covered, along with the fundamentals of open and closed-loop control.&lt;br&gt;&lt;br&gt;Control aspects will then be extended to consider system stability, classical PID controller design, feedback block diagram analysis and practical aspects of industrial system control.&lt;br&gt;</v>
-      </c>
-      <c r="AM12" t="str">
-        <v>By the end of the module students should be able to:&lt;ul&gt;&lt;li&gt;appreciate the importance of control and the role of the control engineer particularly in safety critical systems.&lt;/li&gt;&lt;li&gt;comprehend the basic structure of control systems and how open- and closed-loop control is carried out and how the analysis and solution of dynamic models (particular linear 2nd order differential equations, particularly via Laplace Transforms techniques) is required.&lt;/li&gt;&lt;li&gt;describe typical industrial measurement system used for commonly measured and manipulated system variables.&lt;/li&gt;&lt;li&gt;understand fundamental control concepts, defining feedback and feed-forward modes of control and use relevant software and analytic tools (including Laplace Transforms and Simulink) to analyse&lt;/li&gt;&lt;/ul&gt;</v>
-      </c>
-      <c r="AN12" t="str">
-        <v>Form for Proposing or Modifying ModulesModule proposals and modifications should always be accompanied by a new or modified module specification (below) and completed with sight of the relevant guidance. If the module being proposed here is a new placement, the Proposal to Add a New Placement form must also be completed.The final column in the below forms indicates why the different items of information are required, using the following codes:B: Basic data used for information and programme modelling.Q: Quality assurance processes and considerations.SF: Alignment with the University’s strategic aims and/or the financial risk:reward of the development.Is this a module proposal or modification?Module ProposalIf ‘proposal’, please contact your Library Engagement Advisor to assess whether extra/new Library materials will be required to support the module. Additionally, once a new module is approved, please note that a Resource List should be created as soon as possible, and at least 2 months prior to the module running{School of Chemical Engineering* (if applicable)Choose an item.BXSystems Design and Control`September 2027¬¬ for proposal/modification of module, including why the proposal/modification is necessary. Please use this box to provide any additional detail about modifications, e.g. if changes are phased. To make changes to multiple modules please attach a specification for each module.  SFAlthough a new module proposal, in practice it will be a reworking of Process Systems and Principles of Process Control (0428467) tweaked to be relevant to both Chemical Engineers and Energy Engineers.  It is required for the new Energy Engineering programme and from a staffing (and content) perspective we need the 20 credits to work for both the Chemical Engineering ug and Energy engineering ug programmes.Please describe any resource implications (e.g. staffing/library resource, impact on income) (required for proposals)None (as in practice combining existing modules)SFAre there any related programme paperwork? (for proposals and significant module modifications)YesB QIf yes, have they been submitted for approval alongside this proposal?Yes, there is a new Energy Engineering UG programme that this module proposal is part of.B Q7Consultation (required for modifications, advised for proposals, where applicable)Please describe how, when, and with whom consultations occurred, and the outcomesProspective/existing students where necessaryNone, required due to college request to develop programme.QIf the module is/will be available to students from other Schools /Colleges, e.g. as part of a joint or integrated degree, and/or the Birmingham International Academy, and/or if there is a Dubai-based equivalent, please provide details of consultation with the relevant programme lead(s)N/AQIf the module/programme is subject to accreditation, please provide details of consultation with the professional body IChemE – as small change to existing content, no direct consultation is required.Energy Institute accreditation will be applied for once the programme is runningQIf the module is part of a collaborative arrangement, please provide details of consultation with the Head of Apprenticeships and Partnershipsn/aQWill the change fit into the partial block structure timetabling approach?                                                                                                                                 NoIf ‘No’, please state rationale here and contact Timetabling and Examinations for consultation:If the answer to 7.5 is ‘no, please confirm the details of the consultation with Timetabling and Examinations and whether it will have any significant impact on the integrity of the timetable.If it will cause a significant impact please provide details of the suggested alternative, impact, and future considerations, including details of the consultation with any impacted Schools who share the module.Chemical Engineering as it stands is not part of the partial block approach.  No significant impact expected with timetabling as replacing similar existing content.8ApprovalSchoolDate: 29/11/2024Approving body: Chairs action from School Education CommitteeCollege (mandatory for proposals only)Date: 13/12/2024Approving body: CQAACModule SpecificationThis form should be completed to accompany a module proposal form, or revised to accompany a module modification form by using tracked changes.{School of Chemical Engineering[Choose an item.] module delivered in collaboration with another organisation? NoIf ‘yes’ please state the organisation’s name:B Q SFIs this module to be delivered by more than one School at UoB?NoIf ‘yes’ state which Schools they are and what the split will be, e.g. Mathematics 50%, Chemistry 50%:B SFAccrediting body (if applicable)IChemEʓSystems Design and Control#TBC=Intermediate - LI@20$, if relevant⸮Semester 1ﱙ please state how frequently and when they will be delivered.ﱙAs a compulsory module (i.e. every student in the year should be Ǖ  B.Eng. in Energy Engineering (FT) – TBCM.Eng. in Energy Engineering (PT) – TBCM.Eng. in Energy Engineering with Industrial Study (TBC) B.Eng. in Energy Engineering with Industrial Study  (TBC) As an optional module (including any information about its grouping, if relevant): n/aÀ(or numbers attending teaching events for this module) are expected to meet or exceed the relevant College’s agreed threshold:YesB13.1State the name and code of any pre-requisite modules, i.e. modules students must have taken in previous years to be eligible to take this module. Please also note if these modules need to have been passed, ÁYear 1 Chemical Engineering or Year 1 Energy Engineering would need to be successfully passed.☩ knowledge students must possess to be eligible to take this module. Also describe any particular requirements for incoming exchange students, if applicableNoneÂnoneÃUoB Campus EdgbastonÄÄ on how your School /Department promotes equality of opportunity by ensuring no barriers are posed to applications, access or progression for any protected groupThe School is committed to ensuring an inclusive curriculum and actively promotes equality of opportunity to all. The School adheres to all Student Support agreements. There are no barriers to registration for this module when selected as part of the relevant programme offering.The module will seek to promote equality of opportunity through ensuring that no barriers are posed to students who would like to participate.  The module will also seek to ensure there are no barriers to students progressing through it.Scrutiny of EDI issues will be explicitly carried out by Education Committee within the School.Q Please briefly outline how this module embeds Education for Sustainability or the United Nations Sustainable Development Goals (SDGs; see guidance), or if not, what is the rationale behind that decision (approximately 150 words or less).The module and programme are based on sustainability. This module is directly linked to the Education for Sustainability. In the context of energy transitions, it is directly linked to a number of Sustainable Development Goals, SDG 7 Affordable and Clean energy, SDG 12 Responsible Consumption and Production, and SDG 13 Climate Action.SFÅn/aÆ effort for the module (this should equal the total no. of hours in 19.1-12, otherwise the missing hours will be added to ‘guided independent study’). NB Every 10 credits should equate to 100 hours of student effort, which includes guided independent study. Hover over each section for a definition. 200 hoursB Q Ç22 hours (2 x 11 weeks)È 11 hours (1 x 11 weeks)É11 hours (1 x 11 weeks)ꮛꮜꮝ16 hours (2 x 8 weeks) PC based classesꮞꮟꮠꮡꮢ140 hoursꮣꮤProviding a short, clear description, indicating the broad topic area covered by the module. This creates room for flexibility, so you do not need to deliver the exact same material every year.Ensuring that the description is attractive and accessible to prospective students, thus diminishing the need for a separate module description for marketing purposes.Possibly noting what ‘type’ of module it is, e.g. is it a broad, introductory module or is it a more specialist module that builds on previous learning?A module description should be approximately 150 words.Not recommended:Inclusion of excessive detail regarding the material to be covered in the module. This creates less flexibility to update that material each year.Outlining the full module syllabus, week-by-week. This creates less flexibility for you to vary your delivery plan each year.Over-use of technical jargon, which makes the description less ꮥThe module will develop the modelling and dynamic system analysis skills required for monitoring and control of complex systems.  This will include both paper and software based techniques.The fundamentals of engineering system relevant measurements will be covered, along with the fundamentals of open and closed-loop control.Control aspects will then be extended to consider system stability, classical PID controller design, feedback block diagram analysis and practical aspects of industrial system control.ꮦ each line should contain a different learning outcome (add or remove rows as necessary). All learning outcomes must be assessed by means of a summative assessment – failure to achieve all stated learning outcomes results in a student’s failure of the module. Guidance related to ‘levelness’ can be found in the OfS guidance related to Sector-recognised Standards (PDF – 201KB) and the QAA ꮧ Schools are also encouraged to refer to the Graduate Attributes. By the end of the module students should be able to:appreciate the importance of control and the role of the control engineer particularly in safety critical systems.comprehend the basic structure of control systems and how open- and closed-loop control is carried out and how the analysis and solution of dynamic models (particular linear 2nd order differential equations, particularly via Laplace Transforms techniques) is required.describe typical industrial measurement system used for commonly measured and manipulated system variables.understand fundamental control concepts, defining feedback and feed-forward modes of control and use relevant software and analytic tools (including Laplace Transforms and Simulink) to analyseꮨ(i.e. assessment that does not produce a mark that ꮩ</v>
-      </c>
-      <c r="AO12" t="str">
-        <v>&lt;br&gt;30% coursework &lt;br&gt;(10 page individual report considering a relevant multivariable control system)&lt;br&gt;&lt;br&gt;20% year 2 portfolio work primarily around lab and site visits&lt;br&gt;&lt;br&gt;2 hour written unseen examination&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;</v>
-      </c>
-      <c r="AP12" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="AQ12" t="str">
-        <v>Summer Exam PeriodThere is a class test, but this will be arranged by the school.</v>
-      </c>
-      <c r="AR12" t="str">
-        <v>none</v>
-      </c>
-      <c r="AS12" t="str">
-        <v>Resubmission&lt;br&gt;&lt;br&gt;Retake any failed elements.</v>
-      </c>
-      <c r="AT12" t="str">
-        <v>&lt;strong&gt;Assessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;30% coursework &lt;br&gt;(10 page individual report considering a relevant multivariable control system)&lt;br&gt;&lt;br&gt;20% year 2 portfolio work primarily around lab and site visits&lt;br&gt;&lt;br&gt;2 hour written unseen examination&lt;br&gt;&lt;br&gt;&lt;strong&gt;Reassessment:&lt;/strong&gt;&lt;br&gt;&lt;br&gt;Resubmission&lt;br&gt;&lt;br&gt;Retake any failed elements.</v>
-      </c>
-      <c r="AU12" t="str">
-        <v>Semester 1</v>
-      </c>
-      <c r="AV12" t="str">
-        <v>5</v>
-      </c>
-      <c r="AW12" t="str">
-        <v>Dr Phil Robbins</v>
+        <v>Dr Yuchen Yang &amp; Dr Jennifer Allsopp</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AW12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AW9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>